<commit_message>
Implement eval-HULU, add measurements to excel
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GLUE Results" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="HuLU Results" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -138,8 +139,90 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Matthews Correlation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accuracy</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -211,6 +294,39 @@
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuLU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuCoLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuCoPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuRTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuSST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HuWNLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixtral-8x7b-instruct-v0.1.Q5_K_M.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PULI-LlumiX-32K-Instruct-Q4_K_M.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF</t>
   </si>
 </sst>
 </file>
@@ -222,7 +338,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -265,9 +381,28 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -312,7 +447,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,15 +456,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,11 +496,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,6 +525,81 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -494,39 +716,40 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="6.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="4" width="6.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -596,9 +819,10 @@
         <v>12</v>
       </c>
       <c r="X2" s="5"/>
-      <c r="Y2" s="0"/>
+      <c r="Y2" s="1"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="2"/>
       <c r="D3" s="1" t="n">
         <v>1043</v>
       </c>
@@ -653,7 +877,6 @@
       <c r="X3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
@@ -666,75 +889,75 @@
         <f aca="false">AVERAGE(W4,T4:U4,R4,P4,N4,M4,K4,H4,I4,F4,D4)</f>
         <v>0.658513623474907</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="13" t="n">
         <v>0.523854029130735</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="14" t="n">
         <f aca="false">3/$D$3</f>
         <v>0.00287631831255992</v>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" s="13" t="n">
         <v>0.480334216425515</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="14" t="n">
         <f aca="false">1/$F$3</f>
         <v>0.000101884870096791</v>
       </c>
-      <c r="H4" s="12" t="n">
+      <c r="H4" s="13" t="n">
         <v>0.727941176470588</v>
       </c>
-      <c r="I4" s="12" t="n">
+      <c r="I4" s="13" t="n">
         <v>0.821829855537721</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="14" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K4" s="12" t="n">
+      <c r="K4" s="13" t="n">
         <v>0.696448187477115</v>
       </c>
-      <c r="L4" s="13" t="n">
+      <c r="L4" s="14" t="n">
         <f aca="false">1/$K$3</f>
         <v>0.000183049606443346</v>
       </c>
-      <c r="M4" s="12" t="n">
+      <c r="M4" s="13" t="n">
         <v>0.509271935283136</v>
       </c>
-      <c r="N4" s="12" t="n">
+      <c r="N4" s="13" t="n">
         <v>0.593278732490252</v>
       </c>
-      <c r="O4" s="13" t="n">
+      <c r="O4" s="14" t="n">
         <f aca="false">255/$M$3</f>
         <v>0.0063071976255256</v>
       </c>
-      <c r="P4" s="12" t="n">
+      <c r="P4" s="13" t="n">
         <v>0.249097472924188</v>
       </c>
-      <c r="Q4" s="13" t="n">
+      <c r="Q4" s="14" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R4" s="12" t="n">
+      <c r="R4" s="13" t="n">
         <v>0.934633027522936</v>
       </c>
-      <c r="S4" s="13" t="n">
+      <c r="S4" s="14" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T4" s="12" t="n">
+      <c r="T4" s="13" t="n">
         <v>0.821663265900952</v>
       </c>
-      <c r="U4" s="12" t="n">
+      <c r="U4" s="13" t="n">
         <v>0.825501723380821</v>
       </c>
-      <c r="V4" s="13" t="n">
+      <c r="V4" s="14" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W4" s="12" t="n">
+      <c r="W4" s="13" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X4" s="13" t="n">
+      <c r="X4" s="14" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -750,75 +973,75 @@
         <f aca="false">AVERAGE(W5,T5:U5,R5,P5,N5,M5,K5,H5,I5,F5,D5)</f>
         <v>0.723374373278101</v>
       </c>
-      <c r="D5" s="12" t="n">
+      <c r="D5" s="13" t="n">
         <v>0.451542212782268</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="14" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F5" s="12" t="n">
+      <c r="F5" s="13" t="n">
         <v>0.462964849719817</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="14" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H5" s="12" t="n">
+      <c r="H5" s="13" t="n">
         <v>0.801470588235294</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="13" t="n">
         <v>0.850828729281768</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="14" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="13" t="n">
         <v>0.8555738605162</v>
       </c>
-      <c r="L5" s="13" t="n">
+      <c r="L5" s="14" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="13" t="n">
         <v>0.822681177343557</v>
       </c>
-      <c r="N5" s="12" t="n">
+      <c r="N5" s="13" t="n">
         <v>0.777062536928196</v>
       </c>
-      <c r="O5" s="13" t="n">
+      <c r="O5" s="14" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="12" t="n">
+      <c r="P5" s="13" t="n">
         <v>0.317689530685921</v>
       </c>
-      <c r="Q5" s="13" t="n">
+      <c r="Q5" s="14" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R5" s="12" t="n">
+      <c r="R5" s="13" t="n">
         <v>0.951834862385321</v>
       </c>
-      <c r="S5" s="13" t="n">
+      <c r="S5" s="14" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T5" s="12" t="n">
+      <c r="T5" s="13" t="n">
         <v>0.831672916702132</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="13" t="n">
         <v>0.838861355601802</v>
       </c>
-      <c r="V5" s="13" t="n">
+      <c r="V5" s="14" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W5" s="12" t="n">
+      <c r="W5" s="13" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X5" s="13" t="n">
+      <c r="X5" s="14" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -834,75 +1057,75 @@
         <f aca="false">AVERAGE(W6,T6:U6,R6,P6,N6,M6,K6,H6,I6,F6,D6)</f>
         <v>0.740393758714782</v>
       </c>
-      <c r="D6" s="12" t="n">
+      <c r="D6" s="13" t="n">
         <v>0.526754313381707</v>
       </c>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="14" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F6" s="12" t="n">
+      <c r="F6" s="13" t="n">
         <v>0.418644931227713</v>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="14" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H6" s="12" t="n">
+      <c r="H6" s="13" t="n">
         <v>0.737745098039216</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="13" t="n">
         <v>0.820770519262982</v>
       </c>
-      <c r="J6" s="13" t="n">
+      <c r="J6" s="14" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="13" t="n">
         <v>0.833424858136555</v>
       </c>
-      <c r="L6" s="13" t="n">
+      <c r="L6" s="14" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M6" s="12" t="n">
+      <c r="M6" s="13" t="n">
         <v>0.765767994063814</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="13" t="n">
         <v>0.742172610944732</v>
       </c>
-      <c r="O6" s="13" t="n">
+      <c r="O6" s="14" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="12" t="n">
+      <c r="P6" s="13" t="n">
         <v>0.84115523465704</v>
       </c>
-      <c r="Q6" s="13" t="n">
+      <c r="Q6" s="14" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R6" s="12" t="n">
+      <c r="R6" s="13" t="n">
         <v>0.940366972477064</v>
       </c>
-      <c r="S6" s="13" t="n">
+      <c r="S6" s="14" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T6" s="12" t="n">
+      <c r="T6" s="13" t="n">
         <v>0.767106912789686</v>
       </c>
-      <c r="U6" s="12" t="n">
+      <c r="U6" s="13" t="n">
         <v>0.772505800441942</v>
       </c>
-      <c r="V6" s="13" t="n">
+      <c r="V6" s="14" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W6" s="12" t="n">
+      <c r="W6" s="13" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X6" s="13" t="n">
+      <c r="X6" s="14" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -918,75 +1141,75 @@
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
         <v>0.728207755738953</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="13" t="n">
         <v>0.417240141074992</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="14" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F7" s="12" t="n">
+      <c r="F7" s="13" t="n">
         <v>0.315944982170148</v>
       </c>
-      <c r="G7" s="13" t="n">
+      <c r="G7" s="14" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H7" s="12" t="n">
+      <c r="H7" s="13" t="n">
         <v>0.779411764705882</v>
       </c>
-      <c r="I7" s="12" t="n">
+      <c r="I7" s="13" t="n">
         <v>0.84375</v>
       </c>
-      <c r="J7" s="13" t="n">
+      <c r="J7" s="14" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K7" s="12" t="n">
+      <c r="K7" s="13" t="n">
         <v>0.733088909257562</v>
       </c>
-      <c r="L7" s="13" t="n">
+      <c r="L7" s="14" t="n">
         <f aca="false">8/$K$3</f>
         <v>0.00146439685154677</v>
       </c>
-      <c r="M7" s="12" t="n">
+      <c r="M7" s="13" t="n">
         <v>0.814964135542914</v>
       </c>
-      <c r="N7" s="12" t="n">
+      <c r="N7" s="13" t="n">
         <v>0.753954941621444</v>
       </c>
-      <c r="O7" s="13" t="n">
+      <c r="O7" s="14" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="12" t="n">
+      <c r="P7" s="13" t="n">
         <v>0.707581227436823</v>
       </c>
-      <c r="Q7" s="13" t="n">
+      <c r="Q7" s="14" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R7" s="12" t="n">
+      <c r="R7" s="13" t="n">
         <v>0.907110091743119</v>
       </c>
-      <c r="S7" s="13" t="n">
+      <c r="S7" s="14" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T7" s="12" t="n">
+      <c r="T7" s="13" t="n">
         <v>0.817610857364514</v>
       </c>
-      <c r="U7" s="12" t="n">
+      <c r="U7" s="13" t="n">
         <v>0.830934609499328</v>
       </c>
-      <c r="V7" s="13" t="n">
+      <c r="V7" s="14" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W7" s="12" t="n">
+      <c r="W7" s="13" t="n">
         <v>0.816901408450704</v>
       </c>
-      <c r="X7" s="13" t="n">
+      <c r="X7" s="14" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -1002,75 +1225,75 @@
         <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
         <v>0.613554278796799</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="13" t="n">
         <v>0.375051720670997</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="14" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" s="13" t="n">
         <v>0.538767193071829</v>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="14" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="13" t="n">
         <v>0.730392156862745</v>
       </c>
-      <c r="I8" s="12" t="n">
+      <c r="I8" s="13" t="n">
         <v>0.827044025157233</v>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="J8" s="14" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K8" s="12" t="n">
+      <c r="K8" s="13" t="n">
         <v>0.557386051619989</v>
       </c>
-      <c r="L8" s="13" t="n">
+      <c r="L8" s="14" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M8" s="12" t="n">
+      <c r="M8" s="13" t="n">
         <v>0.608706406134059</v>
       </c>
-      <c r="N8" s="12" t="n">
+      <c r="N8" s="13" t="n">
         <v>0.625189537528431</v>
       </c>
-      <c r="O8" s="13" t="n">
+      <c r="O8" s="14" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P8" s="12" t="n">
+      <c r="P8" s="13" t="n">
         <v>0.425992779783394</v>
       </c>
-      <c r="Q8" s="13" t="n">
+      <c r="Q8" s="14" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R8" s="12" t="n">
+      <c r="R8" s="13" t="n">
         <v>0.932339449541284</v>
       </c>
-      <c r="S8" s="13" t="n">
+      <c r="S8" s="14" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T8" s="12" t="n">
+      <c r="T8" s="13" t="n">
         <v>0.573663619974553</v>
       </c>
-      <c r="U8" s="12" t="n">
+      <c r="U8" s="13" t="n">
         <v>0.590653616484677</v>
       </c>
-      <c r="V8" s="13" t="n">
+      <c r="V8" s="14" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W8" s="12" t="n">
+      <c r="W8" s="13" t="n">
         <v>0.577464788732394</v>
       </c>
-      <c r="X8" s="13" t="n">
+      <c r="X8" s="14" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -1088,6 +1311,131 @@
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="W2:X2"/>
   </mergeCells>
+  <conditionalFormatting sqref="E4:E47 G4:G47 J4:J47 L4:L47 O4:O47 Q4:Q47 S4:S47 V4:V47 X4:X47">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D47">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F47">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H47">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I47">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K47">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M47">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N47">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P47">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R47">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T47">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U47">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W4:W47">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
     <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
@@ -1104,4 +1452,600 @@
   </headerFooter>
   <legacyDrawing r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="6.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="n">
+        <v>910</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="9" t="n">
+        <v>243</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="9" t="n">
+        <v>1165</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="12" t="n">
+        <f aca="false">AVERAGE(D4,F4,H4,J4,L4,N4)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E4" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="13" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G4" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="13" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="13" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K4" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="13" t="n">
+        <v>0.618556701030928</v>
+      </c>
+      <c r="M4" s="14" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N4" s="13" t="n">
+        <v>0.516666666666667</v>
+      </c>
+      <c r="O4" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="12" t="n">
+        <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
+        <v>0.45195286292649</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>0.193271177494123</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G5" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="13" t="n">
+        <v>0.359223300970874</v>
+      </c>
+      <c r="I5" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="13" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K5" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="15" t="n">
+        <v>0.678111587982833</v>
+      </c>
+      <c r="M5" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="13" t="n">
+        <v>0.566666666666667</v>
+      </c>
+      <c r="O5" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="12" t="n">
+        <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
+        <v>0.446939595430147</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>0.214844642079834</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="13" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G6" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13" t="n">
+        <v>0.310679611650485</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="13" t="n">
+        <v>0.448559670781893</v>
+      </c>
+      <c r="K6" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="13" t="n">
+        <v>0.68755364806867</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="13" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O6" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="12" t="n">
+        <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
+        <v>0.432443158810545</v>
+      </c>
+      <c r="D7" s="13" t="n">
+        <v>0.0718486458091463</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="13" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G7" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I7" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="13" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K7" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="13" t="n">
+        <v>0.629725085910653</v>
+      </c>
+      <c r="M7" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="13" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O7" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
+        <v>0.419278530088385</v>
+      </c>
+      <c r="D8" s="13" t="n">
+        <v>-0.0155335936055105</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="13" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G8" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13" t="n">
+        <v>0.368932038834951</v>
+      </c>
+      <c r="I8" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="13" t="n">
+        <v>0.489711934156379</v>
+      </c>
+      <c r="K8" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="13" t="n">
+        <v>0.659227467811159</v>
+      </c>
+      <c r="M8" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="13" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="O8" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="12" t="n">
+        <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
+        <v>0.449693612435578</v>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>0.204119502057382</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <v>0.368932038834951</v>
+      </c>
+      <c r="I9" s="14" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="13" t="n">
+        <v>0.442148760330579</v>
+      </c>
+      <c r="K9" s="14" t="n">
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
+      </c>
+      <c r="L9" s="15" t="n">
+        <v>0.672961373390558</v>
+      </c>
+      <c r="M9" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="13" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O9" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="12" t="n">
+        <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
+        <v>0.426274378090213</v>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>0.0702149056307087</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="13" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13" t="n">
+        <v>0.396039603960396</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <f aca="false">2/$H$3</f>
+        <v>0.0194174757281553</v>
+      </c>
+      <c r="J10" s="13" t="n">
+        <v>0.460905349794239</v>
+      </c>
+      <c r="K10" s="14" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="13" t="n">
+        <v>0.67381974248927</v>
+      </c>
+      <c r="M10" s="14" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="13" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="O10" s="14" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D47">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F47">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H47">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J47">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L47">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N47">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add eval results for gemma2+qwen2.5
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GLUE Results" sheetId="1" state="visible" r:id="rId3"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -270,6 +270,12 @@
     <t xml:space="preserve">Error</t>
   </si>
   <si>
+    <t xml:space="preserve">Qwen2.5-32B-Instruct-Q4_K_L.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">mixtral-8x7b-instruct-v0.1.Q5_K_M.gguf</t>
   </si>
   <si>
@@ -310,6 +316,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemma-2-27b-it-Q5_K_L.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-27b-it-GGUF</t>
   </si>
   <si>
     <t xml:space="preserve">HuLU</t>
@@ -451,7 +463,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,12 +496,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -529,7 +545,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="85">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -556,6 +572,270 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF81B666"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88B266"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3A268"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA5A168"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC78D6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD7846B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEC786C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF6D6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCCCC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF98A967"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99A867"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA1A368"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBA9569"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBE936A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9836B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2746D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7EB866"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF87B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9AA868"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB59869"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCE896B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDA826B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CB067"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BA768"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAB9E69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC0916A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0886B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDC816B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDE806C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8BB067"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF9CA668"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -564,15 +844,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF9DA568"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC3906A"/>
+          <fgColor rgb="FFAF9B69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -588,87 +860,151 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEA796C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCCCC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF98A967"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99A867"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA1A368"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBA9569"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2746D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF95AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB29A69"/>
+          <fgColor rgb="FF84B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB89669"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF83B566"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8AB167"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB19A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBB9469"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9EA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6A168"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDD816B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4736D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FB766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAE67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF96AA67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2A368"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF80B766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9AA768"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -684,271 +1020,31 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5856B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9836B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8DAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAA9E68"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBF926A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCF896B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2876B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7EB866"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF91AD67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BA768"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA6A068"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF78BB66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7CB966"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB19A69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7ABA66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF82B666"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85B366"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAB9D69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB69769"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF96AA67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD7846B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF0766D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7FB766"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAE67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBB9469"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF82B566"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF86B366"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF94AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC88D6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF84B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC98C6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9FA468"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD8846B"/>
+          <fgColor rgb="FFCD8A6B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8FAE67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB09B69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDF806C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -969,7 +1065,39 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF7DB966"/>
+          <fgColor rgb="FFAA9E68"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAD9D69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD4856B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5856B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEF766D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -985,7 +1113,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE57C6C"/>
+          <fgColor rgb="FFD2876B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27E6C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1001,6 +1137,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFF0756D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF93AB67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1009,14 +1153,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFA3A268"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFB29969"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1025,6 +1161,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC2906A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFCA8C6A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1049,14 +1193,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF8AB167"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF93AC67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1065,7 +1201,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFAF9B69"/>
+          <fgColor rgb="FF94AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA0A468"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1081,7 +1225,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFA5A168"/>
+          <fgColor rgb="FFF7716D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1269,10 +1413,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1378,645 +1522,802 @@
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="2"/>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="8" t="n">
         <v>1043</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="8" t="n">
         <v>9815</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="8" t="n">
         <v>408</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="8" t="n">
         <v>5463</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="10" t="n">
         <v>40430</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="N3" s="8"/>
+      <c r="O3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="9" t="n">
+      <c r="P3" s="10" t="n">
         <v>277</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="9" t="n">
+      <c r="R3" s="10" t="n">
         <v>872</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="1" t="n">
+      <c r="T3" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="U3" s="8"/>
+      <c r="V3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="1" t="n">
+      <c r="W3" s="8" t="n">
         <v>71</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="13" t="n">
         <f aca="false">AVERAGE(W4,T4:U4,R4,P4,N4,M4,K4,H4,I4,F4,D4)</f>
+        <v>0.811496442612959</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>0.583123781456463</v>
+      </c>
+      <c r="E4" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="14" t="n">
+        <v>0.362506367804381</v>
+      </c>
+      <c r="G4" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>0.794117647058824</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>0.857627118644068</v>
+      </c>
+      <c r="J4" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="16" t="n">
+        <v>0.900787113307706</v>
+      </c>
+      <c r="L4" s="15" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="14" t="n">
+        <v>0.857853079396488</v>
+      </c>
+      <c r="N4" s="14" t="n">
+        <v>0.815048434332057</v>
+      </c>
+      <c r="O4" s="15" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="14" t="n">
+        <v>0.942238267148014</v>
+      </c>
+      <c r="Q4" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="14" t="n">
+        <v>0.92545871559633</v>
+      </c>
+      <c r="S4" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="14" t="n">
+        <v>0.903148288781267</v>
+      </c>
+      <c r="U4" s="14" t="n">
+        <v>0.908724554167942</v>
+      </c>
+      <c r="V4" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="14" t="n">
+        <v>0.887323943661972</v>
+      </c>
+      <c r="X4" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <f aca="false">AVERAGE(W5,T5:U5,R5,P5,N5,M5,K5,H5,I5,F5,D5)</f>
         <v>0.761759832782204</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D5" s="14" t="n">
         <v>0.597514874790058</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E5" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F4" s="15" t="n">
+      <c r="F5" s="14" t="n">
         <v>0.478247580234335</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H4" s="15" t="n">
+      <c r="H5" s="14" t="n">
         <v>0.757352941176471</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I5" s="14" t="n">
         <v>0.834170854271357</v>
       </c>
-      <c r="J4" s="14" t="n">
+      <c r="J5" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K4" s="15" t="n">
+      <c r="K5" s="14" t="n">
         <v>0.767975055025679</v>
       </c>
-      <c r="L4" s="14" t="n">
+      <c r="L5" s="15" t="n">
         <f aca="false">11/$K$3</f>
         <v>0.00201354567087681</v>
       </c>
-      <c r="M4" s="13" t="n">
+      <c r="M5" s="14" t="n">
         <v>0.824560969577047</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N5" s="14" t="n">
         <v>0.785041064339182</v>
       </c>
-      <c r="O4" s="14" t="n">
+      <c r="O5" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="13" t="n">
+      <c r="P5" s="14" t="n">
         <v>0.746376811594203</v>
       </c>
-      <c r="Q4" s="14" t="n">
+      <c r="Q5" s="15" t="n">
         <f aca="false">1/$P$3</f>
         <v>0.0036101083032491</v>
       </c>
-      <c r="R4" s="13" t="n">
+      <c r="R5" s="14" t="n">
         <v>0.95752009184845</v>
       </c>
-      <c r="S4" s="14" t="n">
+      <c r="S5" s="15" t="n">
         <f aca="false">1/$R$3</f>
         <v>0.00114678899082569</v>
       </c>
-      <c r="T4" s="15" t="n">
+      <c r="T5" s="14" t="n">
         <v>0.87058607341487</v>
       </c>
-      <c r="U4" s="15" t="n">
+      <c r="U5" s="14" t="n">
         <v>0.873884353171137</v>
       </c>
-      <c r="V4" s="14" t="n">
+      <c r="V5" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W4" s="15" t="n">
+      <c r="W5" s="14" t="n">
         <v>0.647887323943662</v>
       </c>
-      <c r="X4" s="14" t="n">
-        <f aca="false">0/$W$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="12" t="n">
-        <f aca="false">AVERAGE(W5,T5:U5,R5,P5,N5,M5,K5,H5,I5,F5,D5)</f>
-        <v>0.740393758714782</v>
-      </c>
-      <c r="D5" s="13" t="n">
-        <v>0.526754313381707</v>
-      </c>
-      <c r="E5" s="14" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="13" t="n">
-        <v>0.418644931227713</v>
-      </c>
-      <c r="G5" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="13" t="n">
-        <v>0.737745098039216</v>
-      </c>
-      <c r="I5" s="13" t="n">
-        <v>0.820770519262982</v>
-      </c>
-      <c r="J5" s="14" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="13" t="n">
-        <v>0.833424858136555</v>
-      </c>
-      <c r="L5" s="14" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="13" t="n">
-        <v>0.765767994063814</v>
-      </c>
-      <c r="N5" s="13" t="n">
-        <v>0.742172610944732</v>
-      </c>
-      <c r="O5" s="14" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="13" t="n">
-        <v>0.84115523465704</v>
-      </c>
-      <c r="Q5" s="14" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="13" t="n">
-        <v>0.940366972477064</v>
-      </c>
-      <c r="S5" s="14" t="n">
-        <f aca="false">0/$R$3</f>
-        <v>0</v>
-      </c>
-      <c r="T5" s="13" t="n">
-        <v>0.767106912789686</v>
-      </c>
-      <c r="U5" s="13" t="n">
-        <v>0.772505800441942</v>
-      </c>
-      <c r="V5" s="14" t="n">
-        <f aca="false">0/$T$3</f>
-        <v>0</v>
-      </c>
-      <c r="W5" s="13" t="n">
-        <v>0.71830985915493</v>
-      </c>
-      <c r="X5" s="14" t="n">
+      <c r="X5" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">AVERAGE(W6,T6:U6,R6,P6,N6,M6,K6,H6,I6,F6,D6)</f>
+        <v>0.740393758714782</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>0.526754313381707</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>0.418644931227713</v>
+      </c>
+      <c r="G6" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>0.737745098039216</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>0.820770519262982</v>
+      </c>
+      <c r="J6" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="14" t="n">
+        <v>0.833424858136555</v>
+      </c>
+      <c r="L6" s="15" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="14" t="n">
+        <v>0.765767994063814</v>
+      </c>
+      <c r="N6" s="14" t="n">
+        <v>0.742172610944732</v>
+      </c>
+      <c r="O6" s="15" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="14" t="n">
+        <v>0.84115523465704</v>
+      </c>
+      <c r="Q6" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="14" t="n">
+        <v>0.940366972477064</v>
+      </c>
+      <c r="S6" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="14" t="n">
+        <v>0.767106912789686</v>
+      </c>
+      <c r="U6" s="14" t="n">
+        <v>0.772505800441942</v>
+      </c>
+      <c r="V6" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="14" t="n">
+        <v>0.71830985915493</v>
+      </c>
+      <c r="X6" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
         <v>0.728207755738953</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D7" s="14" t="n">
         <v>0.417240141074992</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>0.315944982170148</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G7" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H6" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <v>0.779411764705882</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I7" s="14" t="n">
         <v>0.84375</v>
       </c>
-      <c r="J6" s="14" t="n">
+      <c r="J7" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K6" s="13" t="n">
+      <c r="K7" s="14" t="n">
         <v>0.733088909257562</v>
       </c>
-      <c r="L6" s="14" t="n">
+      <c r="L7" s="15" t="n">
         <f aca="false">8/$K$3</f>
         <v>0.00146439685154677</v>
       </c>
-      <c r="M6" s="13" t="n">
+      <c r="M7" s="14" t="n">
         <v>0.814964135542914</v>
       </c>
-      <c r="N6" s="13" t="n">
+      <c r="N7" s="14" t="n">
         <v>0.753954941621444</v>
       </c>
-      <c r="O6" s="14" t="n">
+      <c r="O7" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="13" t="n">
+      <c r="P7" s="14" t="n">
         <v>0.707581227436823</v>
       </c>
-      <c r="Q6" s="14" t="n">
+      <c r="Q7" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R6" s="13" t="n">
+      <c r="R7" s="14" t="n">
         <v>0.907110091743119</v>
       </c>
-      <c r="S6" s="14" t="n">
+      <c r="S7" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T6" s="13" t="n">
+      <c r="T7" s="14" t="n">
         <v>0.817610857364514</v>
       </c>
-      <c r="U6" s="13" t="n">
+      <c r="U7" s="14" t="n">
         <v>0.830934609499328</v>
       </c>
-      <c r="V6" s="14" t="n">
+      <c r="V7" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W6" s="13" t="n">
+      <c r="W7" s="14" t="n">
         <v>0.816901408450704</v>
       </c>
-      <c r="X6" s="14" t="n">
+      <c r="X7" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="12" t="n">
-        <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="13" t="n">
+        <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
         <v>0.723374373278101</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D8" s="14" t="n">
         <v>0.451542212782268</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E8" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>0.462964849719817</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G8" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H8" s="14" t="n">
         <v>0.801470588235294</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I8" s="14" t="n">
         <v>0.850828729281768</v>
       </c>
-      <c r="J7" s="14" t="n">
+      <c r="J8" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K7" s="13" t="n">
+      <c r="K8" s="14" t="n">
         <v>0.8555738605162</v>
       </c>
-      <c r="L7" s="14" t="n">
+      <c r="L8" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M7" s="13" t="n">
+      <c r="M8" s="14" t="n">
         <v>0.822681177343557</v>
       </c>
-      <c r="N7" s="13" t="n">
+      <c r="N8" s="14" t="n">
         <v>0.777062536928196</v>
       </c>
-      <c r="O7" s="14" t="n">
+      <c r="O8" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="13" t="n">
+      <c r="P8" s="14" t="n">
         <v>0.317689530685921</v>
       </c>
-      <c r="Q7" s="14" t="n">
+      <c r="Q8" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R7" s="13" t="n">
+      <c r="R8" s="14" t="n">
         <v>0.951834862385321</v>
       </c>
-      <c r="S7" s="14" t="n">
+      <c r="S8" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T7" s="13" t="n">
+      <c r="T8" s="14" t="n">
         <v>0.831672916702132</v>
       </c>
-      <c r="U7" s="13" t="n">
+      <c r="U8" s="14" t="n">
         <v>0.838861355601802</v>
       </c>
-      <c r="V7" s="14" t="n">
+      <c r="V8" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W7" s="13" t="n">
+      <c r="W8" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X7" s="14" t="n">
+      <c r="X8" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="12" t="n">
-        <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
         <v>0.658513623474907</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D9" s="14" t="n">
         <v>0.523854029130735</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E9" s="15" t="n">
         <f aca="false">3/$D$3</f>
         <v>0.00287631831255992</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F9" s="14" t="n">
         <v>0.480334216425515</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G9" s="15" t="n">
         <f aca="false">1/$F$3</f>
         <v>0.000101884870096791</v>
       </c>
-      <c r="H8" s="13" t="n">
+      <c r="H9" s="14" t="n">
         <v>0.727941176470588</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I9" s="14" t="n">
         <v>0.821829855537721</v>
       </c>
-      <c r="J8" s="14" t="n">
+      <c r="J9" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K9" s="14" t="n">
         <v>0.696448187477115</v>
       </c>
-      <c r="L8" s="14" t="n">
+      <c r="L9" s="15" t="n">
         <f aca="false">1/$K$3</f>
         <v>0.000183049606443346</v>
       </c>
-      <c r="M8" s="13" t="n">
+      <c r="M9" s="14" t="n">
         <v>0.509271935283136</v>
       </c>
-      <c r="N8" s="13" t="n">
+      <c r="N9" s="14" t="n">
         <v>0.593278732490252</v>
       </c>
-      <c r="O8" s="14" t="n">
+      <c r="O9" s="15" t="n">
         <f aca="false">255/$M$3</f>
         <v>0.0063071976255256</v>
       </c>
-      <c r="P8" s="13" t="n">
+      <c r="P9" s="14" t="n">
         <v>0.249097472924188</v>
       </c>
-      <c r="Q8" s="14" t="n">
+      <c r="Q9" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R8" s="13" t="n">
+      <c r="R9" s="14" t="n">
         <v>0.934633027522936</v>
       </c>
-      <c r="S8" s="14" t="n">
+      <c r="S9" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T8" s="13" t="n">
+      <c r="T9" s="14" t="n">
         <v>0.821663265900952</v>
       </c>
-      <c r="U8" s="13" t="n">
+      <c r="U9" s="14" t="n">
         <v>0.825501723380821</v>
       </c>
-      <c r="V8" s="14" t="n">
+      <c r="V9" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W8" s="13" t="n">
+      <c r="W9" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X8" s="14" t="n">
-        <f aca="false">0/$W$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="12" t="n">
-        <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
-        <v>0.613554278796799</v>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>0.375051720670997</v>
-      </c>
-      <c r="E9" s="14" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>0.538767193071829</v>
-      </c>
-      <c r="G9" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="13" t="n">
-        <v>0.730392156862745</v>
-      </c>
-      <c r="I9" s="13" t="n">
-        <v>0.827044025157233</v>
-      </c>
-      <c r="J9" s="14" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="13" t="n">
-        <v>0.557386051619989</v>
-      </c>
-      <c r="L9" s="14" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="13" t="n">
-        <v>0.608706406134059</v>
-      </c>
-      <c r="N9" s="13" t="n">
-        <v>0.625189537528431</v>
-      </c>
-      <c r="O9" s="14" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="13" t="n">
-        <v>0.425992779783394</v>
-      </c>
-      <c r="Q9" s="14" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="13" t="n">
-        <v>0.932339449541284</v>
-      </c>
-      <c r="S9" s="14" t="n">
-        <f aca="false">0/$R$3</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="13" t="n">
-        <v>0.573663619974553</v>
-      </c>
-      <c r="U9" s="13" t="n">
-        <v>0.590653616484677</v>
-      </c>
-      <c r="V9" s="14" t="n">
-        <f aca="false">0/$T$3</f>
-        <v>0</v>
-      </c>
-      <c r="W9" s="13" t="n">
-        <v>0.577464788732394</v>
-      </c>
-      <c r="X9" s="14" t="n">
+      <c r="X9" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="13" t="n">
         <f aca="false">AVERAGE(W10,T10:U10,R10,P10,N10,M10,K10,H10,I10,F10,D10)</f>
+        <v>0.613554278796799</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>0.375051720670997</v>
+      </c>
+      <c r="E10" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>0.538767193071829</v>
+      </c>
+      <c r="G10" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <v>0.730392156862745</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <v>0.827044025157233</v>
+      </c>
+      <c r="J10" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="14" t="n">
+        <v>0.557386051619989</v>
+      </c>
+      <c r="L10" s="15" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="n">
+        <v>0.608706406134059</v>
+      </c>
+      <c r="N10" s="14" t="n">
+        <v>0.625189537528431</v>
+      </c>
+      <c r="O10" s="15" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="14" t="n">
+        <v>0.425992779783394</v>
+      </c>
+      <c r="Q10" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="14" t="n">
+        <v>0.932339449541284</v>
+      </c>
+      <c r="S10" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="14" t="n">
+        <v>0.573663619974553</v>
+      </c>
+      <c r="U10" s="14" t="n">
+        <v>0.590653616484677</v>
+      </c>
+      <c r="V10" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="14" t="n">
+        <v>0.577464788732394</v>
+      </c>
+      <c r="X10" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="13" t="n">
+        <f aca="false">AVERAGE(W11,T11:U11,R11,P11,N11,M11,K11,H11,I11,F11,D11)</f>
         <v>0.499454443668613</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>0.333471865271531</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E11" s="15" t="n">
         <f aca="false">6/$D$3</f>
         <v>0.00575263662511985</v>
       </c>
-      <c r="F10" s="15" t="n">
+      <c r="F11" s="14" t="n">
         <v>0.292103922567499</v>
       </c>
-      <c r="G10" s="14" t="n">
+      <c r="G11" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H10" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <v>0.698529411764706</v>
       </c>
-      <c r="I10" s="13" t="n">
+      <c r="I11" s="14" t="n">
         <v>0.805687203791469</v>
       </c>
-      <c r="J10" s="14" t="n">
+      <c r="J11" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K11" s="14" t="n">
         <v>0.391434449223864</v>
       </c>
-      <c r="L10" s="14" t="n">
+      <c r="L11" s="15" t="n">
         <f aca="false">116/$K$3</f>
         <v>0.0212337543474282</v>
       </c>
-      <c r="M10" s="15" t="n">
+      <c r="M11" s="14" t="n">
         <v>0.691602220900258</v>
       </c>
-      <c r="N10" s="15" t="n">
+      <c r="N11" s="14" t="n">
         <v>0.36669042044182</v>
       </c>
-      <c r="O10" s="14" t="n">
+      <c r="O11" s="15" t="n">
         <f aca="false">86/$M$3</f>
         <v>0.00212713331684393</v>
       </c>
-      <c r="P10" s="15" t="n">
+      <c r="P11" s="14" t="n">
         <v>0.306859205776173</v>
       </c>
-      <c r="Q10" s="14" t="n">
+      <c r="Q11" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R10" s="15" t="n">
+      <c r="R11" s="14" t="n">
         <v>0.855504587155963</v>
       </c>
-      <c r="S10" s="14" t="n">
+      <c r="S11" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T10" s="15" t="n">
+      <c r="T11" s="14" t="n">
         <v>0.370306926073738</v>
       </c>
-      <c r="U10" s="15" t="n">
+      <c r="U11" s="14" t="n">
         <v>0.402389871619712</v>
       </c>
-      <c r="V10" s="14" t="n">
+      <c r="V11" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W10" s="15" t="n">
+      <c r="W11" s="14" t="n">
         <v>0.47887323943662</v>
       </c>
-      <c r="X10" s="14" t="n">
+      <c r="X11" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="13" t="n">
+        <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
+        <v>0.721879431828856</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>0.618250159186482</v>
+      </c>
+      <c r="E12" s="15" t="n">
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>0.411716760061131</v>
+      </c>
+      <c r="G12" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <v>0.806372549019608</v>
+      </c>
+      <c r="I12" s="14" t="n">
+        <v>0.866779089376054</v>
+      </c>
+      <c r="J12" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="14" t="n">
+        <v>0.906278601501007</v>
+      </c>
+      <c r="L12" s="15" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="15" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="14"/>
+      <c r="S12" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="14"/>
+      <c r="X12" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -2036,7 +2337,7 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2161,13 +2462,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2176,8 +2479,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <drawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -2186,10 +2489,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2197,7 +2500,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.16"/>
@@ -2219,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2240,444 +2543,552 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="8" t="n">
         <v>910</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="8" t="n">
         <v>103</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="10" t="n">
         <v>243</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <v>1165</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="1" t="n">
+      <c r="N3" s="8" t="n">
         <v>60</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="12" t="n">
+      <c r="A4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="13" t="n">
         <f aca="false">AVERAGE(D4,F4,H4,J4,L4,N4)</f>
-        <v>0.45195286292649</v>
-      </c>
-      <c r="D4" s="13" t="n">
-        <v>0.193271177494123</v>
-      </c>
-      <c r="E4" s="14" t="n">
+        <v>0.477597373948204</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>0.38169947346544</v>
+      </c>
+      <c r="E4" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="G4" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="13" t="n">
-        <v>0.359223300970874</v>
-      </c>
-      <c r="I4" s="14" t="n">
+      <c r="F4" s="16" t="n">
+        <v>0.472972972972973</v>
+      </c>
+      <c r="G4" s="15" t="n">
+        <f aca="false">26/$F$3</f>
+        <v>0.26</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>0.349514563106796</v>
+      </c>
+      <c r="I4" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K4" s="14" t="n">
+      <c r="K4" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L4" s="15" t="n">
-        <v>0.678111587982833</v>
-      </c>
-      <c r="M4" s="14" t="n">
+      <c r="L4" s="14" t="n">
+        <v>0.666952789699571</v>
+      </c>
+      <c r="M4" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N4" s="13" t="n">
-        <v>0.566666666666667</v>
-      </c>
-      <c r="O4" s="14" t="n">
+      <c r="N4" s="14" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O4" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
+        <v>0.456362837616999</v>
+      </c>
+      <c r="D5" s="16" t="n">
+        <v>0.304699117807113</v>
+      </c>
+      <c r="E5" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="14" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="G5" s="15" t="n">
+        <f aca="false">25/$F$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>0.349514563106796</v>
+      </c>
+      <c r="I5" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="14" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K5" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="16" t="n">
+        <v>0.622852233676976</v>
+      </c>
+      <c r="M5" s="15" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N5" s="14" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O5" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
+        <v>0.45195286292649</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>0.193271177494123</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G6" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>0.359223300970874</v>
+      </c>
+      <c r="I6" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K6" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="14" t="n">
+        <v>0.678111587982833</v>
+      </c>
+      <c r="M6" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="14" t="n">
+        <v>0.566666666666667</v>
+      </c>
+      <c r="O6" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
         <v>0.449693612435578</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D7" s="14" t="n">
         <v>0.204119502057382</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>0.46</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G7" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <v>0.368932038834951</v>
       </c>
-      <c r="I5" s="14" t="n">
+      <c r="I7" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J7" s="14" t="n">
         <v>0.442148760330579</v>
       </c>
-      <c r="K5" s="14" t="n">
+      <c r="K7" s="15" t="n">
         <f aca="false">1/$J$3</f>
         <v>0.00411522633744856</v>
       </c>
-      <c r="L5" s="15" t="n">
+      <c r="L7" s="14" t="n">
         <v>0.672961373390558</v>
       </c>
-      <c r="M5" s="14" t="n">
+      <c r="M7" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N5" s="13" t="n">
+      <c r="N7" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O5" s="14" t="n">
-        <f aca="false">0/$N$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="12" t="n">
-        <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
-        <v>0.446939595430147</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>0.214844642079834</v>
-      </c>
-      <c r="E6" s="14" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="G6" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="13" t="n">
-        <v>0.310679611650485</v>
-      </c>
-      <c r="I6" s="14" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="13" t="n">
-        <v>0.448559670781893</v>
-      </c>
-      <c r="K6" s="14" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="13" t="n">
-        <v>0.68755364806867</v>
-      </c>
-      <c r="M6" s="14" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="13" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="O6" s="14" t="n">
-        <f aca="false">0/$N$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="12" t="n">
-        <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
-        <v>0.432443158810545</v>
-      </c>
-      <c r="D7" s="13" t="n">
-        <v>0.0718486458091463</v>
-      </c>
-      <c r="E7" s="14" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="13" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="G7" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="13" t="n">
-        <v>0.378640776699029</v>
-      </c>
-      <c r="I7" s="14" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="13" t="n">
-        <v>0.444444444444444</v>
-      </c>
-      <c r="K7" s="14" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="13" t="n">
-        <v>0.629725085910653</v>
-      </c>
-      <c r="M7" s="14" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="13" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="O7" s="14" t="n">
+      <c r="O7" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="12" t="n">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="13" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
+        <v>0.446939595430147</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>0.214844642079834</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="14" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G8" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="n">
+        <v>0.310679611650485</v>
+      </c>
+      <c r="I8" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="14" t="n">
+        <v>0.448559670781893</v>
+      </c>
+      <c r="K8" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="14" t="n">
+        <v>0.68755364806867</v>
+      </c>
+      <c r="M8" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="14" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O8" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
+        <v>0.432443158810545</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>0.0718486458091463</v>
+      </c>
+      <c r="E9" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G9" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I9" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="14" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K9" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="14" t="n">
+        <v>0.629725085910653</v>
+      </c>
+      <c r="M9" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="14" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O9" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="13" t="n">
+        <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
         <v>0.426274378090213</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D10" s="14" t="n">
         <v>0.0702149056307087</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E10" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F10" s="14" t="n">
         <v>0.49</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G10" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H8" s="13" t="n">
+      <c r="H10" s="14" t="n">
         <v>0.396039603960396</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I10" s="15" t="n">
         <f aca="false">2/$H$3</f>
         <v>0.0194174757281553</v>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="J10" s="14" t="n">
         <v>0.460905349794239</v>
       </c>
-      <c r="K8" s="14" t="n">
+      <c r="K10" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L8" s="13" t="n">
+      <c r="L10" s="14" t="n">
         <v>0.67381974248927</v>
       </c>
-      <c r="M8" s="14" t="n">
+      <c r="M10" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N8" s="13" t="n">
+      <c r="N10" s="14" t="n">
         <v>0.466666666666667</v>
       </c>
-      <c r="O8" s="14" t="n">
+      <c r="O10" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="13" t="n">
+        <f aca="false">AVERAGE(D11,F11,H11,J11,L11,N11)</f>
+        <v>0.419278530088385</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>-0.0155335936055105</v>
+      </c>
+      <c r="E11" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G11" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="14" t="n">
+        <v>0.368932038834951</v>
+      </c>
+      <c r="I11" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="14" t="n">
+        <v>0.489711934156379</v>
+      </c>
+      <c r="K11" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="14" t="n">
+        <v>0.659227467811159</v>
+      </c>
+      <c r="M11" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="14" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="O11" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="n">
-        <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
-        <v>0.419278530088385</v>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>-0.0155335936055105</v>
-      </c>
-      <c r="E9" s="14" t="n">
+      <c r="C12" s="13" t="n">
+        <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E12" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="G9" s="14" t="n">
+      <c r="F12" s="14" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G12" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H9" s="13" t="n">
-        <v>0.368932038834951</v>
-      </c>
-      <c r="I9" s="14" t="n">
+      <c r="H12" s="14" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I12" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J9" s="13" t="n">
-        <v>0.489711934156379</v>
-      </c>
-      <c r="K9" s="14" t="n">
+      <c r="J12" s="14" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K12" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L9" s="13" t="n">
-        <v>0.659227467811159</v>
-      </c>
-      <c r="M9" s="14" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="13" t="n">
-        <v>0.533333333333333</v>
-      </c>
-      <c r="O9" s="14" t="n">
-        <f aca="false">0/$N$3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="12" t="n">
-        <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
-        <v>0.405257833604129</v>
-      </c>
-      <c r="D10" s="13" t="n">
-        <v>-0.0714529452409867</v>
-      </c>
-      <c r="E10" s="14" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="13" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="G10" s="14" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="13" t="n">
-        <v>0.378640776699029</v>
-      </c>
-      <c r="I10" s="14" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="13" t="n">
-        <v>0.469135802469136</v>
-      </c>
-      <c r="K10" s="14" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="13" t="n">
+      <c r="L12" s="14" t="n">
         <v>0.618556701030928</v>
       </c>
-      <c r="M10" s="14" t="n">
+      <c r="M12" s="15" t="n">
         <f aca="false">1/$L$3</f>
         <v>0.000858369098712446</v>
       </c>
-      <c r="N10" s="13" t="n">
+      <c r="N12" s="14" t="n">
         <v>0.516666666666667</v>
       </c>
-      <c r="O10" s="14" t="n">
+      <c r="O12" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
@@ -2694,7 +3105,7 @@
     <mergeCell ref="N2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2759,13 +3170,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2774,7 +3187,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <drawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding results for Yi + Command R
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GLUE Results" sheetId="1" state="visible" r:id="rId3"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -276,6 +276,18 @@
     <t xml:space="preserve">https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF</t>
   </si>
   <si>
+    <t xml:space="preserve">Yi-1.5-34B-Chat-Q4_K_M.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemma-2-27b-it-Q5_K_L.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-27b-it-GGUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">mixtral-8x7b-instruct-v0.1.Q5_K_M.gguf</t>
   </si>
   <si>
@@ -300,6 +312,12 @@
     <t xml:space="preserve">https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF</t>
   </si>
   <si>
+    <t xml:space="preserve">c4ai-command-r-v01.i1-Q4_K_S.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phi-3-mini-4k-instruct-q4.gguf</t>
   </si>
   <si>
@@ -318,12 +336,6 @@
     <t xml:space="preserve">https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF</t>
   </si>
   <si>
-    <t xml:space="preserve">gemma-2-27b-it-Q5_K_L.gguf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-27b-it-GGUF</t>
-  </si>
-  <si>
     <t xml:space="preserve">HuLU</t>
   </si>
   <si>
@@ -343,6 +355,12 @@
   </si>
   <si>
     <t xml:space="preserve">HuWNLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falcon-mamba-7b-instruct.Q6_K.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF</t>
   </si>
 </sst>
 </file>
@@ -545,7 +563,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="99">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -572,6 +590,382 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF8BB067"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99A867"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB09A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB29A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCF896B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDD806B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE766C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF6D6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCCCC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF98A967"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA1A368"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBA9569"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBE936A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9836B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2746D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF97A967"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BA768"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2A368"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB19A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC68E6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5856B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE07F6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE37D6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92AC67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAE9C69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBB9469"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC78D6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC8A6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27D6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE47C6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF83B566"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF84B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88B266"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA0A468"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA89F68"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC88D6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF86B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF89B167"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8AB167"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9CA668"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB99569"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7ABA66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF81B666"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -580,191 +974,183 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF88B266"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA3A268"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA5A168"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC78D6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD7846B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEC786C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCCCC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF98A967"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99A867"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA1A368"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBA9569"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBE936A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9836B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2746D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7EB866"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF87B366"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9AA868"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB59869"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCE896B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDA826B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8CB067"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BA768"/>
+          <fgColor rgb="FF82B566"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF94AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF87B266"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9EA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6A168"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAA9E68"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDD816B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4736D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FB766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAE67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF96AA67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7CB966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF80B766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9AA768"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC8B6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7BB966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7DB866"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82B666"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCD8A6B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8FAE67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF98A867"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -773,262 +1159,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFAB9E69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC0916A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0886B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDC816B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDE806C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF79BB66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8BB067"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9CA668"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAF9B69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD4866B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF84B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB89669"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF83B566"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8AB167"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB19A69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBB9469"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9EA568"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA6A168"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDD816B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4736D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7FB766"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAE67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF96AA67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2A368"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF80B766"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8CAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8DAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9AA768"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC8B6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCD8A6B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8FAE67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1065,14 +1195,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFAA9E68"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFAD9D69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1081,6 +1203,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC48F6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFD4856B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1089,7 +1219,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5856B"/>
+          <fgColor rgb="FFDB826B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27E6C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1105,6 +1243,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFA5A168"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFBC946A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1121,14 +1267,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE27E6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFE97A6C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1145,87 +1283,79 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF93AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB29969"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC2906A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCA8C6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED776C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9706D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93AC67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF94AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA0A468"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE9796C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7716D"/>
+          <fgColor rgb="FFFC6F6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF90AD67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA1A468"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC1916A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA796C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8716D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFD6E6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7EB766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7EB866"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B466"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1413,10 +1543,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1668,80 +1798,80 @@
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="13" t="n">
         <f aca="false">AVERAGE(W5,T5:U5,R5,P5,N5,M5,K5,H5,I5,F5,D5)</f>
-        <v>0.761759832782204</v>
+        <v>0.809456837704127</v>
       </c>
       <c r="D5" s="14" t="n">
-        <v>0.597514874790058</v>
+        <v>0.665512350161472</v>
       </c>
       <c r="E5" s="15" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>0.478247580234335</v>
+        <v>0.43301069791136</v>
       </c>
       <c r="G5" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H5" s="14" t="n">
-        <v>0.757352941176471</v>
+        <v>0.838235294117647</v>
       </c>
       <c r="I5" s="14" t="n">
-        <v>0.834170854271357</v>
+        <v>0.881294964028777</v>
       </c>
       <c r="J5" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K5" s="14" t="n">
-        <v>0.767975055025679</v>
+        <v>0.85337726523888</v>
       </c>
       <c r="L5" s="15" t="n">
-        <f aca="false">11/$K$3</f>
-        <v>0.00201354567087681</v>
-      </c>
-      <c r="M5" s="14" t="n">
-        <v>0.824560969577047</v>
-      </c>
-      <c r="N5" s="14" t="n">
-        <v>0.785041064339182</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="16" t="n">
+        <v>0.860697501855058</v>
+      </c>
+      <c r="N5" s="16" t="n">
+        <v>0.806951395077809</v>
       </c>
       <c r="O5" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="14" t="n">
-        <v>0.746376811594203</v>
+      <c r="P5" s="16" t="n">
+        <v>0.859205776173285</v>
       </c>
       <c r="Q5" s="15" t="n">
-        <f aca="false">1/$P$3</f>
-        <v>0.0036101083032491</v>
-      </c>
-      <c r="R5" s="14" t="n">
-        <v>0.95752009184845</v>
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="16" t="n">
+        <v>0.951834862385321</v>
       </c>
       <c r="S5" s="15" t="n">
-        <f aca="false">1/$R$3</f>
-        <v>0.00114678899082569</v>
-      </c>
-      <c r="T5" s="14" t="n">
-        <v>0.87058607341487</v>
-      </c>
-      <c r="U5" s="14" t="n">
-        <v>0.873884353171137</v>
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="16" t="n">
+        <v>0.886830850881204</v>
+      </c>
+      <c r="U5" s="16" t="n">
+        <v>0.887798700252512</v>
       </c>
       <c r="V5" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W5" s="14" t="n">
-        <v>0.647887323943662</v>
+      <c r="W5" s="16" t="n">
+        <v>0.788732394366197</v>
       </c>
       <c r="X5" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -1752,80 +1882,80 @@
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="13" t="n">
         <f aca="false">AVERAGE(W6,T6:U6,R6,P6,N6,M6,K6,H6,I6,F6,D6)</f>
-        <v>0.740393758714782</v>
+        <v>0.799244376594315</v>
       </c>
       <c r="D6" s="14" t="n">
-        <v>0.526754313381707</v>
+        <v>0.618250159186482</v>
       </c>
       <c r="E6" s="15" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F6" s="14" t="n">
-        <v>0.418644931227713</v>
+        <v>0.411716760061131</v>
       </c>
       <c r="G6" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H6" s="14" t="n">
-        <v>0.737745098039216</v>
+        <v>0.806372549019608</v>
       </c>
       <c r="I6" s="14" t="n">
-        <v>0.820770519262982</v>
+        <v>0.866779089376054</v>
       </c>
       <c r="J6" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K6" s="14" t="n">
-        <v>0.833424858136555</v>
+        <v>0.906278601501007</v>
       </c>
       <c r="L6" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M6" s="14" t="n">
-        <v>0.765767994063814</v>
-      </c>
-      <c r="N6" s="14" t="n">
-        <v>0.742172610944732</v>
+      <c r="M6" s="16" t="n">
+        <v>0.812663863467722</v>
+      </c>
+      <c r="N6" s="16" t="n">
+        <v>0.780958991266123</v>
       </c>
       <c r="O6" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="14" t="n">
-        <v>0.84115523465704</v>
+      <c r="P6" s="16" t="n">
+        <v>0.862815884476534</v>
       </c>
       <c r="Q6" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R6" s="14" t="n">
-        <v>0.940366972477064</v>
+      <c r="R6" s="16" t="n">
+        <v>0.956422018348624</v>
       </c>
       <c r="S6" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T6" s="14" t="n">
-        <v>0.767106912789686</v>
-      </c>
-      <c r="U6" s="14" t="n">
-        <v>0.772505800441942</v>
+      <c r="T6" s="16" t="n">
+        <v>0.885031858670459</v>
+      </c>
+      <c r="U6" s="16" t="n">
+        <v>0.894910349391839</v>
       </c>
       <c r="V6" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W6" s="14" t="n">
-        <v>0.71830985915493</v>
+      <c r="W6" s="16" t="n">
+        <v>0.788732394366197</v>
       </c>
       <c r="X6" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -1841,75 +1971,75 @@
       </c>
       <c r="C7" s="13" t="n">
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
-        <v>0.728207755738953</v>
+        <v>0.761759832782204</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>0.417240141074992</v>
+        <v>0.597514874790058</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F7" s="14" t="n">
-        <v>0.315944982170148</v>
+        <v>0.478247580234335</v>
       </c>
       <c r="G7" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H7" s="14" t="n">
-        <v>0.779411764705882</v>
+        <v>0.757352941176471</v>
       </c>
       <c r="I7" s="14" t="n">
-        <v>0.84375</v>
+        <v>0.834170854271357</v>
       </c>
       <c r="J7" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K7" s="14" t="n">
-        <v>0.733088909257562</v>
+        <v>0.767975055025679</v>
       </c>
       <c r="L7" s="15" t="n">
-        <f aca="false">8/$K$3</f>
-        <v>0.00146439685154677</v>
+        <f aca="false">11/$K$3</f>
+        <v>0.00201354567087681</v>
       </c>
       <c r="M7" s="14" t="n">
-        <v>0.814964135542914</v>
+        <v>0.824560969577047</v>
       </c>
       <c r="N7" s="14" t="n">
-        <v>0.753954941621444</v>
+        <v>0.785041064339182</v>
       </c>
       <c r="O7" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P7" s="14" t="n">
-        <v>0.707581227436823</v>
+        <v>0.746376811594203</v>
       </c>
       <c r="Q7" s="15" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">1/$P$3</f>
+        <v>0.0036101083032491</v>
       </c>
       <c r="R7" s="14" t="n">
-        <v>0.907110091743119</v>
+        <v>0.95752009184845</v>
       </c>
       <c r="S7" s="15" t="n">
-        <f aca="false">0/$R$3</f>
-        <v>0</v>
+        <f aca="false">1/$R$3</f>
+        <v>0.00114678899082569</v>
       </c>
       <c r="T7" s="14" t="n">
-        <v>0.817610857364514</v>
+        <v>0.87058607341487</v>
       </c>
       <c r="U7" s="14" t="n">
-        <v>0.830934609499328</v>
+        <v>0.873884353171137</v>
       </c>
       <c r="V7" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W7" s="14" t="n">
-        <v>0.816901408450704</v>
+        <v>0.647887323943662</v>
       </c>
       <c r="X7" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -1925,68 +2055,68 @@
       </c>
       <c r="C8" s="13" t="n">
         <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
-        <v>0.723374373278101</v>
+        <v>0.740393758714782</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>0.451542212782268</v>
+        <v>0.526754313381707</v>
       </c>
       <c r="E8" s="15" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F8" s="14" t="n">
-        <v>0.462964849719817</v>
+        <v>0.418644931227713</v>
       </c>
       <c r="G8" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H8" s="14" t="n">
-        <v>0.801470588235294</v>
+        <v>0.737745098039216</v>
       </c>
       <c r="I8" s="14" t="n">
-        <v>0.850828729281768</v>
+        <v>0.820770519262982</v>
       </c>
       <c r="J8" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>0.8555738605162</v>
+        <v>0.833424858136555</v>
       </c>
       <c r="L8" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M8" s="14" t="n">
-        <v>0.822681177343557</v>
+        <v>0.765767994063814</v>
       </c>
       <c r="N8" s="14" t="n">
-        <v>0.777062536928196</v>
+        <v>0.742172610944732</v>
       </c>
       <c r="O8" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P8" s="14" t="n">
-        <v>0.317689530685921</v>
+        <v>0.84115523465704</v>
       </c>
       <c r="Q8" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R8" s="14" t="n">
-        <v>0.951834862385321</v>
+        <v>0.940366972477064</v>
       </c>
       <c r="S8" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T8" s="14" t="n">
-        <v>0.831672916702132</v>
+        <v>0.767106912789686</v>
       </c>
       <c r="U8" s="14" t="n">
-        <v>0.838861355601802</v>
+        <v>0.772505800441942</v>
       </c>
       <c r="V8" s="15" t="n">
         <f aca="false">0/$T$3</f>
@@ -2009,75 +2139,75 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
-        <v>0.658513623474907</v>
+        <v>0.728207755738953</v>
       </c>
       <c r="D9" s="14" t="n">
-        <v>0.523854029130735</v>
+        <v>0.417240141074992</v>
       </c>
       <c r="E9" s="15" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F9" s="14" t="n">
-        <v>0.480334216425515</v>
+        <v>0.315944982170148</v>
       </c>
       <c r="G9" s="15" t="n">
-        <f aca="false">1/$F$3</f>
-        <v>0.000101884870096791</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H9" s="14" t="n">
-        <v>0.727941176470588</v>
+        <v>0.779411764705882</v>
       </c>
       <c r="I9" s="14" t="n">
-        <v>0.821829855537721</v>
+        <v>0.84375</v>
       </c>
       <c r="J9" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K9" s="14" t="n">
-        <v>0.696448187477115</v>
+        <v>0.733088909257562</v>
       </c>
       <c r="L9" s="15" t="n">
-        <f aca="false">1/$K$3</f>
-        <v>0.000183049606443346</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
       </c>
       <c r="M9" s="14" t="n">
-        <v>0.509271935283136</v>
+        <v>0.814964135542914</v>
       </c>
       <c r="N9" s="14" t="n">
-        <v>0.593278732490252</v>
+        <v>0.753954941621444</v>
       </c>
       <c r="O9" s="15" t="n">
-        <f aca="false">255/$M$3</f>
-        <v>0.0063071976255256</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P9" s="14" t="n">
-        <v>0.249097472924188</v>
+        <v>0.707581227436823</v>
       </c>
       <c r="Q9" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R9" s="14" t="n">
-        <v>0.934633027522936</v>
+        <v>0.907110091743119</v>
       </c>
       <c r="S9" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T9" s="14" t="n">
-        <v>0.821663265900952</v>
+        <v>0.817610857364514</v>
       </c>
       <c r="U9" s="14" t="n">
-        <v>0.825501723380821</v>
+        <v>0.830934609499328</v>
       </c>
       <c r="V9" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W9" s="14" t="n">
-        <v>0.71830985915493</v>
+        <v>0.816901408450704</v>
       </c>
       <c r="X9" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -2093,75 +2223,75 @@
       </c>
       <c r="C10" s="13" t="n">
         <f aca="false">AVERAGE(W10,T10:U10,R10,P10,N10,M10,K10,H10,I10,F10,D10)</f>
-        <v>0.613554278796799</v>
+        <v>0.723374373278101</v>
       </c>
       <c r="D10" s="14" t="n">
-        <v>0.375051720670997</v>
+        <v>0.451542212782268</v>
       </c>
       <c r="E10" s="15" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F10" s="14" t="n">
-        <v>0.538767193071829</v>
+        <v>0.462964849719817</v>
       </c>
       <c r="G10" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H10" s="14" t="n">
-        <v>0.730392156862745</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I10" s="14" t="n">
-        <v>0.827044025157233</v>
+        <v>0.850828729281768</v>
       </c>
       <c r="J10" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K10" s="14" t="n">
-        <v>0.557386051619989</v>
+        <v>0.8555738605162</v>
       </c>
       <c r="L10" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M10" s="14" t="n">
-        <v>0.608706406134059</v>
+        <v>0.822681177343557</v>
       </c>
       <c r="N10" s="14" t="n">
-        <v>0.625189537528431</v>
+        <v>0.777062536928196</v>
       </c>
       <c r="O10" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P10" s="14" t="n">
-        <v>0.425992779783394</v>
+        <v>0.317689530685921</v>
       </c>
       <c r="Q10" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R10" s="14" t="n">
-        <v>0.932339449541284</v>
+        <v>0.951834862385321</v>
       </c>
       <c r="S10" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T10" s="14" t="n">
-        <v>0.573663619974553</v>
+        <v>0.831672916702132</v>
       </c>
       <c r="U10" s="14" t="n">
-        <v>0.590653616484677</v>
+        <v>0.838861355601802</v>
       </c>
       <c r="V10" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W10" s="14" t="n">
-        <v>0.577464788732394</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X10" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -2172,80 +2302,80 @@
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="13" t="n">
         <f aca="false">AVERAGE(W11,T11:U11,R11,P11,N11,M11,K11,H11,I11,F11,D11)</f>
-        <v>0.499454443668613</v>
-      </c>
-      <c r="D11" s="14" t="n">
-        <v>0.333471865271531</v>
+        <v>0.704245669484917</v>
+      </c>
+      <c r="D11" s="16" t="n">
+        <v>0.61400038680535</v>
       </c>
       <c r="E11" s="15" t="n">
-        <f aca="false">6/$D$3</f>
-        <v>0.00575263662511985</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F11" s="14" t="n">
-        <v>0.292103922567499</v>
+        <v>0.417524197656648</v>
       </c>
       <c r="G11" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H11" s="14" t="n">
-        <v>0.698529411764706</v>
+      <c r="H11" s="16" t="n">
+        <v>0.742647058823529</v>
       </c>
       <c r="I11" s="14" t="n">
-        <v>0.805687203791469</v>
+        <v>0.837209302325581</v>
       </c>
       <c r="J11" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K11" s="14" t="n">
-        <v>0.391434449223864</v>
+        <v>0.317480719794344</v>
       </c>
       <c r="L11" s="15" t="n">
-        <f aca="false">116/$K$3</f>
-        <v>0.0212337543474282</v>
-      </c>
-      <c r="M11" s="14" t="n">
-        <v>0.691602220900258</v>
+        <f aca="false">17/$K$3</f>
+        <v>0.00311184330953688</v>
+      </c>
+      <c r="M11" s="16" t="n">
+        <v>0.720652980460054</v>
       </c>
       <c r="N11" s="14" t="n">
-        <v>0.36669042044182</v>
+        <v>0.719543084181773</v>
       </c>
       <c r="O11" s="15" t="n">
-        <f aca="false">86/$M$3</f>
-        <v>0.00212713331684393</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P11" s="14" t="n">
-        <v>0.306859205776173</v>
+        <v>0.68231046931408</v>
       </c>
       <c r="Q11" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R11" s="14" t="n">
-        <v>0.855504587155963</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S11" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T11" s="14" t="n">
-        <v>0.370306926073738</v>
-      </c>
-      <c r="U11" s="14" t="n">
-        <v>0.402389871619712</v>
+      <c r="T11" s="16" t="n">
+        <v>0.860305870097761</v>
+      </c>
+      <c r="U11" s="16" t="n">
+        <v>0.871099781648942</v>
       </c>
       <c r="V11" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W11" s="14" t="n">
-        <v>0.47887323943662</v>
+      <c r="W11" s="16" t="n">
+        <v>0.732394366197183</v>
       </c>
       <c r="X11" s="15" t="n">
         <f aca="false">0/$W$3</f>
@@ -2256,68 +2386,250 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="13" t="n">
         <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
-        <v>0.721879431828856</v>
+        <v>0.658513623474907</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>0.618250159186482</v>
+        <v>0.523854029130735</v>
       </c>
       <c r="E12" s="15" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F12" s="14" t="n">
-        <v>0.411716760061131</v>
+        <v>0.480334216425515</v>
       </c>
       <c r="G12" s="15" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">1/$F$3</f>
+        <v>0.000101884870096791</v>
       </c>
       <c r="H12" s="14" t="n">
-        <v>0.806372549019608</v>
+        <v>0.727941176470588</v>
       </c>
       <c r="I12" s="14" t="n">
-        <v>0.866779089376054</v>
+        <v>0.821829855537721</v>
       </c>
       <c r="J12" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K12" s="14" t="n">
-        <v>0.906278601501007</v>
+        <v>0.696448187477115</v>
       </c>
       <c r="L12" s="15" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+        <f aca="false">1/$K$3</f>
+        <v>0.000183049606443346</v>
+      </c>
+      <c r="M12" s="14" t="n">
+        <v>0.509271935283136</v>
+      </c>
+      <c r="N12" s="14" t="n">
+        <v>0.593278732490252</v>
+      </c>
       <c r="O12" s="15" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="14"/>
+        <f aca="false">255/$M$3</f>
+        <v>0.0063071976255256</v>
+      </c>
+      <c r="P12" s="14" t="n">
+        <v>0.249097472924188</v>
+      </c>
       <c r="Q12" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R12" s="14"/>
+      <c r="R12" s="14" t="n">
+        <v>0.934633027522936</v>
+      </c>
       <c r="S12" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
+      <c r="T12" s="14" t="n">
+        <v>0.821663265900952</v>
+      </c>
+      <c r="U12" s="14" t="n">
+        <v>0.825501723380821</v>
+      </c>
       <c r="V12" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W12" s="14"/>
+      <c r="W12" s="14" t="n">
+        <v>0.71830985915493</v>
+      </c>
       <c r="X12" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <f aca="false">AVERAGE(W13,T13:U13,R13,P13,N13,M13,K13,H13,I13,F13,D13)</f>
+        <v>0.613554278796799</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>0.375051720670997</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <v>0.538767193071829</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <v>0.730392156862745</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <v>0.827044025157233</v>
+      </c>
+      <c r="J13" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="14" t="n">
+        <v>0.557386051619989</v>
+      </c>
+      <c r="L13" s="15" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="14" t="n">
+        <v>0.608706406134059</v>
+      </c>
+      <c r="N13" s="14" t="n">
+        <v>0.625189537528431</v>
+      </c>
+      <c r="O13" s="15" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="14" t="n">
+        <v>0.425992779783394</v>
+      </c>
+      <c r="Q13" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="14" t="n">
+        <v>0.932339449541284</v>
+      </c>
+      <c r="S13" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="14" t="n">
+        <v>0.573663619974553</v>
+      </c>
+      <c r="U13" s="14" t="n">
+        <v>0.590653616484677</v>
+      </c>
+      <c r="V13" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="14" t="n">
+        <v>0.577464788732394</v>
+      </c>
+      <c r="X13" s="15" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="13" t="n">
+        <f aca="false">AVERAGE(W14,T14:U14,R14,P14,N14,M14,K14,H14,I14,F14,D14)</f>
+        <v>0.499454443668613</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>0.333471865271531</v>
+      </c>
+      <c r="E14" s="15" t="n">
+        <f aca="false">6/$D$3</f>
+        <v>0.00575263662511985</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <v>0.292103922567499</v>
+      </c>
+      <c r="G14" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <v>0.698529411764706</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <v>0.805687203791469</v>
+      </c>
+      <c r="J14" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="14" t="n">
+        <v>0.391434449223864</v>
+      </c>
+      <c r="L14" s="15" t="n">
+        <f aca="false">116/$K$3</f>
+        <v>0.0212337543474282</v>
+      </c>
+      <c r="M14" s="14" t="n">
+        <v>0.691602220900258</v>
+      </c>
+      <c r="N14" s="14" t="n">
+        <v>0.36669042044182</v>
+      </c>
+      <c r="O14" s="15" t="n">
+        <f aca="false">86/$M$3</f>
+        <v>0.00212713331684393</v>
+      </c>
+      <c r="P14" s="14" t="n">
+        <v>0.306859205776173</v>
+      </c>
+      <c r="Q14" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="14" t="n">
+        <v>0.855504587155963</v>
+      </c>
+      <c r="S14" s="15" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="14" t="n">
+        <v>0.370306926073738</v>
+      </c>
+      <c r="U14" s="14" t="n">
+        <v>0.402389871619712</v>
+      </c>
+      <c r="V14" s="15" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="14" t="n">
+        <v>0.47887323943662</v>
+      </c>
+      <c r="X14" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -2336,8 +2648,8 @@
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="W2:X2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+  <conditionalFormatting sqref="G4:G48 J4:J48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48 E4:E48 L4:L48">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2463,14 +2775,16 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2479,8 +2793,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <drawing r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -2489,10 +2803,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2522,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2543,27 +2857,27 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="1"/>
@@ -2609,10 +2923,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C4" s="13" t="n">
         <f aca="false">AVERAGE(D4,F4,H4,J4,L4,N4)</f>
@@ -2717,10 +3031,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" s="13" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
@@ -2771,10 +3085,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="13" t="n">
         <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
@@ -2825,10 +3139,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" s="13" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
@@ -2879,49 +3193,49 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
-        <v>0.432443158810545</v>
+        <v>0.43930732492985</v>
       </c>
       <c r="D9" s="14" t="n">
-        <v>0.0718486458091463</v>
+        <v>0.127338801833183</v>
       </c>
       <c r="E9" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F9" s="14" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H9" s="14" t="n">
-        <v>0.378640776699029</v>
+      <c r="H9" s="16" t="n">
+        <v>0.388349514563107</v>
       </c>
       <c r="I9" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J9" s="14" t="n">
-        <v>0.444444444444444</v>
+      <c r="J9" s="16" t="n">
+        <v>0.442148760330579</v>
       </c>
       <c r="K9" s="15" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L9" s="14" t="n">
-        <v>0.629725085910653</v>
+        <v>0.628006872852234</v>
       </c>
       <c r="M9" s="15" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N9" s="14" t="n">
         <v>0.55</v>
@@ -2935,50 +3249,50 @@
       <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="13" t="n">
         <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
-        <v>0.426274378090213</v>
-      </c>
-      <c r="D10" s="14" t="n">
-        <v>0.0702149056307087</v>
+        <v>0.436042704459863</v>
+      </c>
+      <c r="D10" s="16" t="n">
+        <v>0.0518271447518188</v>
       </c>
       <c r="E10" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F10" s="14" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H10" s="14" t="n">
-        <v>0.396039603960396</v>
+      <c r="H10" s="16" t="n">
+        <v>0.398058252427184</v>
       </c>
       <c r="I10" s="15" t="n">
-        <f aca="false">2/$H$3</f>
-        <v>0.0194174757281553</v>
-      </c>
-      <c r="J10" s="14" t="n">
-        <v>0.460905349794239</v>
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="16" t="n">
+        <v>0.448559670781893</v>
       </c>
       <c r="K10" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L10" s="14" t="n">
-        <v>0.67381974248927</v>
+      <c r="L10" s="16" t="n">
+        <v>0.667811158798283</v>
       </c>
       <c r="M10" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N10" s="14" t="n">
-        <v>0.466666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="O10" s="15" t="n">
         <f aca="false">0/$N$3</f>
@@ -2987,52 +3301,52 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="13" t="n">
         <f aca="false">AVERAGE(D11,F11,H11,J11,L11,N11)</f>
-        <v>0.419278530088385</v>
+        <v>0.432443158810545</v>
       </c>
       <c r="D11" s="14" t="n">
-        <v>-0.0155335936055105</v>
+        <v>0.0718486458091463</v>
       </c>
       <c r="E11" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F11" s="14" t="n">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G11" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H11" s="14" t="n">
-        <v>0.368932038834951</v>
+        <v>0.378640776699029</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J11" s="14" t="n">
-        <v>0.489711934156379</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K11" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L11" s="14" t="n">
-        <v>0.659227467811159</v>
+        <v>0.629725085910653</v>
       </c>
       <c r="M11" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N11" s="14" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O11" s="15" t="n">
         <f aca="false">0/$N$3</f>
@@ -3041,56 +3355,218 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C12" s="13" t="n">
         <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
-        <v>0.405257833604129</v>
+        <v>0.426274378090213</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>-0.0714529452409867</v>
+        <v>0.0702149056307087</v>
       </c>
       <c r="E12" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F12" s="14" t="n">
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="G12" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H12" s="14" t="n">
-        <v>0.378640776699029</v>
+        <v>0.396039603960396</v>
       </c>
       <c r="I12" s="15" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
+        <f aca="false">2/$H$3</f>
+        <v>0.0194174757281553</v>
       </c>
       <c r="J12" s="14" t="n">
-        <v>0.469135802469136</v>
+        <v>0.460905349794239</v>
       </c>
       <c r="K12" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L12" s="14" t="n">
+        <v>0.67381974248927</v>
+      </c>
+      <c r="M12" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="14" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="O12" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <f aca="false">AVERAGE(D13,F13,H13,J13,L13,N13)</f>
+        <v>0.419278530088385</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>-0.0155335936055105</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <v>0.368932038834951</v>
+      </c>
+      <c r="I13" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="14" t="n">
+        <v>0.489711934156379</v>
+      </c>
+      <c r="K13" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="14" t="n">
+        <v>0.659227467811159</v>
+      </c>
+      <c r="M13" s="15" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="14" t="n">
+        <v>0.533333333333333</v>
+      </c>
+      <c r="O13" s="15" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="13" t="n">
+        <f aca="false">AVERAGE(D14,F14,H14,J14,L14,N14)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E14" s="15" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G14" s="15" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I14" s="15" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="14" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K14" s="15" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="14" t="n">
         <v>0.618556701030928</v>
       </c>
-      <c r="M12" s="15" t="n">
+      <c r="M14" s="15" t="n">
         <f aca="false">1/$L$3</f>
         <v>0.000858369098712446</v>
       </c>
-      <c r="N12" s="14" t="n">
+      <c r="N14" s="14" t="n">
         <v>0.516666666666667</v>
       </c>
-      <c r="O12" s="15" t="n">
+      <c r="O14" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="13" t="n">
+        <f aca="false">AVERAGE(D15,F15,H15,J15,L15,N15)</f>
+        <v>0.364587789621774</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>0.0266825503923221</v>
+      </c>
+      <c r="E15" s="15" t="n">
+        <f aca="false">187/$D$3</f>
+        <v>0.205494505494505</v>
+      </c>
+      <c r="F15" s="14" t="n">
+        <v>0.461538461538462</v>
+      </c>
+      <c r="G15" s="15" t="n">
+        <f aca="false">9/$F$3</f>
+        <v>0.09</v>
+      </c>
+      <c r="H15" s="14" t="n">
+        <v>0.237113402061856</v>
+      </c>
+      <c r="I15" s="15" t="n">
+        <f aca="false">6/$H$3</f>
+        <v>0.058252427184466</v>
+      </c>
+      <c r="J15" s="16" t="n">
+        <v>0.558823529411765</v>
+      </c>
+      <c r="K15" s="15" t="n">
+        <f aca="false">39/$J$3</f>
+        <v>0.160493827160494</v>
+      </c>
+      <c r="L15" s="14" t="n">
+        <v>0.403368794326241</v>
+      </c>
+      <c r="M15" s="15" t="n">
+        <f aca="false">37/$L$3</f>
+        <v>0.0317596566523605</v>
+      </c>
+      <c r="N15" s="14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="15" t="n">
+        <f aca="false">2/$N$3</f>
+        <v>0.0333333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -3104,8 +3580,8 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+  <conditionalFormatting sqref="G4:G28 I4:I28 K4:K28 M4:M28 O4:O28 E4:E28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3175,10 +3651,13 @@
     <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
     <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
     <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3187,7 +3666,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <drawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BLEU eval, and results
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'GLUE Results'!$A$3:$X$48</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'HuLU Results'!$A$3:$O$47</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'HuLU Results'!$A$3:$S$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -221,12 +221,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="P2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">BLEU score,
+Length ratio,
+Spell error %</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -345,6 +359,9 @@
     <t xml:space="preserve">HuLU</t>
   </si>
   <si>
+    <t xml:space="preserve">BLEU</t>
+  </si>
+  <si>
     <t xml:space="preserve">HuCoLA</t>
   </si>
   <si>
@@ -361,6 +378,9 @@
   </si>
   <si>
     <t xml:space="preserve">HuWNLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English → Hungarian</t>
   </si>
   <si>
     <t xml:space="preserve">gpt-35-turbo-instruct</t>
@@ -379,12 +399,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -431,13 +453,6 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -493,76 +508,108 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,7 +622,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="123">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1432,6 +1479,126 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF85B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FA468"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB49969"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB79769"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD7846B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDC816B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79BB65"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FB865"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82B665"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8AB166"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CB066"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4A267"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC09269"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC68E69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF5736C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFC6F6C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1635,1172 +1802,1172 @@
   <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="15:15 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="4" width="6.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="6" t="s">
+    <row r="2" s="6" customFormat="true" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4" t="s">
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="4"/>
+      <c r="X2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>1043</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="8" t="n">
         <v>9815</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="8" t="n">
         <v>408</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="7" t="n">
+      <c r="K3" s="8" t="n">
         <v>5463</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="10" t="n">
         <v>40430</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="8" t="s">
+      <c r="N3" s="8"/>
+      <c r="O3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="9" t="n">
+      <c r="P3" s="10" t="n">
         <v>277</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="9" t="n">
+      <c r="R3" s="10" t="n">
         <v>872</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="8" t="s">
+      <c r="U3" s="8"/>
+      <c r="V3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="W3" s="8" t="n">
         <v>71</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="13" t="n">
         <f aca="false">AVERAGE(W4,T4:U4,R4,P4,N4,M4,K4,H4,I4,F4,D4)</f>
         <v>0.811496442612959</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="14" t="n">
         <v>0.583123781456463</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="14" t="n">
         <v>0.362506367804381</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="14" t="n">
         <v>0.794117647058824</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="14" t="n">
         <v>0.857627118644068</v>
       </c>
-      <c r="J4" s="14" t="n">
+      <c r="J4" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K4" s="13" t="n">
+      <c r="K4" s="14" t="n">
         <v>0.900787113307706</v>
       </c>
-      <c r="L4" s="14" t="n">
+      <c r="L4" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M4" s="13" t="n">
+      <c r="M4" s="14" t="n">
         <v>0.857853079396488</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N4" s="14" t="n">
         <v>0.815048434332057</v>
       </c>
-      <c r="O4" s="14" t="n">
+      <c r="O4" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="13" t="n">
+      <c r="P4" s="14" t="n">
         <v>0.942238267148014</v>
       </c>
-      <c r="Q4" s="14" t="n">
+      <c r="Q4" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R4" s="13" t="n">
+      <c r="R4" s="14" t="n">
         <v>0.92545871559633</v>
       </c>
-      <c r="S4" s="14" t="n">
+      <c r="S4" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T4" s="13" t="n">
+      <c r="T4" s="14" t="n">
         <v>0.903148288781267</v>
       </c>
-      <c r="U4" s="13" t="n">
+      <c r="U4" s="14" t="n">
         <v>0.908724554167942</v>
       </c>
-      <c r="V4" s="14" t="n">
+      <c r="V4" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W4" s="13" t="n">
+      <c r="W4" s="14" t="n">
         <v>0.887323943661972</v>
       </c>
-      <c r="X4" s="14" t="n">
+      <c r="X4" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">AVERAGE(W5,T5:U5,R5,P5,N5,M5,K5,H5,I5,F5,D5)</f>
         <v>0.809456837704127</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="14" t="n">
         <v>0.665512350161472</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="14" t="n">
         <v>0.43301069791136</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H5" s="14" t="n">
         <v>0.838235294117647</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="14" t="n">
         <v>0.881294964028777</v>
       </c>
-      <c r="J5" s="14" t="n">
+      <c r="J5" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K5" s="13" t="n">
+      <c r="K5" s="14" t="n">
         <v>0.85337726523888</v>
       </c>
-      <c r="L5" s="14" t="n">
+      <c r="L5" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M5" s="13" t="n">
+      <c r="M5" s="14" t="n">
         <v>0.860697501855058</v>
       </c>
-      <c r="N5" s="13" t="n">
+      <c r="N5" s="14" t="n">
         <v>0.806951395077809</v>
       </c>
-      <c r="O5" s="14" t="n">
+      <c r="O5" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="13" t="n">
+      <c r="P5" s="14" t="n">
         <v>0.859205776173285</v>
       </c>
-      <c r="Q5" s="14" t="n">
+      <c r="Q5" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R5" s="13" t="n">
+      <c r="R5" s="14" t="n">
         <v>0.951834862385321</v>
       </c>
-      <c r="S5" s="14" t="n">
+      <c r="S5" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T5" s="13" t="n">
+      <c r="T5" s="14" t="n">
         <v>0.886830850881204</v>
       </c>
-      <c r="U5" s="13" t="n">
+      <c r="U5" s="14" t="n">
         <v>0.887798700252512</v>
       </c>
-      <c r="V5" s="14" t="n">
+      <c r="V5" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W5" s="13" t="n">
+      <c r="W5" s="14" t="n">
         <v>0.788732394366197</v>
       </c>
-      <c r="X5" s="14" t="n">
+      <c r="X5" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">AVERAGE(W6,T6:U6,R6,P6,N6,M6,K6,H6,I6,F6,D6)</f>
         <v>0.799244376594315</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="14" t="n">
         <v>0.618250159186482</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="14" t="n">
         <v>0.411716760061131</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G6" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H6" s="13" t="n">
+      <c r="H6" s="14" t="n">
         <v>0.806372549019608</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I6" s="14" t="n">
         <v>0.866779089376054</v>
       </c>
-      <c r="J6" s="14" t="n">
+      <c r="J6" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K6" s="13" t="n">
+      <c r="K6" s="14" t="n">
         <v>0.906278601501007</v>
       </c>
-      <c r="L6" s="14" t="n">
+      <c r="L6" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M6" s="13" t="n">
+      <c r="M6" s="14" t="n">
         <v>0.812663863467722</v>
       </c>
-      <c r="N6" s="13" t="n">
+      <c r="N6" s="14" t="n">
         <v>0.780958991266123</v>
       </c>
-      <c r="O6" s="14" t="n">
+      <c r="O6" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="13" t="n">
+      <c r="P6" s="14" t="n">
         <v>0.862815884476534</v>
       </c>
-      <c r="Q6" s="14" t="n">
+      <c r="Q6" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R6" s="13" t="n">
+      <c r="R6" s="14" t="n">
         <v>0.956422018348624</v>
       </c>
-      <c r="S6" s="14" t="n">
+      <c r="S6" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T6" s="13" t="n">
+      <c r="T6" s="14" t="n">
         <v>0.885031858670459</v>
       </c>
-      <c r="U6" s="13" t="n">
+      <c r="U6" s="14" t="n">
         <v>0.894910349391839</v>
       </c>
-      <c r="V6" s="14" t="n">
+      <c r="V6" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W6" s="13" t="n">
+      <c r="W6" s="14" t="n">
         <v>0.788732394366197</v>
       </c>
-      <c r="X6" s="14" t="n">
+      <c r="X6" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="13" t="n">
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
         <v>0.761759832782204</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="14" t="n">
         <v>0.597514874790058</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>0.478247580234335</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G7" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <v>0.757352941176471</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I7" s="14" t="n">
         <v>0.834170854271357</v>
       </c>
-      <c r="J7" s="14" t="n">
+      <c r="J7" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K7" s="13" t="n">
+      <c r="K7" s="14" t="n">
         <v>0.767975055025679</v>
       </c>
-      <c r="L7" s="14" t="n">
+      <c r="L7" s="15" t="n">
         <f aca="false">11/$K$3</f>
         <v>0.00201354567087681</v>
       </c>
-      <c r="M7" s="13" t="n">
+      <c r="M7" s="14" t="n">
         <v>0.824560969577047</v>
       </c>
-      <c r="N7" s="13" t="n">
+      <c r="N7" s="14" t="n">
         <v>0.785041064339182</v>
       </c>
-      <c r="O7" s="14" t="n">
+      <c r="O7" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="13" t="n">
+      <c r="P7" s="14" t="n">
         <v>0.746376811594203</v>
       </c>
-      <c r="Q7" s="14" t="n">
+      <c r="Q7" s="15" t="n">
         <f aca="false">1/$P$3</f>
         <v>0.0036101083032491</v>
       </c>
-      <c r="R7" s="13" t="n">
+      <c r="R7" s="14" t="n">
         <v>0.95752009184845</v>
       </c>
-      <c r="S7" s="14" t="n">
+      <c r="S7" s="15" t="n">
         <f aca="false">1/$R$3</f>
         <v>0.00114678899082569</v>
       </c>
-      <c r="T7" s="13" t="n">
+      <c r="T7" s="14" t="n">
         <v>0.87058607341487</v>
       </c>
-      <c r="U7" s="13" t="n">
+      <c r="U7" s="14" t="n">
         <v>0.873884353171137</v>
       </c>
-      <c r="V7" s="14" t="n">
+      <c r="V7" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W7" s="13" t="n">
+      <c r="W7" s="14" t="n">
         <v>0.647887323943662</v>
       </c>
-      <c r="X7" s="14" t="n">
+      <c r="X7" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
         <v>0.740393758714782</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="14" t="n">
         <v>0.526754313381707</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>0.418644931227713</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G8" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H8" s="13" t="n">
+      <c r="H8" s="14" t="n">
         <v>0.737745098039216</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="14" t="n">
         <v>0.820770519262982</v>
       </c>
-      <c r="J8" s="14" t="n">
+      <c r="J8" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="14" t="n">
         <v>0.833424858136555</v>
       </c>
-      <c r="L8" s="14" t="n">
+      <c r="L8" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M8" s="13" t="n">
+      <c r="M8" s="14" t="n">
         <v>0.765767994063814</v>
       </c>
-      <c r="N8" s="13" t="n">
+      <c r="N8" s="14" t="n">
         <v>0.742172610944732</v>
       </c>
-      <c r="O8" s="14" t="n">
+      <c r="O8" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P8" s="13" t="n">
+      <c r="P8" s="14" t="n">
         <v>0.84115523465704</v>
       </c>
-      <c r="Q8" s="14" t="n">
+      <c r="Q8" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R8" s="13" t="n">
+      <c r="R8" s="14" t="n">
         <v>0.940366972477064</v>
       </c>
-      <c r="S8" s="14" t="n">
+      <c r="S8" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T8" s="13" t="n">
+      <c r="T8" s="14" t="n">
         <v>0.767106912789686</v>
       </c>
-      <c r="U8" s="13" t="n">
+      <c r="U8" s="14" t="n">
         <v>0.772505800441942</v>
       </c>
-      <c r="V8" s="14" t="n">
+      <c r="V8" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W8" s="13" t="n">
+      <c r="W8" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X8" s="14" t="n">
+      <c r="X8" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="13" t="n">
         <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
         <v>0.728207755738953</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="14" t="n">
         <v>0.417240141074992</v>
       </c>
-      <c r="E9" s="14" t="n">
+      <c r="E9" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F9" s="13" t="n">
+      <c r="F9" s="14" t="n">
         <v>0.315944982170148</v>
       </c>
-      <c r="G9" s="14" t="n">
+      <c r="G9" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H9" s="13" t="n">
+      <c r="H9" s="14" t="n">
         <v>0.779411764705882</v>
       </c>
-      <c r="I9" s="13" t="n">
+      <c r="I9" s="14" t="n">
         <v>0.84375</v>
       </c>
-      <c r="J9" s="14" t="n">
+      <c r="J9" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="K9" s="14" t="n">
         <v>0.733088909257562</v>
       </c>
-      <c r="L9" s="14" t="n">
+      <c r="L9" s="15" t="n">
         <f aca="false">8/$K$3</f>
         <v>0.00146439685154677</v>
       </c>
-      <c r="M9" s="13" t="n">
+      <c r="M9" s="14" t="n">
         <v>0.814964135542914</v>
       </c>
-      <c r="N9" s="13" t="n">
+      <c r="N9" s="14" t="n">
         <v>0.753954941621444</v>
       </c>
-      <c r="O9" s="14" t="n">
+      <c r="O9" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P9" s="13" t="n">
+      <c r="P9" s="14" t="n">
         <v>0.707581227436823</v>
       </c>
-      <c r="Q9" s="14" t="n">
+      <c r="Q9" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R9" s="13" t="n">
+      <c r="R9" s="14" t="n">
         <v>0.907110091743119</v>
       </c>
-      <c r="S9" s="14" t="n">
+      <c r="S9" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T9" s="13" t="n">
+      <c r="T9" s="14" t="n">
         <v>0.817610857364514</v>
       </c>
-      <c r="U9" s="13" t="n">
+      <c r="U9" s="14" t="n">
         <v>0.830934609499328</v>
       </c>
-      <c r="V9" s="14" t="n">
+      <c r="V9" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W9" s="13" t="n">
+      <c r="W9" s="14" t="n">
         <v>0.816901408450704</v>
       </c>
-      <c r="X9" s="14" t="n">
+      <c r="X9" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="13" t="n">
         <f aca="false">AVERAGE(W10,T10:U10,R10,P10,N10,M10,K10,H10,I10,F10,D10)</f>
         <v>0.723374373278101</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="14" t="n">
         <v>0.451542212782268</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E10" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="14" t="n">
         <v>0.462964849719817</v>
       </c>
-      <c r="G10" s="14" t="n">
+      <c r="G10" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H10" s="13" t="n">
+      <c r="H10" s="14" t="n">
         <v>0.801470588235294</v>
       </c>
-      <c r="I10" s="13" t="n">
+      <c r="I10" s="14" t="n">
         <v>0.850828729281768</v>
       </c>
-      <c r="J10" s="14" t="n">
+      <c r="J10" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="14" t="n">
         <v>0.8555738605162</v>
       </c>
-      <c r="L10" s="14" t="n">
+      <c r="L10" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M10" s="13" t="n">
+      <c r="M10" s="14" t="n">
         <v>0.822681177343557</v>
       </c>
-      <c r="N10" s="13" t="n">
+      <c r="N10" s="14" t="n">
         <v>0.777062536928196</v>
       </c>
-      <c r="O10" s="14" t="n">
+      <c r="O10" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P10" s="13" t="n">
+      <c r="P10" s="14" t="n">
         <v>0.317689530685921</v>
       </c>
-      <c r="Q10" s="14" t="n">
+      <c r="Q10" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R10" s="13" t="n">
+      <c r="R10" s="14" t="n">
         <v>0.951834862385321</v>
       </c>
-      <c r="S10" s="14" t="n">
+      <c r="S10" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T10" s="13" t="n">
+      <c r="T10" s="14" t="n">
         <v>0.831672916702132</v>
       </c>
-      <c r="U10" s="13" t="n">
+      <c r="U10" s="14" t="n">
         <v>0.838861355601802</v>
       </c>
-      <c r="V10" s="14" t="n">
+      <c r="V10" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W10" s="13" t="n">
+      <c r="W10" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X10" s="14" t="n">
+      <c r="X10" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="13" t="n">
         <f aca="false">AVERAGE(W11,T11:U11,R11,P11,N11,M11,K11,H11,I11,F11,D11)</f>
         <v>0.704245669484917</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>0.61400038680535</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="15" t="n">
         <f aca="false">3/$D$3</f>
         <v>0.00287631831255992</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F11" s="14" t="n">
         <v>0.417524197656648</v>
       </c>
-      <c r="G11" s="14" t="n">
+      <c r="G11" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <v>0.742647058823529</v>
       </c>
-      <c r="I11" s="13" t="n">
+      <c r="I11" s="14" t="n">
         <v>0.837209302325581</v>
       </c>
-      <c r="J11" s="14" t="n">
+      <c r="J11" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K11" s="13" t="n">
+      <c r="K11" s="14" t="n">
         <v>0.317480719794344</v>
       </c>
-      <c r="L11" s="14" t="n">
+      <c r="L11" s="15" t="n">
         <f aca="false">17/$K$3</f>
         <v>0.00311184330953688</v>
       </c>
-      <c r="M11" s="13" t="n">
+      <c r="M11" s="14" t="n">
         <v>0.720652980460054</v>
       </c>
-      <c r="N11" s="13" t="n">
+      <c r="N11" s="14" t="n">
         <v>0.719543084181773</v>
       </c>
-      <c r="O11" s="14" t="n">
+      <c r="O11" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P11" s="13" t="n">
+      <c r="P11" s="14" t="n">
         <v>0.68231046931408</v>
       </c>
-      <c r="Q11" s="14" t="n">
+      <c r="Q11" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R11" s="13" t="n">
+      <c r="R11" s="14" t="n">
         <v>0.935779816513762</v>
       </c>
-      <c r="S11" s="14" t="n">
+      <c r="S11" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T11" s="13" t="n">
+      <c r="T11" s="14" t="n">
         <v>0.860305870097761</v>
       </c>
-      <c r="U11" s="13" t="n">
+      <c r="U11" s="14" t="n">
         <v>0.871099781648942</v>
       </c>
-      <c r="V11" s="14" t="n">
+      <c r="V11" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W11" s="13" t="n">
+      <c r="W11" s="14" t="n">
         <v>0.732394366197183</v>
       </c>
-      <c r="X11" s="14" t="n">
+      <c r="X11" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="12" t="n">
+      <c r="C12" s="13" t="n">
         <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
         <v>0.658513623474907</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="14" t="n">
         <v>0.523854029130735</v>
       </c>
-      <c r="E12" s="14" t="n">
+      <c r="E12" s="15" t="n">
         <f aca="false">3/$D$3</f>
         <v>0.00287631831255992</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F12" s="14" t="n">
         <v>0.480334216425515</v>
       </c>
-      <c r="G12" s="14" t="n">
+      <c r="G12" s="15" t="n">
         <f aca="false">1/$F$3</f>
         <v>0.000101884870096791</v>
       </c>
-      <c r="H12" s="13" t="n">
+      <c r="H12" s="14" t="n">
         <v>0.727941176470588</v>
       </c>
-      <c r="I12" s="13" t="n">
+      <c r="I12" s="14" t="n">
         <v>0.821829855537721</v>
       </c>
-      <c r="J12" s="14" t="n">
+      <c r="J12" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K12" s="13" t="n">
+      <c r="K12" s="14" t="n">
         <v>0.696448187477115</v>
       </c>
-      <c r="L12" s="14" t="n">
+      <c r="L12" s="15" t="n">
         <f aca="false">1/$K$3</f>
         <v>0.000183049606443346</v>
       </c>
-      <c r="M12" s="13" t="n">
+      <c r="M12" s="14" t="n">
         <v>0.509271935283136</v>
       </c>
-      <c r="N12" s="13" t="n">
+      <c r="N12" s="14" t="n">
         <v>0.593278732490252</v>
       </c>
-      <c r="O12" s="14" t="n">
+      <c r="O12" s="15" t="n">
         <f aca="false">255/$M$3</f>
         <v>0.0063071976255256</v>
       </c>
-      <c r="P12" s="13" t="n">
+      <c r="P12" s="14" t="n">
         <v>0.249097472924188</v>
       </c>
-      <c r="Q12" s="14" t="n">
+      <c r="Q12" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R12" s="13" t="n">
+      <c r="R12" s="14" t="n">
         <v>0.934633027522936</v>
       </c>
-      <c r="S12" s="14" t="n">
+      <c r="S12" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T12" s="13" t="n">
+      <c r="T12" s="14" t="n">
         <v>0.821663265900952</v>
       </c>
-      <c r="U12" s="13" t="n">
+      <c r="U12" s="14" t="n">
         <v>0.825501723380821</v>
       </c>
-      <c r="V12" s="14" t="n">
+      <c r="V12" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W12" s="13" t="n">
+      <c r="W12" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X12" s="14" t="n">
+      <c r="X12" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="13" t="n">
         <f aca="false">AVERAGE(W13,T13:U13,R13,P13,N13,M13,K13,H13,I13,F13,D13)</f>
         <v>0.653779197430066</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="14" t="n">
         <v>0.455627237079107</v>
       </c>
-      <c r="E13" s="14" t="n">
+      <c r="E13" s="15" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F13" s="13" t="n">
+      <c r="F13" s="14" t="n">
         <v>0.386958736627611</v>
       </c>
-      <c r="G13" s="14" t="n">
+      <c r="G13" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H13" s="13" t="n">
+      <c r="H13" s="14" t="n">
         <v>0.754901960784314</v>
       </c>
-      <c r="I13" s="13" t="n">
+      <c r="I13" s="14" t="n">
         <v>0.835526315789474</v>
       </c>
-      <c r="J13" s="14" t="n">
+      <c r="J13" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K13" s="13" t="n">
+      <c r="K13" s="14" t="n">
         <v>0.136371956800293</v>
       </c>
-      <c r="L13" s="14" t="n">
+      <c r="L13" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M13" s="13" t="n">
+      <c r="M13" s="14" t="n">
         <v>0.82352213702696</v>
       </c>
-      <c r="N13" s="13" t="n">
+      <c r="N13" s="14" t="n">
         <v>0.77733046219143</v>
       </c>
-      <c r="O13" s="14" t="n">
+      <c r="O13" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P13" s="13" t="n">
+      <c r="P13" s="14" t="n">
         <v>0.353790613718412</v>
       </c>
-      <c r="Q13" s="14" t="n">
+      <c r="Q13" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R13" s="13" t="n">
+      <c r="R13" s="14" t="n">
         <v>0.935779816513762</v>
       </c>
-      <c r="S13" s="14" t="n">
+      <c r="S13" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T13" s="13" t="n">
+      <c r="T13" s="14" t="n">
         <v>0.826388381403035</v>
       </c>
-      <c r="U13" s="13" t="n">
+      <c r="U13" s="14" t="n">
         <v>0.840842892071465</v>
       </c>
-      <c r="V13" s="14" t="n">
+      <c r="V13" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W13" s="13" t="n">
+      <c r="W13" s="14" t="n">
         <v>0.71830985915493</v>
       </c>
-      <c r="X13" s="14" t="n">
+      <c r="X13" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="13" t="n">
         <f aca="false">AVERAGE(W14,T14:U14,R14,P14,N14,M14,K14,H14,I14,F14,D14)</f>
         <v>0.613554278796799</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="14" t="n">
         <v>0.375051720670997</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F14" s="13" t="n">
+      <c r="F14" s="14" t="n">
         <v>0.538767193071829</v>
       </c>
-      <c r="G14" s="14" t="n">
+      <c r="G14" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H14" s="13" t="n">
+      <c r="H14" s="14" t="n">
         <v>0.730392156862745</v>
       </c>
-      <c r="I14" s="13" t="n">
+      <c r="I14" s="14" t="n">
         <v>0.827044025157233</v>
       </c>
-      <c r="J14" s="14" t="n">
+      <c r="J14" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K14" s="13" t="n">
+      <c r="K14" s="14" t="n">
         <v>0.557386051619989</v>
       </c>
-      <c r="L14" s="14" t="n">
+      <c r="L14" s="15" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M14" s="13" t="n">
+      <c r="M14" s="14" t="n">
         <v>0.608706406134059</v>
       </c>
-      <c r="N14" s="13" t="n">
+      <c r="N14" s="14" t="n">
         <v>0.625189537528431</v>
       </c>
-      <c r="O14" s="14" t="n">
+      <c r="O14" s="15" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P14" s="13" t="n">
+      <c r="P14" s="14" t="n">
         <v>0.425992779783394</v>
       </c>
-      <c r="Q14" s="14" t="n">
+      <c r="Q14" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R14" s="13" t="n">
+      <c r="R14" s="14" t="n">
         <v>0.932339449541284</v>
       </c>
-      <c r="S14" s="14" t="n">
+      <c r="S14" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T14" s="13" t="n">
+      <c r="T14" s="14" t="n">
         <v>0.573663619974553</v>
       </c>
-      <c r="U14" s="13" t="n">
+      <c r="U14" s="14" t="n">
         <v>0.590653616484677</v>
       </c>
-      <c r="V14" s="14" t="n">
+      <c r="V14" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W14" s="13" t="n">
+      <c r="W14" s="14" t="n">
         <v>0.577464788732394</v>
       </c>
-      <c r="X14" s="14" t="n">
+      <c r="X14" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="12" t="n">
+      <c r="C15" s="13" t="n">
         <f aca="false">AVERAGE(W15,T15:U15,R15,P15,N15,M15,K15,H15,I15,F15,D15)</f>
         <v>0.499454443668613</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="14" t="n">
         <v>0.333471865271531</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="15" t="n">
         <f aca="false">6/$D$3</f>
         <v>0.00575263662511985</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="14" t="n">
         <v>0.292103922567499</v>
       </c>
-      <c r="G15" s="14" t="n">
+      <c r="G15" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="14" t="n">
         <v>0.698529411764706</v>
       </c>
-      <c r="I15" s="13" t="n">
+      <c r="I15" s="14" t="n">
         <v>0.805687203791469</v>
       </c>
-      <c r="J15" s="14" t="n">
+      <c r="J15" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K15" s="13" t="n">
+      <c r="K15" s="14" t="n">
         <v>0.391434449223864</v>
       </c>
-      <c r="L15" s="14" t="n">
+      <c r="L15" s="15" t="n">
         <f aca="false">116/$K$3</f>
         <v>0.0212337543474282</v>
       </c>
-      <c r="M15" s="13" t="n">
+      <c r="M15" s="14" t="n">
         <v>0.691602220900258</v>
       </c>
-      <c r="N15" s="13" t="n">
+      <c r="N15" s="14" t="n">
         <v>0.36669042044182</v>
       </c>
-      <c r="O15" s="14" t="n">
+      <c r="O15" s="15" t="n">
         <f aca="false">86/$M$3</f>
         <v>0.00212713331684393</v>
       </c>
-      <c r="P15" s="13" t="n">
+      <c r="P15" s="14" t="n">
         <v>0.306859205776173</v>
       </c>
-      <c r="Q15" s="14" t="n">
+      <c r="Q15" s="15" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R15" s="13" t="n">
+      <c r="R15" s="14" t="n">
         <v>0.855504587155963</v>
       </c>
-      <c r="S15" s="14" t="n">
+      <c r="S15" s="15" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T15" s="13" t="n">
+      <c r="T15" s="14" t="n">
         <v>0.370306926073738</v>
       </c>
-      <c r="U15" s="13" t="n">
+      <c r="U15" s="14" t="n">
         <v>0.402389871619712</v>
       </c>
-      <c r="V15" s="14" t="n">
+      <c r="V15" s="15" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W15" s="13" t="n">
+      <c r="W15" s="14" t="n">
         <v>0.47887323943662</v>
       </c>
-      <c r="X15" s="14" t="n">
+      <c r="X15" s="15" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -2975,898 +3142,1086 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="15:15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="16" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>910</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="8" t="n">
         <v>103</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="10" t="n">
         <v>243</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <v>1165</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="7" t="n">
+      <c r="N3" s="8" t="n">
         <v>60</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="S3" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="12" t="n">
+      <c r="A4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="13" t="n">
         <f aca="false">AVERAGE(D4,F4,H4,J4,L4,N4)</f>
         <v>0.479783624027799</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="14" t="n">
         <v>0.369274416448439</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="15" t="n">
         <f aca="false">4/$D$3</f>
         <v>0.0043956043956044</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="14" t="n">
         <v>0.52</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="14" t="n">
         <v>0.349514563106796</v>
       </c>
-      <c r="I4" s="14" t="n">
+      <c r="I4" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="14" t="n">
         <v>0.44017094017094</v>
       </c>
-      <c r="K4" s="14" t="n">
+      <c r="K4" s="15" t="n">
         <f aca="false">9/$J$3</f>
         <v>0.037037037037037</v>
       </c>
-      <c r="L4" s="13" t="n">
+      <c r="L4" s="14" t="n">
         <v>0.649741824440619</v>
       </c>
-      <c r="M4" s="14" t="n">
+      <c r="M4" s="15" t="n">
         <f aca="false">3/$L$3</f>
         <v>0.00257510729613734</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N4" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O4" s="14" t="n">
+      <c r="O4" s="15" t="n">
         <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="15" t="n">
+        <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
         <v>0.477597373948204</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="14" t="n">
         <v>0.38169947346544</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="14" t="n">
         <v>0.472972972972973</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">26/$F$3</f>
         <v>0.26</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H5" s="14" t="n">
         <v>0.349514563106796</v>
       </c>
-      <c r="I5" s="14" t="n">
+      <c r="I5" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K5" s="14" t="n">
+      <c r="K5" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L5" s="13" t="n">
+      <c r="L5" s="14" t="n">
         <v>0.666952789699571</v>
       </c>
-      <c r="M5" s="14" t="n">
+      <c r="M5" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N5" s="13" t="n">
+      <c r="N5" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O5" s="14" t="n">
+      <c r="O5" s="15" t="n">
         <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="22" t="n">
+        <v>0.136446672153424</v>
+      </c>
+      <c r="Q5" s="14" t="n">
+        <v>1.06958782892184</v>
+      </c>
+      <c r="R5" s="21" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="S5" s="15" t="n">
+        <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
         <v>0.456362837616999</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="14" t="n">
         <v>0.304699117807113</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="14" t="n">
         <v>0.466666666666667</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G6" s="15" t="n">
         <f aca="false">25/$F$3</f>
         <v>0.25</v>
       </c>
-      <c r="H6" s="13" t="n">
+      <c r="H6" s="14" t="n">
         <v>0.349514563106796</v>
       </c>
-      <c r="I6" s="14" t="n">
+      <c r="I6" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J6" s="13" t="n">
+      <c r="J6" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K6" s="14" t="n">
+      <c r="K6" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L6" s="13" t="n">
+      <c r="L6" s="14" t="n">
         <v>0.622852233676976</v>
       </c>
-      <c r="M6" s="14" t="n">
+      <c r="M6" s="15" t="n">
         <f aca="false">1/$L$3</f>
         <v>0.000858369098712446</v>
       </c>
-      <c r="N6" s="13" t="n">
+      <c r="N6" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O6" s="14" t="n">
+      <c r="O6" s="15" t="n">
         <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="22" t="n">
+        <v>0.0704660506880692</v>
+      </c>
+      <c r="Q6" s="14" t="n">
+        <v>1.10242179616549</v>
+      </c>
+      <c r="R6" s="21" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="S6" s="15" t="n">
+        <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="13" t="n">
         <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
         <v>0.45195286292649</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="14" t="n">
         <v>0.193271177494123</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>0.47</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G7" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <v>0.359223300970874</v>
       </c>
-      <c r="I7" s="14" t="n">
+      <c r="I7" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J7" s="13" t="n">
+      <c r="J7" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K7" s="14" t="n">
+      <c r="K7" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L7" s="13" t="n">
+      <c r="L7" s="14" t="n">
         <v>0.678111587982833</v>
       </c>
-      <c r="M7" s="14" t="n">
+      <c r="M7" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N7" s="13" t="n">
+      <c r="N7" s="14" t="n">
         <v>0.566666666666667</v>
       </c>
-      <c r="O7" s="14" t="n">
+      <c r="O7" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P7" s="23" t="n">
+        <v>0.126175582563965</v>
+      </c>
+      <c r="Q7" s="24" t="n">
+        <v>1.05372360133383</v>
+      </c>
+      <c r="R7" s="21" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="S7" s="25" t="n">
+        <f aca="false">1818/$P$3</f>
+        <v>0.909</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
         <v>0.449693612435578</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="14" t="n">
         <v>0.204119502057382</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>0.46</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G8" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H8" s="13" t="n">
+      <c r="H8" s="14" t="n">
         <v>0.368932038834951</v>
       </c>
-      <c r="I8" s="14" t="n">
+      <c r="I8" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="J8" s="14" t="n">
         <v>0.442148760330579</v>
       </c>
-      <c r="K8" s="14" t="n">
+      <c r="K8" s="15" t="n">
         <f aca="false">1/$J$3</f>
         <v>0.00411522633744856</v>
       </c>
-      <c r="L8" s="13" t="n">
+      <c r="L8" s="14" t="n">
         <v>0.672961373390558</v>
       </c>
-      <c r="M8" s="14" t="n">
+      <c r="M8" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N8" s="13" t="n">
+      <c r="N8" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O8" s="14" t="n">
+      <c r="O8" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P8" s="23" t="n">
+        <v>0.101979532543943</v>
+      </c>
+      <c r="Q8" s="24" t="n">
+        <v>0.984716530054645</v>
+      </c>
+      <c r="R8" s="21" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="S8" s="25" t="n">
+        <f aca="false">1138/$P$3</f>
+        <v>0.569</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="13" t="n">
         <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
         <v>0.446939595430147</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="14" t="n">
         <v>0.214844642079834</v>
       </c>
-      <c r="E9" s="14" t="n">
+      <c r="E9" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="n">
+      <c r="F9" s="14" t="n">
         <v>0.47</v>
       </c>
-      <c r="G9" s="14" t="n">
+      <c r="G9" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H9" s="13" t="n">
+      <c r="H9" s="14" t="n">
         <v>0.310679611650485</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J9" s="13" t="n">
+      <c r="J9" s="14" t="n">
         <v>0.448559670781893</v>
       </c>
-      <c r="K9" s="14" t="n">
+      <c r="K9" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L9" s="13" t="n">
+      <c r="L9" s="14" t="n">
         <v>0.68755364806867</v>
       </c>
-      <c r="M9" s="14" t="n">
+      <c r="M9" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N9" s="13" t="n">
+      <c r="N9" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O9" s="14" t="n">
+      <c r="O9" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P9" s="22" t="n">
+        <v>0.0869997613324107</v>
+      </c>
+      <c r="Q9" s="14" t="n">
+        <v>1.1923877607133</v>
+      </c>
+      <c r="R9" s="21" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="S9" s="15" t="n">
+        <f aca="false">28/$P$3</f>
+        <v>0.014</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="13" t="n">
         <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
         <v>0.439307324929851</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="14" t="n">
         <v>0.127338801833183</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E10" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="G10" s="14" t="n">
+      <c r="G10" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H10" s="13" t="n">
+      <c r="H10" s="14" t="n">
         <v>0.388349514563107</v>
       </c>
-      <c r="I10" s="14" t="n">
+      <c r="I10" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J10" s="13" t="n">
+      <c r="J10" s="14" t="n">
         <v>0.442148760330579</v>
       </c>
-      <c r="K10" s="14" t="n">
+      <c r="K10" s="15" t="n">
         <f aca="false">1/$J$3</f>
         <v>0.00411522633744856</v>
       </c>
-      <c r="L10" s="13" t="n">
+      <c r="L10" s="14" t="n">
         <v>0.628006872852234</v>
       </c>
-      <c r="M10" s="14" t="n">
+      <c r="M10" s="15" t="n">
         <f aca="false">1/$L$3</f>
         <v>0.000858369098712446</v>
       </c>
-      <c r="N10" s="13" t="n">
+      <c r="N10" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O10" s="14" t="n">
+      <c r="O10" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P10" s="23" t="n">
+        <v>0.0462020736542011</v>
+      </c>
+      <c r="Q10" s="24" t="n">
+        <v>1.07801109103371</v>
+      </c>
+      <c r="R10" s="21" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="S10" s="25" t="n">
+        <f aca="false">776/$P$3</f>
+        <v>0.388</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="13" t="n">
         <f aca="false">AVERAGE(D11,F11,H11,J11,L11,N11)</f>
         <v>0.436042704459863</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>0.0518271447518188</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F11" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="G11" s="14" t="n">
+      <c r="G11" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <v>0.398058252427184</v>
       </c>
-      <c r="I11" s="14" t="n">
+      <c r="I11" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J11" s="13" t="n">
+      <c r="J11" s="14" t="n">
         <v>0.448559670781893</v>
       </c>
-      <c r="K11" s="14" t="n">
+      <c r="K11" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L11" s="13" t="n">
+      <c r="L11" s="14" t="n">
         <v>0.667811158798283</v>
       </c>
-      <c r="M11" s="14" t="n">
+      <c r="M11" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N11" s="13" t="n">
+      <c r="N11" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O11" s="14" t="n">
+      <c r="O11" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P11" s="23" t="n">
+        <v>0.0816039377198555</v>
+      </c>
+      <c r="Q11" s="24" t="n">
+        <v>1.02776848444296</v>
+      </c>
+      <c r="R11" s="21" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="S11" s="25" t="n">
+        <f aca="false">1758/$P$3</f>
+        <v>0.879</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="12" t="n">
+      <c r="C12" s="13" t="n">
         <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
         <v>0.432443158810545</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="14" t="n">
         <v>0.0718486458091463</v>
       </c>
-      <c r="E12" s="14" t="n">
+      <c r="E12" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F12" s="14" t="n">
         <v>0.52</v>
       </c>
-      <c r="G12" s="14" t="n">
+      <c r="G12" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H12" s="13" t="n">
+      <c r="H12" s="14" t="n">
         <v>0.378640776699029</v>
       </c>
-      <c r="I12" s="14" t="n">
+      <c r="I12" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J12" s="13" t="n">
+      <c r="J12" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K12" s="14" t="n">
+      <c r="K12" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L12" s="13" t="n">
+      <c r="L12" s="14" t="n">
         <v>0.629725085910653</v>
       </c>
-      <c r="M12" s="14" t="n">
+      <c r="M12" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N12" s="13" t="n">
+      <c r="N12" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O12" s="14" t="n">
+      <c r="O12" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P12" s="22" t="n">
+        <v>0.0497002425066837</v>
+      </c>
+      <c r="Q12" s="14" t="n">
+        <v>1.29332825735224</v>
+      </c>
+      <c r="R12" s="21" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="S12" s="15" t="n">
+        <f aca="false">1339/$P$3</f>
+        <v>0.6695</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="13" t="n">
         <f aca="false">AVERAGE(D13,F13,H13,J13,L13,N13)</f>
         <v>0.426274378090213</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="14" t="n">
         <v>0.0702149056307087</v>
       </c>
-      <c r="E13" s="14" t="n">
+      <c r="E13" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F13" s="13" t="n">
+      <c r="F13" s="14" t="n">
         <v>0.49</v>
       </c>
-      <c r="G13" s="14" t="n">
+      <c r="G13" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H13" s="13" t="n">
+      <c r="H13" s="14" t="n">
         <v>0.396039603960396</v>
       </c>
-      <c r="I13" s="14" t="n">
+      <c r="I13" s="15" t="n">
         <f aca="false">2/$H$3</f>
         <v>0.0194174757281553</v>
       </c>
-      <c r="J13" s="13" t="n">
+      <c r="J13" s="14" t="n">
         <v>0.460905349794239</v>
       </c>
-      <c r="K13" s="14" t="n">
+      <c r="K13" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L13" s="13" t="n">
+      <c r="L13" s="14" t="n">
         <v>0.67381974248927</v>
       </c>
-      <c r="M13" s="14" t="n">
+      <c r="M13" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N13" s="13" t="n">
+      <c r="N13" s="14" t="n">
         <v>0.466666666666667</v>
       </c>
-      <c r="O13" s="14" t="n">
+      <c r="O13" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P13" s="23" t="n">
+        <v>0.113227204219314</v>
+      </c>
+      <c r="Q13" s="24" t="n">
+        <v>1.02468032181585</v>
+      </c>
+      <c r="R13" s="21" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="S13" s="15" t="n">
+        <f aca="false">3/$P$3</f>
+        <v>0.0015</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="13" t="n">
         <f aca="false">AVERAGE(D14,F14,H14,J14,L14,N14)</f>
         <v>0.419278530088385</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="14" t="n">
         <v>-0.0155335936055105</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F14" s="13" t="n">
+      <c r="F14" s="14" t="n">
         <v>0.48</v>
       </c>
-      <c r="G14" s="14" t="n">
+      <c r="G14" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H14" s="13" t="n">
+      <c r="H14" s="14" t="n">
         <v>0.368932038834951</v>
       </c>
-      <c r="I14" s="14" t="n">
+      <c r="I14" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J14" s="13" t="n">
+      <c r="J14" s="14" t="n">
         <v>0.489711934156379</v>
       </c>
-      <c r="K14" s="14" t="n">
+      <c r="K14" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L14" s="13" t="n">
+      <c r="L14" s="14" t="n">
         <v>0.659227467811159</v>
       </c>
-      <c r="M14" s="14" t="n">
+      <c r="M14" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N14" s="13" t="n">
+      <c r="N14" s="14" t="n">
         <v>0.533333333333333</v>
       </c>
-      <c r="O14" s="14" t="n">
+      <c r="O14" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P14" s="23" t="n">
+        <v>0.0534217525346316</v>
+      </c>
+      <c r="Q14" s="24" t="n">
+        <v>1.26345272449499</v>
+      </c>
+      <c r="R14" s="21" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="S14" s="25" t="n">
+        <f aca="false">213/$P$3</f>
+        <v>0.1065</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="12" t="n">
+      <c r="C15" s="13" t="n">
         <f aca="false">AVERAGE(D15,F15,H15,J15,L15,N15)</f>
-        <v>0.416323225087403</v>
-      </c>
-      <c r="D15" s="17" t="n">
+        <v>0.416323225087402</v>
+      </c>
+      <c r="D15" s="14" t="n">
         <v>0.00078604321068414</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="14" t="n">
         <v>0.49</v>
       </c>
-      <c r="G15" s="14" t="n">
+      <c r="G15" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="14" t="n">
         <v>0.368932038834951</v>
       </c>
-      <c r="I15" s="14" t="n">
+      <c r="I15" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J15" s="13" t="n">
+      <c r="J15" s="14" t="n">
         <v>0.444444444444444</v>
       </c>
-      <c r="K15" s="14" t="n">
+      <c r="K15" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L15" s="13" t="n">
+      <c r="L15" s="14" t="n">
         <v>0.643776824034335</v>
       </c>
-      <c r="M15" s="14" t="n">
+      <c r="M15" s="15" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N15" s="13" t="n">
+      <c r="N15" s="14" t="n">
         <v>0.55</v>
       </c>
-      <c r="O15" s="14" t="n">
+      <c r="O15" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
+      </c>
+      <c r="P15" s="23" t="n">
+        <v>0.0844210902399286</v>
+      </c>
+      <c r="Q15" s="24" t="n">
+        <v>1.04035874439462</v>
+      </c>
+      <c r="R15" s="21" t="n">
+        <v>0.121</v>
+      </c>
+      <c r="S15" s="25" t="n">
+        <f aca="false">1964/$P$3</f>
+        <v>0.982</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="12" t="n">
+      <c r="C16" s="13" t="n">
         <f aca="false">AVERAGE(D16,F16,H16,J16,L16,N16)</f>
         <v>0.405257833604129</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="14" t="n">
         <v>-0.0714529452409867</v>
       </c>
-      <c r="E16" s="14" t="n">
+      <c r="E16" s="15" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="n">
+      <c r="F16" s="14" t="n">
         <v>0.52</v>
       </c>
-      <c r="G16" s="14" t="n">
+      <c r="G16" s="15" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H16" s="13" t="n">
+      <c r="H16" s="14" t="n">
         <v>0.378640776699029</v>
       </c>
-      <c r="I16" s="14" t="n">
+      <c r="I16" s="15" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J16" s="13" t="n">
+      <c r="J16" s="14" t="n">
         <v>0.469135802469136</v>
       </c>
-      <c r="K16" s="14" t="n">
+      <c r="K16" s="15" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L16" s="13" t="n">
+      <c r="L16" s="14" t="n">
         <v>0.618556701030928</v>
       </c>
-      <c r="M16" s="14" t="n">
+      <c r="M16" s="15" t="n">
         <f aca="false">1/$L$3</f>
         <v>0.000858369098712446</v>
       </c>
-      <c r="N16" s="13" t="n">
+      <c r="N16" s="14" t="n">
         <v>0.516666666666667</v>
       </c>
-      <c r="O16" s="14" t="n">
+      <c r="O16" s="15" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
+      <c r="P16" s="23" t="n">
+        <v>0.018613476307488</v>
+      </c>
+      <c r="Q16" s="24" t="n">
+        <v>1.12997748971513</v>
+      </c>
+      <c r="R16" s="21" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="S16" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="12" t="n">
+    <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="13" t="n">
         <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
         <v>0.364587789621774</v>
       </c>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="14" t="n">
         <v>0.0266825503923221</v>
       </c>
-      <c r="E17" s="14" t="n">
+      <c r="E17" s="15" t="n">
         <f aca="false">187/$D$3</f>
         <v>0.205494505494505</v>
       </c>
-      <c r="F17" s="13" t="n">
+      <c r="F17" s="14" t="n">
         <v>0.461538461538462</v>
       </c>
-      <c r="G17" s="14" t="n">
+      <c r="G17" s="15" t="n">
         <f aca="false">9/$F$3</f>
         <v>0.09</v>
       </c>
-      <c r="H17" s="13" t="n">
+      <c r="H17" s="14" t="n">
         <v>0.237113402061856</v>
       </c>
-      <c r="I17" s="14" t="n">
+      <c r="I17" s="15" t="n">
         <f aca="false">6/$H$3</f>
         <v>0.058252427184466</v>
       </c>
-      <c r="J17" s="13" t="n">
+      <c r="J17" s="14" t="n">
         <v>0.558823529411765</v>
       </c>
-      <c r="K17" s="14" t="n">
+      <c r="K17" s="15" t="n">
         <f aca="false">39/$J$3</f>
         <v>0.160493827160494</v>
       </c>
-      <c r="L17" s="13" t="n">
+      <c r="L17" s="14" t="n">
         <v>0.403368794326241</v>
       </c>
-      <c r="M17" s="14" t="n">
+      <c r="M17" s="15" t="n">
         <f aca="false">37/$L$3</f>
         <v>0.0317596566523605</v>
       </c>
-      <c r="N17" s="13" t="n">
+      <c r="N17" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="O17" s="14" t="n">
+      <c r="O17" s="15" t="n">
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="15" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
+    <row r="18" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:O47">
-    <sortState ref="A4:O47">
-      <sortCondition ref="C4:C47" descending="1" customList=""/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="7">
+  <autoFilter ref="A3:S47"/>
+  <mergeCells count="9">
     <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:S1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+  <conditionalFormatting sqref="E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28 S4:S17">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3930,6 +4285,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P17">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R27">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF77BC65"/>
+        <color rgb="FFFF6D6D"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId2" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
     <hyperlink ref="B6" r:id="rId3" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>

</xml_diff>

<commit_message>
Add Solar eval data
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar-10.7b-instruct-v1.0.Q6_K.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF</t>
   </si>
   <si>
     <t xml:space="preserve">Phi-3-mini-4k-instruct-q4.gguf</t>
@@ -540,7 +546,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,7 +631,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,10 +651,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -662,7 +664,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="137">
+  <dxfs count="143">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -689,6 +691,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF84B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF87B366"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -889,6 +899,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC68E6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFCC8A6A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1057,14 +1075,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF84B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF78BB66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1105,6 +1115,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFCA8C6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFD2876B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1209,7 +1227,95 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF8BB067"/>
+          <fgColor rgb="FF85B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3A268"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCE896B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDA826B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE17E6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27D6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE47C6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEC786C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99A867"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1225,70 +1331,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFA6A168"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA796C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEB786C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2746D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4736D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6726D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF79BB66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99A867"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFAB9D69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1313,14 +1355,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF85B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF8CAF67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1330,6 +1364,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFC98C6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7BBA66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1430,6 +1472,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF9AA868"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFAD9D69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1486,31 +1536,47 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE17E6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97A6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF0756D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFC6F6D"/>
+          <fgColor rgb="FFEA796C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1756D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6726D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8716D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB6F6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFE6D6D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1526,7 +1592,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDA826B"/>
+          <fgColor rgb="FFA6A168"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1550,22 +1616,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF1756D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFB6F6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFD6E6D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1606,6 +1656,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFBC936A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFBD936A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1615,14 +1673,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCA8B6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCE896B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1951,10 +2001,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2060,7 +2110,7 @@
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -2797,80 +2847,80 @@
       <c r="A12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
-        <v>0.658513623474907</v>
-      </c>
-      <c r="D12" s="15" t="n">
-        <v>0.523854029130735</v>
+        <v>0.699391112337297</v>
+      </c>
+      <c r="D12" s="18" t="n">
+        <v>0.625980868840778</v>
       </c>
       <c r="E12" s="16" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
-      </c>
-      <c r="F12" s="15" t="n">
-        <v>0.480334216425515</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
+      </c>
+      <c r="F12" s="18" t="n">
+        <v>0.37493632195619</v>
       </c>
       <c r="G12" s="16" t="n">
-        <f aca="false">1/$F$3</f>
-        <v>0.000101884870096791</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H12" s="15" t="n">
-        <v>0.727941176470588</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I12" s="15" t="n">
-        <v>0.821829855537721</v>
+        <v>0.86522462562396</v>
       </c>
       <c r="J12" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K12" s="15" t="n">
-        <v>0.696448187477115</v>
+      <c r="K12" s="18" t="n">
+        <v>0.438496791934006</v>
       </c>
       <c r="L12" s="16" t="n">
-        <f aca="false">1/$K$3</f>
-        <v>0.000183049606443346</v>
-      </c>
-      <c r="M12" s="15" t="n">
-        <v>0.509271935283136</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
+      </c>
+      <c r="M12" s="18" t="n">
+        <v>0.852128527963984</v>
       </c>
       <c r="N12" s="15" t="n">
-        <v>0.593278732490252</v>
+        <v>0.805846053913608</v>
       </c>
       <c r="O12" s="16" t="n">
-        <f aca="false">255/$M$3</f>
-        <v>0.0063071976255256</v>
+        <f aca="false">3/$M$3</f>
+        <v>7.42023250061835E-005</v>
       </c>
       <c r="P12" s="15" t="n">
-        <v>0.249097472924188</v>
+        <v>0.133574007220217</v>
       </c>
       <c r="Q12" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R12" s="15" t="n">
-        <v>0.934633027522936</v>
+        <v>0.930045871559633</v>
       </c>
       <c r="S12" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T12" s="15" t="n">
-        <v>0.821663265900952</v>
+      <c r="T12" s="18" t="n">
+        <v>0.886137481283129</v>
       </c>
       <c r="U12" s="15" t="n">
-        <v>0.825501723380821</v>
+        <v>0.890119815150565</v>
       </c>
       <c r="V12" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W12" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.788732394366197</v>
       </c>
       <c r="X12" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2886,68 +2936,68 @@
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(W13,T13:U13,R13,P13,N13,M13,K13,H13,I13,F13,D13)</f>
-        <v>0.653779197430066</v>
+        <v>0.658513623474907</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.455627237079107</v>
+        <v>0.523854029130735</v>
       </c>
       <c r="E13" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.386958736627611</v>
+        <v>0.480334216425515</v>
       </c>
       <c r="G13" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">1/$F$3</f>
+        <v>0.000101884870096791</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.754901960784314</v>
+        <v>0.727941176470588</v>
       </c>
       <c r="I13" s="15" t="n">
-        <v>0.835526315789474</v>
+        <v>0.821829855537721</v>
       </c>
       <c r="J13" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K13" s="15" t="n">
-        <v>0.136371956800293</v>
+        <v>0.696448187477115</v>
       </c>
       <c r="L13" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">1/$K$3</f>
+        <v>0.000183049606443346</v>
       </c>
       <c r="M13" s="15" t="n">
-        <v>0.82352213702696</v>
+        <v>0.509271935283136</v>
       </c>
       <c r="N13" s="15" t="n">
-        <v>0.77733046219143</v>
+        <v>0.593278732490252</v>
       </c>
       <c r="O13" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
+        <f aca="false">255/$M$3</f>
+        <v>0.0063071976255256</v>
       </c>
       <c r="P13" s="15" t="n">
-        <v>0.353790613718412</v>
+        <v>0.249097472924188</v>
       </c>
       <c r="Q13" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R13" s="15" t="n">
-        <v>0.935779816513762</v>
+        <v>0.934633027522936</v>
       </c>
       <c r="S13" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T13" s="15" t="n">
-        <v>0.826388381403035</v>
+        <v>0.821663265900952</v>
       </c>
       <c r="U13" s="15" t="n">
-        <v>0.840842892071465</v>
+        <v>0.825501723380821</v>
       </c>
       <c r="V13" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -2965,80 +3015,80 @@
       <c r="A14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(W14,T14:U14,R14,P14,N14,M14,K14,H14,I14,F14,D14)</f>
-        <v>0.64108637065082</v>
-      </c>
-      <c r="D14" s="18" t="n">
-        <v>0.531920773750409</v>
+        <v>0.653779197430066</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.455627237079107</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
-      <c r="F14" s="18" t="n">
-        <v>0.42985226693836</v>
+      <c r="F14" s="15" t="n">
+        <v>0.386958736627611</v>
       </c>
       <c r="G14" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.705882352941177</v>
+        <v>0.754901960784314</v>
       </c>
       <c r="I14" s="15" t="n">
-        <v>0.82089552238806</v>
+        <v>0.835526315789474</v>
       </c>
       <c r="J14" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K14" s="18" t="n">
-        <v>0.540377220289324</v>
+      <c r="K14" s="15" t="n">
+        <v>0.136371956800293</v>
       </c>
       <c r="L14" s="16" t="n">
-        <f aca="false">2/$K$3</f>
-        <v>0.000366099212886692</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M14" s="15" t="n">
-        <v>0.80123670541677</v>
+        <v>0.82352213702696</v>
       </c>
       <c r="N14" s="15" t="n">
-        <v>0.772955868226253</v>
+        <v>0.77733046219143</v>
       </c>
       <c r="O14" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
-      <c r="P14" s="18" t="n">
-        <v>0.296028880866426</v>
+      <c r="P14" s="15" t="n">
+        <v>0.353790613718412</v>
       </c>
       <c r="Q14" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R14" s="15" t="n">
-        <v>0.928899082568807</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S14" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T14" s="15" t="n">
-        <v>0.621129369842947</v>
+        <v>0.826388381403035</v>
       </c>
       <c r="U14" s="15" t="n">
-        <v>0.666393615848911</v>
+        <v>0.840842892071465</v>
       </c>
       <c r="V14" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W14" s="15" t="n">
-        <v>0.577464788732394</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X14" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3054,68 +3104,68 @@
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(W15,T15:U15,R15,P15,N15,M15,K15,H15,I15,F15,D15)</f>
-        <v>0.613554278796799</v>
+        <v>0.64108637065082</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>0.375051720670997</v>
+        <v>0.531920773750409</v>
       </c>
       <c r="E15" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.538767193071829</v>
+        <v>0.42985226693836</v>
       </c>
       <c r="G15" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.730392156862745</v>
+        <v>0.705882352941177</v>
       </c>
       <c r="I15" s="15" t="n">
-        <v>0.827044025157233</v>
+        <v>0.82089552238806</v>
       </c>
       <c r="J15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K15" s="15" t="n">
-        <v>0.557386051619989</v>
+        <v>0.540377220289324</v>
       </c>
       <c r="L15" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">2/$K$3</f>
+        <v>0.000366099212886692</v>
       </c>
       <c r="M15" s="15" t="n">
-        <v>0.608706406134059</v>
+        <v>0.80123670541677</v>
       </c>
       <c r="N15" s="15" t="n">
-        <v>0.625189537528431</v>
+        <v>0.772955868226253</v>
       </c>
       <c r="O15" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P15" s="15" t="n">
-        <v>0.425992779783394</v>
+        <v>0.296028880866426</v>
       </c>
       <c r="Q15" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R15" s="15" t="n">
-        <v>0.932339449541284</v>
+        <v>0.928899082568807</v>
       </c>
       <c r="S15" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T15" s="15" t="n">
-        <v>0.573663619974553</v>
+        <v>0.621129369842947</v>
       </c>
       <c r="U15" s="15" t="n">
-        <v>0.590653616484677</v>
+        <v>0.666393615848911</v>
       </c>
       <c r="V15" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3133,80 +3183,80 @@
       <c r="A16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(W16,T16:U16,R16,P16,N16,M16,K16,H16,I16,F16,D16)</f>
-        <v>0.588337454921144</v>
-      </c>
-      <c r="D16" s="18" t="n">
-        <v>0.275218494690191</v>
+        <v>0.613554278796799</v>
+      </c>
+      <c r="D16" s="15" t="n">
+        <v>0.375051720670997</v>
       </c>
       <c r="E16" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
-      </c>
-      <c r="F16" s="18" t="n">
-        <v>0.256342333163525</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="15" t="n">
+        <v>0.538767193071829</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H16" s="18" t="n">
-        <v>0.718137254901961</v>
+      <c r="H16" s="15" t="n">
+        <v>0.730392156862745</v>
       </c>
       <c r="I16" s="15" t="n">
-        <v>0.822804314329738</v>
+        <v>0.827044025157233</v>
       </c>
       <c r="J16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K16" s="18" t="n">
-        <v>0.33260113490756</v>
+      <c r="K16" s="15" t="n">
+        <v>0.557386051619989</v>
       </c>
       <c r="L16" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M16" s="15" t="n">
-        <v>0.730112793113684</v>
+        <v>0.608706406134059</v>
       </c>
       <c r="N16" s="15" t="n">
-        <v>0.707110836711137</v>
+        <v>0.625189537528431</v>
       </c>
       <c r="O16" s="16" t="n">
-        <f aca="false">2/$M$3</f>
-        <v>4.9468216670789E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P16" s="15" t="n">
-        <v>0.339350180505415</v>
+        <v>0.425992779783394</v>
       </c>
       <c r="Q16" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R16" s="15" t="n">
-        <v>0.918577981651376</v>
+        <v>0.932339449541284</v>
       </c>
       <c r="S16" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T16" s="15" t="n">
-        <v>0.730177716008711</v>
+        <v>0.573663619974553</v>
       </c>
       <c r="U16" s="15" t="n">
-        <v>0.750743179633811</v>
+        <v>0.590653616484677</v>
       </c>
       <c r="V16" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W16" s="15" t="n">
-        <v>0.47887323943662</v>
+        <v>0.577464788732394</v>
       </c>
       <c r="X16" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3222,68 +3272,68 @@
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(W17,T17:U17,R17,P17,N17,M17,K17,H17,I17,F17,D17)</f>
-        <v>0.499454443668613</v>
+        <v>0.588337454921144</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.333471865271531</v>
+        <v>0.275218494690191</v>
       </c>
       <c r="E17" s="16" t="n">
-        <f aca="false">6/$D$3</f>
-        <v>0.00575263662511985</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F17" s="15" t="n">
-        <v>0.292103922567499</v>
+        <v>0.256342333163525</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.698529411764706</v>
+        <v>0.718137254901961</v>
       </c>
       <c r="I17" s="15" t="n">
-        <v>0.805687203791469</v>
+        <v>0.822804314329738</v>
       </c>
       <c r="J17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K17" s="15" t="n">
-        <v>0.391434449223864</v>
+        <v>0.33260113490756</v>
       </c>
       <c r="L17" s="16" t="n">
-        <f aca="false">116/$K$3</f>
-        <v>0.0212337543474282</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M17" s="15" t="n">
-        <v>0.691602220900258</v>
+        <v>0.730112793113684</v>
       </c>
       <c r="N17" s="15" t="n">
-        <v>0.36669042044182</v>
+        <v>0.707110836711137</v>
       </c>
       <c r="O17" s="16" t="n">
-        <f aca="false">86/$M$3</f>
-        <v>0.00212713331684393</v>
+        <f aca="false">2/$M$3</f>
+        <v>4.9468216670789E-005</v>
       </c>
       <c r="P17" s="15" t="n">
-        <v>0.306859205776173</v>
+        <v>0.339350180505415</v>
       </c>
       <c r="Q17" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R17" s="15" t="n">
-        <v>0.855504587155963</v>
+        <v>0.918577981651376</v>
       </c>
       <c r="S17" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T17" s="15" t="n">
-        <v>0.370306926073738</v>
+        <v>0.730177716008711</v>
       </c>
       <c r="U17" s="15" t="n">
-        <v>0.402389871619712</v>
+        <v>0.750743179633811</v>
       </c>
       <c r="V17" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3301,82 +3351,166 @@
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(W18,T18:U18,R18,P18,N18,M18,K18,H18,I18,F18,D18)</f>
+        <v>0.499454443668613</v>
+      </c>
+      <c r="D18" s="15" t="n">
+        <v>0.333471865271531</v>
+      </c>
+      <c r="E18" s="16" t="n">
+        <f aca="false">6/$D$3</f>
+        <v>0.00575263662511985</v>
+      </c>
+      <c r="F18" s="15" t="n">
+        <v>0.292103922567499</v>
+      </c>
+      <c r="G18" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="15" t="n">
+        <v>0.698529411764706</v>
+      </c>
+      <c r="I18" s="15" t="n">
+        <v>0.805687203791469</v>
+      </c>
+      <c r="J18" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="15" t="n">
+        <v>0.391434449223864</v>
+      </c>
+      <c r="L18" s="16" t="n">
+        <f aca="false">116/$K$3</f>
+        <v>0.0212337543474282</v>
+      </c>
+      <c r="M18" s="15" t="n">
+        <v>0.691602220900258</v>
+      </c>
+      <c r="N18" s="15" t="n">
+        <v>0.36669042044182</v>
+      </c>
+      <c r="O18" s="16" t="n">
+        <f aca="false">86/$M$3</f>
+        <v>0.00212713331684393</v>
+      </c>
+      <c r="P18" s="15" t="n">
+        <v>0.306859205776173</v>
+      </c>
+      <c r="Q18" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="15" t="n">
+        <v>0.855504587155963</v>
+      </c>
+      <c r="S18" s="16" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="15" t="n">
+        <v>0.370306926073738</v>
+      </c>
+      <c r="U18" s="15" t="n">
+        <v>0.402389871619712</v>
+      </c>
+      <c r="V18" s="16" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="15" t="n">
+        <v>0.47887323943662</v>
+      </c>
+      <c r="X18" s="16" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="14" t="n">
+        <f aca="false">AVERAGE(W19,T19:U19,R19,P19,N19,M19,K19,H19,I19,F19,D19)</f>
         <v>0.338674923063942</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D19" s="15" t="n">
         <v>0.241606739317903</v>
       </c>
-      <c r="E18" s="16" t="n">
+      <c r="E19" s="16" t="n">
         <f aca="false">7/$D$3</f>
         <v>0.00671140939597315</v>
       </c>
-      <c r="F18" s="15" t="n">
+      <c r="F19" s="15" t="n">
         <v>0.285161027313494</v>
       </c>
-      <c r="G18" s="16" t="n">
+      <c r="G19" s="16" t="n">
         <f aca="false">3/$F$3</f>
         <v>0.000305654610290372</v>
       </c>
-      <c r="H18" s="15" t="n">
+      <c r="H19" s="15" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="I18" s="15" t="n">
+      <c r="I19" s="15" t="n">
         <v>0.0620689655172414</v>
       </c>
-      <c r="J18" s="16" t="n">
+      <c r="J19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K18" s="18" t="n">
+      <c r="K19" s="15" t="n">
         <v>0.32644239804548</v>
       </c>
-      <c r="L18" s="16" t="n">
+      <c r="L19" s="16" t="n">
         <f aca="false">142/$K$3</f>
         <v>0.0259930441149552</v>
       </c>
-      <c r="M18" s="15" t="n">
+      <c r="M19" s="15" t="n">
         <v>0.459092373658512</v>
       </c>
-      <c r="N18" s="15" t="n">
+      <c r="N19" s="15" t="n">
         <v>0.524490151647202</v>
       </c>
-      <c r="O18" s="16" t="n">
+      <c r="O19" s="16" t="n">
         <f aca="false">83/$M$3</f>
         <v>0.00205293099183774</v>
       </c>
-      <c r="P18" s="18" t="n">
+      <c r="P19" s="15" t="n">
         <v>0.357400722021661</v>
       </c>
-      <c r="Q18" s="16" t="n">
+      <c r="Q19" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R18" s="15" t="n">
+      <c r="R19" s="15" t="n">
         <v>0.894374282433984</v>
       </c>
-      <c r="S18" s="16" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">1/$R$3</f>
         <v>0.00114678899082569</v>
       </c>
-      <c r="T18" s="15" t="n">
+      <c r="T19" s="15" t="n">
         <v>0.0103797859681123</v>
       </c>
-      <c r="U18" s="15" t="n">
+      <c r="U19" s="15" t="n">
         <v>0.119045072158263</v>
       </c>
-      <c r="V18" s="16" t="n">
+      <c r="V19" s="16" t="n">
         <f aca="false">10/$T$3</f>
         <v>0.00666666666666667</v>
       </c>
-      <c r="W18" s="15" t="n">
+      <c r="W19" s="15" t="n">
         <v>0.450704225352113</v>
       </c>
-      <c r="X18" s="16" t="n">
+      <c r="X19" s="16" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -3396,7 +3530,7 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3529,13 +3663,14 @@
     <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
     <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
     <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3544,8 +3679,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <drawing r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -3554,10 +3689,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3591,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3605,7 +3740,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="20"/>
       <c r="R1" s="20"/>
@@ -3618,31 +3753,31 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -3651,7 +3786,7 @@
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -3694,10 +3829,10 @@
         <v>2000</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>13</v>
@@ -3772,16 +3907,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C5" s="14" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
         <v>0.415289583163276</v>
       </c>
-      <c r="D5" s="18" t="n">
+      <c r="D5" s="15" t="n">
         <v>0.0619341592153086</v>
       </c>
       <c r="E5" s="16" t="n">
@@ -3802,14 +3937,14 @@
         <f aca="false">1/$H$3</f>
         <v>0.00970873786407767</v>
       </c>
-      <c r="J5" s="18" t="n">
+      <c r="J5" s="15" t="n">
         <v>0.510288065843621</v>
       </c>
       <c r="K5" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L5" s="18" t="n">
+      <c r="L5" s="15" t="n">
         <v>0.648927038626609</v>
       </c>
       <c r="M5" s="16" t="n">
@@ -3823,10 +3958,10 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="25" t="n">
+      <c r="P5" s="23" t="n">
         <v>0.130232557010572</v>
       </c>
-      <c r="Q5" s="18" t="n">
+      <c r="Q5" s="15" t="n">
         <v>1.02813785608942</v>
       </c>
       <c r="R5" s="24" t="n">
@@ -3839,10 +3974,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="14" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
@@ -3862,7 +3997,7 @@
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H6" s="18" t="n">
+      <c r="H6" s="15" t="n">
         <v>0.388349514563107</v>
       </c>
       <c r="I6" s="16" t="n">
@@ -3890,16 +4025,16 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="25" t="n">
+      <c r="P6" s="23" t="n">
         <v>0.115675852676348</v>
       </c>
-      <c r="Q6" s="18" t="n">
+      <c r="Q6" s="15" t="n">
         <v>1.05320394846913</v>
       </c>
       <c r="R6" s="24" t="n">
         <v>0.029</v>
       </c>
-      <c r="S6" s="26" t="n">
+      <c r="S6" s="16" t="n">
         <f aca="false">1622/$P$3</f>
         <v>0.811</v>
       </c>
@@ -3973,10 +4108,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
@@ -4091,16 +4226,16 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P9" s="25" t="n">
+      <c r="P9" s="23" t="n">
         <v>0.0946010077074703</v>
       </c>
-      <c r="Q9" s="18" t="n">
+      <c r="Q9" s="15" t="n">
         <v>0.950708101886604</v>
       </c>
       <c r="R9" s="24" t="n">
         <v>0.036</v>
       </c>
-      <c r="S9" s="26" t="n">
+      <c r="S9" s="16" t="n">
         <f aca="false">506/$P$3</f>
         <v>0.253</v>
       </c>
@@ -4241,112 +4376,112 @@
     </row>
     <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
-        <v>0.416323225087402</v>
-      </c>
-      <c r="D12" s="15" t="n">
-        <v>0.00078604321068414</v>
+        <v>0.478378567077423</v>
+      </c>
+      <c r="D12" s="18" t="n">
+        <v>0.267184035681135</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F12" s="15" t="n">
-        <v>0.49</v>
+      <c r="F12" s="18" t="n">
+        <v>0.653846153846154</v>
       </c>
       <c r="G12" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="15" t="n">
-        <v>0.368932038834951</v>
+        <f aca="false">74/$F$3</f>
+        <v>0.74</v>
+      </c>
+      <c r="H12" s="18" t="n">
+        <v>0.343137254901961</v>
       </c>
       <c r="I12" s="16" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="15" t="n">
+        <f aca="false">1/$H$3</f>
+        <v>0.00970873786407767</v>
+      </c>
+      <c r="J12" s="18" t="n">
         <v>0.444444444444444</v>
       </c>
       <c r="K12" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L12" s="15" t="n">
-        <v>0.643776824034335</v>
+      <c r="L12" s="18" t="n">
+        <v>0.628326180257511</v>
       </c>
       <c r="M12" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N12" s="15" t="n">
-        <v>0.55</v>
+      <c r="N12" s="18" t="n">
+        <v>0.533333333333333</v>
       </c>
       <c r="O12" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P12" s="25" t="n">
-        <v>0.0672142694158681</v>
+        <v>0.0672850889690679</v>
       </c>
       <c r="Q12" s="18" t="n">
-        <v>1.08084074373484</v>
+        <v>1.14115440228223</v>
       </c>
       <c r="R12" s="24" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="S12" s="26" t="n">
-        <f aca="false">1817/$P$3</f>
-        <v>0.9085</v>
+        <v>0.08</v>
+      </c>
+      <c r="S12" s="16" t="n">
+        <f aca="false">21/$P$3</f>
+        <v>0.0105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(D13,F13,H13,J13,L13,N13)</f>
-        <v>0.436042704459863</v>
+        <v>0.416323225087402</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.0518271447518188</v>
+        <v>0.00078604321068414</v>
       </c>
       <c r="E13" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="G13" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.398058252427184</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I13" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J13" s="15" t="n">
-        <v>0.448559670781893</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K13" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L13" s="15" t="n">
-        <v>0.667811158798283</v>
+        <v>0.643776824034335</v>
       </c>
       <c r="M13" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -4359,199 +4494,199 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P13" s="25" t="n">
-        <v>0.0666584744053729</v>
-      </c>
-      <c r="Q13" s="18" t="n">
-        <v>1.05036977813312</v>
+      <c r="P13" s="23" t="n">
+        <v>0.0672142694158681</v>
+      </c>
+      <c r="Q13" s="15" t="n">
+        <v>1.08084074373484</v>
       </c>
       <c r="R13" s="24" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="S13" s="26" t="n">
-        <f aca="false">1206/$P$3</f>
-        <v>0.603</v>
+        <v>0.068</v>
+      </c>
+      <c r="S13" s="16" t="n">
+        <f aca="false">1817/$P$3</f>
+        <v>0.9085</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(D14,F14,H14,J14,L14,N14)</f>
-        <v>0.419278530088385</v>
+        <v>0.436042704459863</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>-0.0155335936055105</v>
+        <v>0.0518271447518188</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F14" s="15" t="n">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.398058252427184</v>
       </c>
       <c r="I14" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J14" s="15" t="n">
-        <v>0.489711934156379</v>
+        <v>0.448559670781893</v>
       </c>
       <c r="K14" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L14" s="15" t="n">
-        <v>0.659227467811159</v>
+        <v>0.667811158798283</v>
       </c>
       <c r="M14" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N14" s="15" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O14" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P14" s="23" t="n">
-        <v>0.0534217525346316</v>
+        <v>0.0666584744053729</v>
       </c>
       <c r="Q14" s="15" t="n">
-        <v>1.26345272449499</v>
+        <v>1.05036977813312</v>
       </c>
       <c r="R14" s="24" t="n">
-        <v>0.041</v>
+        <v>0.061</v>
       </c>
       <c r="S14" s="16" t="n">
-        <f aca="false">213/$P$3</f>
-        <v>0.1065</v>
+        <f aca="false">1206/$P$3</f>
+        <v>0.603</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(D15,F15,H15,J15,L15,N15)</f>
-        <v>0.432443158810545</v>
+        <v>0.419278530088385</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>0.0718486458091463</v>
+        <v>-0.0155335936055105</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G15" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J15" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.489711934156379</v>
       </c>
       <c r="K15" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L15" s="15" t="n">
-        <v>0.629725085910653</v>
+        <v>0.659227467811159</v>
       </c>
       <c r="M15" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N15" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O15" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P15" s="23" t="n">
-        <v>0.0497002425066837</v>
+        <v>0.0534217525346316</v>
       </c>
       <c r="Q15" s="15" t="n">
-        <v>1.29332825735224</v>
+        <v>1.26345272449499</v>
       </c>
       <c r="R15" s="24" t="n">
-        <v>0.079</v>
+        <v>0.041</v>
       </c>
       <c r="S15" s="16" t="n">
-        <f aca="false">1339/$P$3</f>
-        <v>0.6695</v>
+        <f aca="false">213/$P$3</f>
+        <v>0.1065</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(D16,F16,H16,J16,L16,N16)</f>
-        <v>0.439307324929851</v>
+        <v>0.432443158810545</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>0.127338801833183</v>
+        <v>0.0718486458091463</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.388349514563107</v>
+        <v>0.378640776699029</v>
       </c>
       <c r="I16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J16" s="15" t="n">
-        <v>0.442148760330579</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K16" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L16" s="15" t="n">
-        <v>0.628006872852234</v>
+        <v>0.629725085910653</v>
       </c>
       <c r="M16" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N16" s="15" t="n">
         <v>0.55</v>
@@ -4561,32 +4696,32 @@
         <v>0</v>
       </c>
       <c r="P16" s="23" t="n">
-        <v>0.0462020736542011</v>
+        <v>0.0497002425066837</v>
       </c>
       <c r="Q16" s="15" t="n">
-        <v>1.07801109103371</v>
+        <v>1.29332825735224</v>
       </c>
       <c r="R16" s="24" t="n">
-        <v>0.123</v>
+        <v>0.079</v>
       </c>
       <c r="S16" s="16" t="n">
-        <f aca="false">776/$P$3</f>
-        <v>0.388</v>
+        <f aca="false">1339/$P$3</f>
+        <v>0.6695</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
-        <v>0.411633605752468</v>
+        <v>0.439307324929851</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.0289209788221949</v>
+        <v>0.127338801833183</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">0/$D$3</f>
@@ -4600,25 +4735,25 @@
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.281553398058252</v>
+        <v>0.388349514563107</v>
       </c>
       <c r="I17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J17" s="15" t="n">
-        <v>0.452674897119342</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K17" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L17" s="15" t="n">
-        <v>0.656652360515021</v>
+        <v>0.628006872852234</v>
       </c>
       <c r="M17" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N17" s="15" t="n">
         <v>0.55</v>
@@ -4627,65 +4762,65 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P17" s="25" t="n">
-        <v>0.0450466025027233</v>
-      </c>
-      <c r="Q17" s="18" t="n">
-        <v>1.17910447761194</v>
+      <c r="P17" s="23" t="n">
+        <v>0.0462020736542011</v>
+      </c>
+      <c r="Q17" s="15" t="n">
+        <v>1.07801109103371</v>
       </c>
       <c r="R17" s="24" t="n">
-        <v>0.135</v>
-      </c>
-      <c r="S17" s="26" t="n">
-        <f aca="false">1829/$P$3</f>
-        <v>0.9145</v>
+        <v>0.123</v>
+      </c>
+      <c r="S17" s="16" t="n">
+        <f aca="false">776/$P$3</f>
+        <v>0.388</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(D18,F18,H18,J18,L18,N18)</f>
-        <v>0.479783624027799</v>
+        <v>0.411633605752468</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.369274416448439</v>
+        <v>0.0289209788221949</v>
       </c>
       <c r="E18" s="16" t="n">
-        <f aca="false">4/$D$3</f>
-        <v>0.0043956043956044</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F18" s="15" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.281553398058252</v>
       </c>
       <c r="I18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J18" s="15" t="n">
-        <v>0.44017094017094</v>
+        <v>0.452674897119342</v>
       </c>
       <c r="K18" s="16" t="n">
-        <f aca="false">9/$J$3</f>
-        <v>0.037037037037037</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L18" s="15" t="n">
-        <v>0.649741824440619</v>
+        <v>0.656652360515021</v>
       </c>
       <c r="M18" s="16" t="n">
-        <f aca="false">3/$L$3</f>
-        <v>0.00257510729613734</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N18" s="15" t="n">
         <v>0.55</v>
@@ -4695,36 +4830,36 @@
         <v>0</v>
       </c>
       <c r="P18" s="23" t="n">
-        <v>0.0263546139456426</v>
+        <v>0.0450466025027233</v>
       </c>
       <c r="Q18" s="15" t="n">
-        <v>0.384891506009518</v>
+        <v>1.17910447761194</v>
       </c>
       <c r="R18" s="24" t="n">
-        <v>0.08</v>
+        <v>0.135</v>
       </c>
       <c r="S18" s="16" t="n">
-        <f aca="false">80/$P$3</f>
-        <v>0.04</v>
+        <f aca="false">1829/$P$3</f>
+        <v>0.9145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(D19,F19,H19,J19,L19,N19)</f>
-        <v>0.405257833604129</v>
+        <v>0.479783624027799</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>-0.0714529452409867</v>
+        <v>0.369274416448439</v>
       </c>
       <c r="E19" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">4/$D$3</f>
+        <v>0.0043956043956044</v>
       </c>
       <c r="F19" s="15" t="n">
         <v>0.52</v>
@@ -4734,110 +4869,177 @@
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>0.469135802469136</v>
+        <v>0.44017094017094</v>
       </c>
       <c r="K19" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">9/$J$3</f>
+        <v>0.037037037037037</v>
       </c>
       <c r="L19" s="15" t="n">
-        <v>0.618556701030928</v>
+        <v>0.649741824440619</v>
       </c>
       <c r="M19" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">3/$L$3</f>
+        <v>0.00257510729613734</v>
       </c>
       <c r="N19" s="15" t="n">
-        <v>0.516666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="O19" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P19" s="23" t="n">
-        <v>0.018613476307488</v>
+        <v>0.0263546139456426</v>
       </c>
       <c r="Q19" s="15" t="n">
-        <v>1.12997748971513</v>
+        <v>0.384891506009518</v>
       </c>
       <c r="R19" s="24" t="n">
-        <v>0.116</v>
+        <v>0.08</v>
       </c>
       <c r="S19" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">80/$P$3</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(D20,F20,H20,J20,L20,N20)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D20" s="15" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G20" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="15" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I20" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="15" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K20" s="16" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="15" t="n">
+        <v>0.618556701030928</v>
+      </c>
+      <c r="M20" s="16" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N20" s="15" t="n">
+        <v>0.516666666666667</v>
+      </c>
+      <c r="O20" s="16" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="23" t="n">
+        <v>0.018613476307488</v>
+      </c>
+      <c r="Q20" s="15" t="n">
+        <v>1.12997748971513</v>
+      </c>
+      <c r="R20" s="24" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="S20" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="14" t="n">
+        <f aca="false">AVERAGE(D21,F21,H21,J21,L21,N21)</f>
         <v>0.364587789621774</v>
       </c>
-      <c r="D20" s="15" t="n">
+      <c r="D21" s="15" t="n">
         <v>0.0266825503923221</v>
       </c>
-      <c r="E20" s="16" t="n">
+      <c r="E21" s="16" t="n">
         <f aca="false">187/$D$3</f>
         <v>0.205494505494505</v>
       </c>
-      <c r="F20" s="15" t="n">
+      <c r="F21" s="15" t="n">
         <v>0.461538461538462</v>
       </c>
-      <c r="G20" s="16" t="n">
+      <c r="G21" s="16" t="n">
         <f aca="false">9/$F$3</f>
         <v>0.09</v>
       </c>
-      <c r="H20" s="15" t="n">
+      <c r="H21" s="15" t="n">
         <v>0.237113402061856</v>
       </c>
-      <c r="I20" s="16" t="n">
+      <c r="I21" s="16" t="n">
         <f aca="false">6/$H$3</f>
         <v>0.058252427184466</v>
       </c>
-      <c r="J20" s="15" t="n">
+      <c r="J21" s="15" t="n">
         <v>0.558823529411765</v>
       </c>
-      <c r="K20" s="16" t="n">
+      <c r="K21" s="16" t="n">
         <f aca="false">39/$J$3</f>
         <v>0.160493827160494</v>
       </c>
-      <c r="L20" s="15" t="n">
+      <c r="L21" s="15" t="n">
         <v>0.403368794326241</v>
       </c>
-      <c r="M20" s="16" t="n">
+      <c r="M21" s="16" t="n">
         <f aca="false">37/$L$3</f>
         <v>0.0317596566523605</v>
       </c>
-      <c r="N20" s="15" t="n">
+      <c r="N21" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="O20" s="16" t="n">
+      <c r="O21" s="16" t="n">
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="P20" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="18" t="n">
+      <c r="P21" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="15" t="n">
         <v>1.02530466506249</v>
       </c>
-      <c r="R20" s="24" t="n">
+      <c r="R21" s="24" t="n">
         <v>0.544</v>
       </c>
-      <c r="S20" s="16" t="n">
+      <c r="S21" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
@@ -4859,8 +5061,8 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="S4:S20 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
+  <conditionalFormatting sqref="S4:S21 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4924,7 +5126,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P20">
+  <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4953,14 +5155,15 @@
     <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
     <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
     <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B20" r:id="rId17" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B20" r:id="rId17" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B21" r:id="rId18" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4969,7 +5172,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tried to extend measurements with falconmamba... but it's very bad... gave up
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -380,6 +380,15 @@
     <t xml:space="preserve">https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF</t>
   </si>
   <si>
+    <t xml:space="preserve">falcon-mamba-7b-instruct.Q6_K.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
     <t xml:space="preserve">HuLU</t>
   </si>
   <si>
@@ -417,12 +426,6 @@
   </si>
   <si>
     <t xml:space="preserve">Azure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falcon-mamba-7b-instruct.Q6_K.gguf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,6 +626,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -664,7 +675,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="142">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -691,6 +702,366 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF80B766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF81B666"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82B566"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88B266"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93AC67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF94AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2A368"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3A268"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAA9E68"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB39969"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBB9469"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC78D6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCE896B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF6D6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCCCC"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF95AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9CA668"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAC9D69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB19A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB29A69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB59869"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC1916A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC68E6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC8A6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27E6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE37D6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE776C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2756D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF83B566"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF87B266"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAE67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF91AD67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF95AA67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF98A967"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BA768"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9DA668"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7ABA66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7BB966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7DB966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7EB866"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FB766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82B666"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF84B466"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -699,6 +1070,94 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF78BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF80B666"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF90AD67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF96AA67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB89669"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC2906A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCA8C6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD2876B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDD816B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDE806C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE07F6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF87B366"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -707,15 +1166,183 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF88B266"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8DAF67"/>
+          <fgColor rgb="FF8CB067"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4A268"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA7A068"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCD8A6B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEF766D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8AB167"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EAF67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF98A867"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0886B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDA826B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE17E6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE27D6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE47C6C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEC786C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99A867"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9EA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAB9D69"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC8B6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7CB966"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CAF67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -731,638 +1358,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFA2A368"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA4A268"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA5A168"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBB9469"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBC946A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC78D6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD5856B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE27E6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF5736D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF6D6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCCCC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF94AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF95AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9CA668"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAA9E68"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAC9D69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB19A69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB29A69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB59869"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC1916A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC68E6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC8A6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE37D6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEE776C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2756D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF80B766"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF81B666"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF83B566"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF87B266"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAE67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF91AD67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93AC67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF95AA67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF98A967"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BA768"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9DA668"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7ABA66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7BB966"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7DB966"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7EB866"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7FB766"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF82B666"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF78BB66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF80B666"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF90AD67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF96AA67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB89669"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCA8C6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2876B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDD816B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDE806C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE07F6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8CB067"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA7A068"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCD8A6B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF766D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF82B566"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8AB167"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF98A867"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0886B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85B366"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9FA568"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA3A268"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCE896B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDA826B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE17E6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE27D6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE47C6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEC786C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF79BB66"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99A867"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9EA568"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAB9D69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC8B6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7CB966"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8CAF67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFC98C6A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1428,14 +1423,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFA89F68"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC2906A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1512,6 +1499,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFD5856B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFD6856B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1633,6 +1628,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF93AB67"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA5A168"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2001,10 +2004,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2110,7 +2113,7 @@
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -3514,6 +3517,93 @@
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="14" t="n">
+        <f aca="false">AVERAGE(W20,T20:U20,R20,P20,N20,M20,K20,H20,I20,F20,D20)</f>
+        <v>0.457777805523234</v>
+      </c>
+      <c r="D20" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <f aca="false">12/$D$3</f>
+        <v>0.0115052732502397</v>
+      </c>
+      <c r="F20" s="15" t="n">
+        <v>0.31758314125782</v>
+      </c>
+      <c r="G20" s="19" t="n">
+        <f aca="false">3741/$F$3</f>
+        <v>0.381151299032094</v>
+      </c>
+      <c r="H20" s="15" t="n">
+        <v>0.679389312977099</v>
+      </c>
+      <c r="I20" s="15" t="n">
+        <v>0.809090909090909</v>
+      </c>
+      <c r="J20" s="16" t="n">
+        <f aca="false">15/$H$3</f>
+        <v>0.0367647058823529</v>
+      </c>
+      <c r="K20" s="15" t="n">
+        <v>0.482825664290343</v>
+      </c>
+      <c r="L20" s="19" t="n">
+        <f aca="false">3920/$K$3</f>
+        <v>0.717554457257917</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="O20" s="16" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q20" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="S20" s="16" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="U20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="V20" s="16" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="X20" s="16" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:X48"/>
@@ -3530,7 +3620,7 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3671,6 +3761,7 @@
     <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
     <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
     <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3679,8 +3770,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -3692,7 +3783,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3714,7 +3805,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="19" width="8.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="21" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="7.69"/>
   </cols>
   <sheetData>
@@ -3726,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3739,12 +3830,12 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="P1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -3753,38 +3844,38 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="P2" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
+      <c r="A3" s="23" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
         <v>18</v>
       </c>
@@ -3829,10 +3920,10 @@
         <v>2000</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>13</v>
@@ -3891,13 +3982,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="25" t="n">
         <v>0.136446672153424</v>
       </c>
       <c r="Q4" s="15" t="n">
         <v>1.06958782892184</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="26" t="n">
         <v>0.033</v>
       </c>
       <c r="S4" s="16" t="n">
@@ -3958,13 +4049,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="23" t="n">
+      <c r="P5" s="25" t="n">
         <v>0.130232557010572</v>
       </c>
       <c r="Q5" s="15" t="n">
         <v>1.02813785608942</v>
       </c>
-      <c r="R5" s="24" t="n">
+      <c r="R5" s="26" t="n">
         <v>0.018</v>
       </c>
       <c r="S5" s="16" t="n">
@@ -4025,13 +4116,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="23" t="n">
+      <c r="P6" s="25" t="n">
         <v>0.115675852676348</v>
       </c>
       <c r="Q6" s="15" t="n">
         <v>1.05320394846913</v>
       </c>
-      <c r="R6" s="24" t="n">
+      <c r="R6" s="26" t="n">
         <v>0.029</v>
       </c>
       <c r="S6" s="16" t="n">
@@ -4092,13 +4183,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="23" t="n">
+      <c r="P7" s="25" t="n">
         <v>0.114080663228868</v>
       </c>
       <c r="Q7" s="15" t="n">
         <v>1.03143346379648</v>
       </c>
-      <c r="R7" s="24" t="n">
+      <c r="R7" s="26" t="n">
         <v>0.045</v>
       </c>
       <c r="S7" s="16" t="n">
@@ -4159,13 +4250,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P8" s="23" t="n">
+      <c r="P8" s="25" t="n">
         <v>0.113227204219314</v>
       </c>
       <c r="Q8" s="15" t="n">
         <v>1.02468032181585</v>
       </c>
-      <c r="R8" s="24" t="n">
+      <c r="R8" s="26" t="n">
         <v>0.029</v>
       </c>
       <c r="S8" s="16" t="n">
@@ -4226,13 +4317,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P9" s="23" t="n">
+      <c r="P9" s="25" t="n">
         <v>0.0946010077074703</v>
       </c>
       <c r="Q9" s="15" t="n">
         <v>0.950708101886604</v>
       </c>
-      <c r="R9" s="24" t="n">
+      <c r="R9" s="26" t="n">
         <v>0.036</v>
       </c>
       <c r="S9" s="16" t="n">
@@ -4293,13 +4384,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P10" s="23" t="n">
+      <c r="P10" s="25" t="n">
         <v>0.0869997613324107</v>
       </c>
       <c r="Q10" s="15" t="n">
         <v>1.1923877607133</v>
       </c>
-      <c r="R10" s="24" t="n">
+      <c r="R10" s="26" t="n">
         <v>0.035</v>
       </c>
       <c r="S10" s="16" t="n">
@@ -4360,13 +4451,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P11" s="23" t="n">
+      <c r="P11" s="25" t="n">
         <v>0.0704660506880692</v>
       </c>
       <c r="Q11" s="15" t="n">
         <v>1.10242179616549</v>
       </c>
-      <c r="R11" s="24" t="n">
+      <c r="R11" s="26" t="n">
         <v>0.083</v>
       </c>
       <c r="S11" s="16" t="n">
@@ -4427,13 +4518,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P12" s="25" t="n">
+      <c r="P12" s="27" t="n">
         <v>0.0672850889690679</v>
       </c>
       <c r="Q12" s="18" t="n">
         <v>1.14115440228223</v>
       </c>
-      <c r="R12" s="24" t="n">
+      <c r="R12" s="26" t="n">
         <v>0.08</v>
       </c>
       <c r="S12" s="16" t="n">
@@ -4494,13 +4585,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P13" s="23" t="n">
+      <c r="P13" s="25" t="n">
         <v>0.0672142694158681</v>
       </c>
       <c r="Q13" s="15" t="n">
         <v>1.08084074373484</v>
       </c>
-      <c r="R13" s="24" t="n">
+      <c r="R13" s="26" t="n">
         <v>0.068</v>
       </c>
       <c r="S13" s="16" t="n">
@@ -4561,13 +4652,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P14" s="23" t="n">
+      <c r="P14" s="25" t="n">
         <v>0.0666584744053729</v>
       </c>
       <c r="Q14" s="15" t="n">
         <v>1.05036977813312</v>
       </c>
-      <c r="R14" s="24" t="n">
+      <c r="R14" s="26" t="n">
         <v>0.061</v>
       </c>
       <c r="S14" s="16" t="n">
@@ -4628,13 +4719,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P15" s="23" t="n">
+      <c r="P15" s="25" t="n">
         <v>0.0534217525346316</v>
       </c>
       <c r="Q15" s="15" t="n">
         <v>1.26345272449499</v>
       </c>
-      <c r="R15" s="24" t="n">
+      <c r="R15" s="26" t="n">
         <v>0.041</v>
       </c>
       <c r="S15" s="16" t="n">
@@ -4695,13 +4786,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P16" s="23" t="n">
+      <c r="P16" s="25" t="n">
         <v>0.0497002425066837</v>
       </c>
       <c r="Q16" s="15" t="n">
         <v>1.29332825735224</v>
       </c>
-      <c r="R16" s="24" t="n">
+      <c r="R16" s="26" t="n">
         <v>0.079</v>
       </c>
       <c r="S16" s="16" t="n">
@@ -4762,13 +4853,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P17" s="23" t="n">
+      <c r="P17" s="25" t="n">
         <v>0.0462020736542011</v>
       </c>
       <c r="Q17" s="15" t="n">
         <v>1.07801109103371</v>
       </c>
-      <c r="R17" s="24" t="n">
+      <c r="R17" s="26" t="n">
         <v>0.123</v>
       </c>
       <c r="S17" s="16" t="n">
@@ -4829,13 +4920,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P18" s="23" t="n">
+      <c r="P18" s="25" t="n">
         <v>0.0450466025027233</v>
       </c>
       <c r="Q18" s="15" t="n">
         <v>1.17910447761194</v>
       </c>
-      <c r="R18" s="24" t="n">
+      <c r="R18" s="26" t="n">
         <v>0.135</v>
       </c>
       <c r="S18" s="16" t="n">
@@ -4845,10 +4936,10 @@
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(D19,F19,H19,J19,L19,N19)</f>
@@ -4896,13 +4987,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P19" s="23" t="n">
+      <c r="P19" s="25" t="n">
         <v>0.0263546139456426</v>
       </c>
       <c r="Q19" s="15" t="n">
         <v>0.384891506009518</v>
       </c>
-      <c r="R19" s="24" t="n">
+      <c r="R19" s="26" t="n">
         <v>0.08</v>
       </c>
       <c r="S19" s="16" t="n">
@@ -4963,13 +5054,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P20" s="23" t="n">
+      <c r="P20" s="25" t="n">
         <v>0.018613476307488</v>
       </c>
       <c r="Q20" s="15" t="n">
         <v>1.12997748971513</v>
       </c>
-      <c r="R20" s="24" t="n">
+      <c r="R20" s="26" t="n">
         <v>0.116</v>
       </c>
       <c r="S20" s="16" t="n">
@@ -4979,10 +5070,10 @@
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(D21,F21,H21,J21,L21,N21)</f>
@@ -5030,13 +5121,13 @@
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="P21" s="23" t="n">
+      <c r="P21" s="25" t="n">
         <v>0</v>
       </c>
       <c r="Q21" s="15" t="n">
         <v>1.02530466506249</v>
       </c>
-      <c r="R21" s="24" t="n">
+      <c r="R21" s="26" t="n">
         <v>0.544</v>
       </c>
       <c r="S21" s="16" t="n">
@@ -5062,7 +5153,7 @@
     <mergeCell ref="P2:S2"/>
   </mergeCells>
   <conditionalFormatting sqref="S4:S21 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add gemma2 9b results
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -302,6 +302,12 @@
     <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-27b-it-GGUF</t>
   </si>
   <si>
+    <t xml:space="preserve">gemma-2-9b-it-Q6_K_L.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-9b-it-GGUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">mixtral-8x7b-instruct-v0.1.Q5_K_M.gguf</t>
   </si>
   <si>
@@ -374,19 +380,19 @@
     <t xml:space="preserve">https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF</t>
   </si>
   <si>
+    <t xml:space="preserve">falcon-mamba-7b-instruct.Q6_K.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
     <t xml:space="preserve">SambaLingo-Hungarian-Chat-Q5_K_M.gguf</t>
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falcon-mamba-7b-instruct.Q6_K.gguf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--</t>
   </si>
   <si>
     <t xml:space="preserve">HuLU</t>
@@ -549,7 +555,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -626,14 +632,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -675,7 +673,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="142">
+  <dxfs count="145">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -734,6 +732,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF86B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF88B266"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -910,6 +916,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFD2876B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFE27E6C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -958,6 +972,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF8BB067"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF8DAF67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1126,14 +1148,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD2876B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFDD816B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1206,6 +1220,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF85B466"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF8AB167"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1238,14 +1260,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF85B466"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF9FA568"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1342,6 +1356,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF7EB766"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF8CAF67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1374,15 +1396,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF7DB866"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF84B566"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF86B366"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1539,6 +1561,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFA6A068"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFF1756D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1612,14 +1642,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFD6E6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7EB766"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2007,7 +2029,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="9:9 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2113,7 +2135,7 @@
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -2430,80 +2452,80 @@
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
-        <v>0.761759832782204</v>
-      </c>
-      <c r="D7" s="15" t="n">
-        <v>0.597514874790058</v>
+        <v>0.779541622537469</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>0.592121670308154</v>
       </c>
       <c r="E7" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.478247580234335</v>
+        <v>0.351299032093734</v>
       </c>
       <c r="G7" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>0.757352941176471</v>
+        <v>0.767156862745098</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.834170854271357</v>
+        <v>0.816955684007707</v>
       </c>
       <c r="J7" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>0.767975055025679</v>
+        <v>0.894197327475746</v>
       </c>
       <c r="L7" s="16" t="n">
-        <f aca="false">11/$K$3</f>
-        <v>0.00201354567087681</v>
-      </c>
-      <c r="M7" s="15" t="n">
-        <v>0.824560969577047</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="18" t="n">
+        <v>0.814914667326243</v>
       </c>
       <c r="N7" s="15" t="n">
-        <v>0.785041064339182</v>
+        <v>0.772172324554727</v>
       </c>
       <c r="O7" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P7" s="15" t="n">
-        <v>0.746376811594203</v>
+        <v>0.88086642599278</v>
       </c>
       <c r="Q7" s="16" t="n">
-        <f aca="false">1/$P$3</f>
-        <v>0.0036101083032491</v>
-      </c>
-      <c r="R7" s="15" t="n">
-        <v>0.95752009184845</v>
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="18" t="n">
+        <v>0.942660550458716</v>
       </c>
       <c r="S7" s="16" t="n">
-        <f aca="false">1/$R$3</f>
-        <v>0.00114678899082569</v>
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
       </c>
       <c r="T7" s="15" t="n">
-        <v>0.87058607341487</v>
+        <v>0.85733495291754</v>
       </c>
       <c r="U7" s="15" t="n">
-        <v>0.873884353171137</v>
+        <v>0.876087578202987</v>
       </c>
       <c r="V7" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W7" s="15" t="n">
-        <v>0.647887323943662</v>
+        <v>0.788732394366197</v>
       </c>
       <c r="X7" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2519,75 +2541,75 @@
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
-        <v>0.740393758714782</v>
+        <v>0.761759832782204</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.526754313381707</v>
+        <v>0.597514874790058</v>
       </c>
       <c r="E8" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.418644931227713</v>
+        <v>0.478247580234335</v>
       </c>
       <c r="G8" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.737745098039216</v>
+        <v>0.757352941176471</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>0.820770519262982</v>
+        <v>0.834170854271357</v>
       </c>
       <c r="J8" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>0.833424858136555</v>
+        <v>0.767975055025679</v>
       </c>
       <c r="L8" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">11/$K$3</f>
+        <v>0.00201354567087681</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.765767994063814</v>
+        <v>0.824560969577047</v>
       </c>
       <c r="N8" s="15" t="n">
-        <v>0.742172610944732</v>
+        <v>0.785041064339182</v>
       </c>
       <c r="O8" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P8" s="15" t="n">
-        <v>0.84115523465704</v>
+        <v>0.746376811594203</v>
       </c>
       <c r="Q8" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">1/$P$3</f>
+        <v>0.0036101083032491</v>
       </c>
       <c r="R8" s="15" t="n">
-        <v>0.940366972477064</v>
+        <v>0.95752009184845</v>
       </c>
       <c r="S8" s="16" t="n">
-        <f aca="false">0/$R$3</f>
-        <v>0</v>
+        <f aca="false">1/$R$3</f>
+        <v>0.00114678899082569</v>
       </c>
       <c r="T8" s="15" t="n">
-        <v>0.767106912789686</v>
+        <v>0.87058607341487</v>
       </c>
       <c r="U8" s="15" t="n">
-        <v>0.772505800441942</v>
+        <v>0.873884353171137</v>
       </c>
       <c r="V8" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W8" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.647887323943662</v>
       </c>
       <c r="X8" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2603,75 +2625,75 @@
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
-        <v>0.728207755738953</v>
+        <v>0.740393758714782</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.417240141074992</v>
+        <v>0.526754313381707</v>
       </c>
       <c r="E9" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>0.315944982170148</v>
+        <v>0.418644931227713</v>
       </c>
       <c r="G9" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.779411764705882</v>
+        <v>0.737745098039216</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.84375</v>
+        <v>0.820770519262982</v>
       </c>
       <c r="J9" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>0.733088909257562</v>
+        <v>0.833424858136555</v>
       </c>
       <c r="L9" s="16" t="n">
-        <f aca="false">8/$K$3</f>
-        <v>0.00146439685154677</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.814964135542914</v>
+        <v>0.765767994063814</v>
       </c>
       <c r="N9" s="15" t="n">
-        <v>0.753954941621444</v>
+        <v>0.742172610944732</v>
       </c>
       <c r="O9" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P9" s="15" t="n">
-        <v>0.707581227436823</v>
+        <v>0.84115523465704</v>
       </c>
       <c r="Q9" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R9" s="15" t="n">
-        <v>0.907110091743119</v>
+        <v>0.940366972477064</v>
       </c>
       <c r="S9" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T9" s="15" t="n">
-        <v>0.817610857364514</v>
+        <v>0.767106912789686</v>
       </c>
       <c r="U9" s="15" t="n">
-        <v>0.830934609499328</v>
+        <v>0.772505800441942</v>
       </c>
       <c r="V9" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W9" s="15" t="n">
-        <v>0.816901408450704</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X9" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2687,75 +2709,75 @@
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">AVERAGE(W10,T10:U10,R10,P10,N10,M10,K10,H10,I10,F10,D10)</f>
-        <v>0.723374373278101</v>
+        <v>0.728207755738953</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.451542212782268</v>
+        <v>0.417240141074992</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.462964849719817</v>
+        <v>0.315944982170148</v>
       </c>
       <c r="G10" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.801470588235294</v>
+        <v>0.779411764705882</v>
       </c>
       <c r="I10" s="15" t="n">
-        <v>0.850828729281768</v>
+        <v>0.84375</v>
       </c>
       <c r="J10" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K10" s="15" t="n">
-        <v>0.8555738605162</v>
+        <v>0.733088909257562</v>
       </c>
       <c r="L10" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
       </c>
       <c r="M10" s="15" t="n">
-        <v>0.822681177343557</v>
+        <v>0.814964135542914</v>
       </c>
       <c r="N10" s="15" t="n">
-        <v>0.777062536928196</v>
+        <v>0.753954941621444</v>
       </c>
       <c r="O10" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P10" s="15" t="n">
-        <v>0.317689530685921</v>
+        <v>0.707581227436823</v>
       </c>
       <c r="Q10" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R10" s="15" t="n">
-        <v>0.951834862385321</v>
+        <v>0.907110091743119</v>
       </c>
       <c r="S10" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T10" s="15" t="n">
-        <v>0.831672916702132</v>
+        <v>0.817610857364514</v>
       </c>
       <c r="U10" s="15" t="n">
-        <v>0.838861355601802</v>
+        <v>0.830934609499328</v>
       </c>
       <c r="V10" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W10" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.816901408450704</v>
       </c>
       <c r="X10" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2771,75 +2793,75 @@
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">AVERAGE(W11,T11:U11,R11,P11,N11,M11,K11,H11,I11,F11,D11)</f>
-        <v>0.704245669484917</v>
+        <v>0.723374373278101</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>0.61400038680535</v>
+        <v>0.451542212782268</v>
       </c>
       <c r="E11" s="16" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F11" s="15" t="n">
-        <v>0.417524197656648</v>
+        <v>0.462964849719817</v>
       </c>
       <c r="G11" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H11" s="15" t="n">
-        <v>0.742647058823529</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I11" s="15" t="n">
-        <v>0.837209302325581</v>
+        <v>0.850828729281768</v>
       </c>
       <c r="J11" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K11" s="15" t="n">
-        <v>0.317480719794344</v>
+        <v>0.8555738605162</v>
       </c>
       <c r="L11" s="16" t="n">
-        <f aca="false">17/$K$3</f>
-        <v>0.00311184330953688</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M11" s="15" t="n">
-        <v>0.720652980460054</v>
+        <v>0.822681177343557</v>
       </c>
       <c r="N11" s="15" t="n">
-        <v>0.719543084181773</v>
+        <v>0.777062536928196</v>
       </c>
       <c r="O11" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P11" s="15" t="n">
-        <v>0.68231046931408</v>
+        <v>0.317689530685921</v>
       </c>
       <c r="Q11" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R11" s="15" t="n">
-        <v>0.935779816513762</v>
+        <v>0.951834862385321</v>
       </c>
       <c r="S11" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T11" s="15" t="n">
-        <v>0.860305870097761</v>
+        <v>0.831672916702132</v>
       </c>
       <c r="U11" s="15" t="n">
-        <v>0.871099781648942</v>
+        <v>0.838861355601802</v>
       </c>
       <c r="V11" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W11" s="15" t="n">
-        <v>0.732394366197183</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X11" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2850,80 +2872,80 @@
       <c r="A12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
-        <v>0.699391112337297</v>
-      </c>
-      <c r="D12" s="18" t="n">
-        <v>0.625980868840778</v>
+        <v>0.704245669484917</v>
+      </c>
+      <c r="D12" s="15" t="n">
+        <v>0.61400038680535</v>
       </c>
       <c r="E12" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
-      </c>
-      <c r="F12" s="18" t="n">
-        <v>0.37493632195619</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
+      </c>
+      <c r="F12" s="15" t="n">
+        <v>0.417524197656648</v>
       </c>
       <c r="G12" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H12" s="15" t="n">
-        <v>0.801470588235294</v>
+        <v>0.742647058823529</v>
       </c>
       <c r="I12" s="15" t="n">
-        <v>0.86522462562396</v>
+        <v>0.837209302325581</v>
       </c>
       <c r="J12" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K12" s="18" t="n">
-        <v>0.438496791934006</v>
+      <c r="K12" s="15" t="n">
+        <v>0.317480719794344</v>
       </c>
       <c r="L12" s="16" t="n">
-        <f aca="false">8/$K$3</f>
-        <v>0.00146439685154677</v>
-      </c>
-      <c r="M12" s="18" t="n">
-        <v>0.852128527963984</v>
+        <f aca="false">17/$K$3</f>
+        <v>0.00311184330953688</v>
+      </c>
+      <c r="M12" s="15" t="n">
+        <v>0.720652980460054</v>
       </c>
       <c r="N12" s="15" t="n">
-        <v>0.805846053913608</v>
+        <v>0.719543084181773</v>
       </c>
       <c r="O12" s="16" t="n">
-        <f aca="false">3/$M$3</f>
-        <v>7.42023250061835E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P12" s="15" t="n">
-        <v>0.133574007220217</v>
+        <v>0.68231046931408</v>
       </c>
       <c r="Q12" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R12" s="15" t="n">
-        <v>0.930045871559633</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S12" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T12" s="18" t="n">
-        <v>0.886137481283129</v>
+      <c r="T12" s="15" t="n">
+        <v>0.860305870097761</v>
       </c>
       <c r="U12" s="15" t="n">
-        <v>0.890119815150565</v>
+        <v>0.871099781648942</v>
       </c>
       <c r="V12" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W12" s="15" t="n">
-        <v>0.788732394366197</v>
+        <v>0.732394366197183</v>
       </c>
       <c r="X12" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2939,75 +2961,75 @@
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(W13,T13:U13,R13,P13,N13,M13,K13,H13,I13,F13,D13)</f>
-        <v>0.658513623474907</v>
+        <v>0.699391112337297</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.523854029130735</v>
+        <v>0.625980868840778</v>
       </c>
       <c r="E13" s="16" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.480334216425515</v>
+        <v>0.37493632195619</v>
       </c>
       <c r="G13" s="16" t="n">
-        <f aca="false">1/$F$3</f>
-        <v>0.000101884870096791</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.727941176470588</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I13" s="15" t="n">
-        <v>0.821829855537721</v>
+        <v>0.86522462562396</v>
       </c>
       <c r="J13" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K13" s="15" t="n">
-        <v>0.696448187477115</v>
+        <v>0.438496791934006</v>
       </c>
       <c r="L13" s="16" t="n">
-        <f aca="false">1/$K$3</f>
-        <v>0.000183049606443346</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
       </c>
       <c r="M13" s="15" t="n">
-        <v>0.509271935283136</v>
+        <v>0.852128527963984</v>
       </c>
       <c r="N13" s="15" t="n">
-        <v>0.593278732490252</v>
+        <v>0.805846053913608</v>
       </c>
       <c r="O13" s="16" t="n">
-        <f aca="false">255/$M$3</f>
-        <v>0.0063071976255256</v>
+        <f aca="false">3/$M$3</f>
+        <v>7.42023250061835E-005</v>
       </c>
       <c r="P13" s="15" t="n">
-        <v>0.249097472924188</v>
+        <v>0.133574007220217</v>
       </c>
       <c r="Q13" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R13" s="15" t="n">
-        <v>0.934633027522936</v>
+        <v>0.930045871559633</v>
       </c>
       <c r="S13" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T13" s="15" t="n">
-        <v>0.821663265900952</v>
+        <v>0.886137481283129</v>
       </c>
       <c r="U13" s="15" t="n">
-        <v>0.825501723380821</v>
+        <v>0.890119815150565</v>
       </c>
       <c r="V13" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W13" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.788732394366197</v>
       </c>
       <c r="X13" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3023,68 +3045,68 @@
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(W14,T14:U14,R14,P14,N14,M14,K14,H14,I14,F14,D14)</f>
-        <v>0.653779197430066</v>
+        <v>0.658513623474907</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>0.455627237079107</v>
+        <v>0.523854029130735</v>
       </c>
       <c r="E14" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F14" s="15" t="n">
-        <v>0.386958736627611</v>
+        <v>0.480334216425515</v>
       </c>
       <c r="G14" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">1/$F$3</f>
+        <v>0.000101884870096791</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.754901960784314</v>
+        <v>0.727941176470588</v>
       </c>
       <c r="I14" s="15" t="n">
-        <v>0.835526315789474</v>
+        <v>0.821829855537721</v>
       </c>
       <c r="J14" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K14" s="15" t="n">
-        <v>0.136371956800293</v>
+        <v>0.696448187477115</v>
       </c>
       <c r="L14" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">1/$K$3</f>
+        <v>0.000183049606443346</v>
       </c>
       <c r="M14" s="15" t="n">
-        <v>0.82352213702696</v>
+        <v>0.509271935283136</v>
       </c>
       <c r="N14" s="15" t="n">
-        <v>0.77733046219143</v>
+        <v>0.593278732490252</v>
       </c>
       <c r="O14" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
+        <f aca="false">255/$M$3</f>
+        <v>0.0063071976255256</v>
       </c>
       <c r="P14" s="15" t="n">
-        <v>0.353790613718412</v>
+        <v>0.249097472924188</v>
       </c>
       <c r="Q14" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R14" s="15" t="n">
-        <v>0.935779816513762</v>
+        <v>0.934633027522936</v>
       </c>
       <c r="S14" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T14" s="15" t="n">
-        <v>0.826388381403035</v>
+        <v>0.821663265900952</v>
       </c>
       <c r="U14" s="15" t="n">
-        <v>0.840842892071465</v>
+        <v>0.825501723380821</v>
       </c>
       <c r="V14" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3107,75 +3129,75 @@
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(W15,T15:U15,R15,P15,N15,M15,K15,H15,I15,F15,D15)</f>
-        <v>0.64108637065082</v>
+        <v>0.653779197430066</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>0.531920773750409</v>
+        <v>0.455627237079107</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.42985226693836</v>
+        <v>0.386958736627611</v>
       </c>
       <c r="G15" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.705882352941177</v>
+        <v>0.754901960784314</v>
       </c>
       <c r="I15" s="15" t="n">
-        <v>0.82089552238806</v>
+        <v>0.835526315789474</v>
       </c>
       <c r="J15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K15" s="15" t="n">
-        <v>0.540377220289324</v>
+        <v>0.136371956800293</v>
       </c>
       <c r="L15" s="16" t="n">
-        <f aca="false">2/$K$3</f>
-        <v>0.000366099212886692</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M15" s="15" t="n">
-        <v>0.80123670541677</v>
+        <v>0.82352213702696</v>
       </c>
       <c r="N15" s="15" t="n">
-        <v>0.772955868226253</v>
+        <v>0.77733046219143</v>
       </c>
       <c r="O15" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P15" s="15" t="n">
-        <v>0.296028880866426</v>
+        <v>0.353790613718412</v>
       </c>
       <c r="Q15" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R15" s="15" t="n">
-        <v>0.928899082568807</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S15" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T15" s="15" t="n">
-        <v>0.621129369842947</v>
+        <v>0.826388381403035</v>
       </c>
       <c r="U15" s="15" t="n">
-        <v>0.666393615848911</v>
+        <v>0.840842892071465</v>
       </c>
       <c r="V15" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W15" s="15" t="n">
-        <v>0.577464788732394</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X15" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3191,68 +3213,68 @@
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(W16,T16:U16,R16,P16,N16,M16,K16,H16,I16,F16,D16)</f>
-        <v>0.613554278796799</v>
+        <v>0.64108637065082</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>0.375051720670997</v>
+        <v>0.531920773750409</v>
       </c>
       <c r="E16" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.538767193071829</v>
+        <v>0.42985226693836</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.730392156862745</v>
+        <v>0.705882352941177</v>
       </c>
       <c r="I16" s="15" t="n">
-        <v>0.827044025157233</v>
+        <v>0.82089552238806</v>
       </c>
       <c r="J16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K16" s="15" t="n">
-        <v>0.557386051619989</v>
+        <v>0.540377220289324</v>
       </c>
       <c r="L16" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">2/$K$3</f>
+        <v>0.000366099212886692</v>
       </c>
       <c r="M16" s="15" t="n">
-        <v>0.608706406134059</v>
+        <v>0.80123670541677</v>
       </c>
       <c r="N16" s="15" t="n">
-        <v>0.625189537528431</v>
+        <v>0.772955868226253</v>
       </c>
       <c r="O16" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P16" s="15" t="n">
-        <v>0.425992779783394</v>
+        <v>0.296028880866426</v>
       </c>
       <c r="Q16" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R16" s="15" t="n">
-        <v>0.932339449541284</v>
+        <v>0.928899082568807</v>
       </c>
       <c r="S16" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T16" s="15" t="n">
-        <v>0.573663619974553</v>
+        <v>0.621129369842947</v>
       </c>
       <c r="U16" s="15" t="n">
-        <v>0.590653616484677</v>
+        <v>0.666393615848911</v>
       </c>
       <c r="V16" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3275,75 +3297,75 @@
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(W17,T17:U17,R17,P17,N17,M17,K17,H17,I17,F17,D17)</f>
-        <v>0.588337454921144</v>
+        <v>0.613554278796799</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.275218494690191</v>
+        <v>0.375051720670997</v>
       </c>
       <c r="E17" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F17" s="15" t="n">
-        <v>0.256342333163525</v>
+        <v>0.538767193071829</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.718137254901961</v>
+        <v>0.730392156862745</v>
       </c>
       <c r="I17" s="15" t="n">
-        <v>0.822804314329738</v>
+        <v>0.827044025157233</v>
       </c>
       <c r="J17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K17" s="15" t="n">
-        <v>0.33260113490756</v>
+        <v>0.557386051619989</v>
       </c>
       <c r="L17" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M17" s="15" t="n">
-        <v>0.730112793113684</v>
+        <v>0.608706406134059</v>
       </c>
       <c r="N17" s="15" t="n">
-        <v>0.707110836711137</v>
+        <v>0.625189537528431</v>
       </c>
       <c r="O17" s="16" t="n">
-        <f aca="false">2/$M$3</f>
-        <v>4.9468216670789E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P17" s="15" t="n">
-        <v>0.339350180505415</v>
+        <v>0.425992779783394</v>
       </c>
       <c r="Q17" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R17" s="15" t="n">
-        <v>0.918577981651376</v>
+        <v>0.932339449541284</v>
       </c>
       <c r="S17" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T17" s="15" t="n">
-        <v>0.730177716008711</v>
+        <v>0.573663619974553</v>
       </c>
       <c r="U17" s="15" t="n">
-        <v>0.750743179633811</v>
+        <v>0.590653616484677</v>
       </c>
       <c r="V17" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W17" s="15" t="n">
-        <v>0.47887323943662</v>
+        <v>0.577464788732394</v>
       </c>
       <c r="X17" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3359,68 +3381,68 @@
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(W18,T18:U18,R18,P18,N18,M18,K18,H18,I18,F18,D18)</f>
-        <v>0.499454443668613</v>
+        <v>0.588337454921144</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.333471865271531</v>
+        <v>0.275218494690191</v>
       </c>
       <c r="E18" s="16" t="n">
-        <f aca="false">6/$D$3</f>
-        <v>0.00575263662511985</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F18" s="15" t="n">
-        <v>0.292103922567499</v>
+        <v>0.256342333163525</v>
       </c>
       <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.698529411764706</v>
+        <v>0.718137254901961</v>
       </c>
       <c r="I18" s="15" t="n">
-        <v>0.805687203791469</v>
+        <v>0.822804314329738</v>
       </c>
       <c r="J18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K18" s="15" t="n">
-        <v>0.391434449223864</v>
+        <v>0.33260113490756</v>
       </c>
       <c r="L18" s="16" t="n">
-        <f aca="false">116/$K$3</f>
-        <v>0.0212337543474282</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M18" s="15" t="n">
-        <v>0.691602220900258</v>
+        <v>0.730112793113684</v>
       </c>
       <c r="N18" s="15" t="n">
-        <v>0.36669042044182</v>
+        <v>0.707110836711137</v>
       </c>
       <c r="O18" s="16" t="n">
-        <f aca="false">86/$M$3</f>
-        <v>0.00212713331684393</v>
+        <f aca="false">2/$M$3</f>
+        <v>4.9468216670789E-005</v>
       </c>
       <c r="P18" s="15" t="n">
-        <v>0.306859205776173</v>
+        <v>0.339350180505415</v>
       </c>
       <c r="Q18" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R18" s="15" t="n">
-        <v>0.855504587155963</v>
+        <v>0.918577981651376</v>
       </c>
       <c r="S18" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T18" s="15" t="n">
-        <v>0.370306926073738</v>
+        <v>0.730177716008711</v>
       </c>
       <c r="U18" s="15" t="n">
-        <v>0.402389871619712</v>
+        <v>0.750743179633811</v>
       </c>
       <c r="V18" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3443,75 +3465,75 @@
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(W19,T19:U19,R19,P19,N19,M19,K19,H19,I19,F19,D19)</f>
-        <v>0.338674923063942</v>
+        <v>0.499454443668613</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.241606739317903</v>
+        <v>0.333471865271531</v>
       </c>
       <c r="E19" s="16" t="n">
-        <f aca="false">7/$D$3</f>
-        <v>0.00671140939597315</v>
+        <f aca="false">6/$D$3</f>
+        <v>0.00575263662511985</v>
       </c>
       <c r="F19" s="15" t="n">
-        <v>0.285161027313494</v>
+        <v>0.292103922567499</v>
       </c>
       <c r="G19" s="16" t="n">
-        <f aca="false">3/$F$3</f>
-        <v>0.000305654610290372</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.333333333333333</v>
+        <v>0.698529411764706</v>
       </c>
       <c r="I19" s="15" t="n">
-        <v>0.0620689655172414</v>
+        <v>0.805687203791469</v>
       </c>
       <c r="J19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K19" s="15" t="n">
-        <v>0.32644239804548</v>
+        <v>0.391434449223864</v>
       </c>
       <c r="L19" s="16" t="n">
-        <f aca="false">142/$K$3</f>
-        <v>0.0259930441149552</v>
+        <f aca="false">116/$K$3</f>
+        <v>0.0212337543474282</v>
       </c>
       <c r="M19" s="15" t="n">
-        <v>0.459092373658512</v>
+        <v>0.691602220900258</v>
       </c>
       <c r="N19" s="15" t="n">
-        <v>0.524490151647202</v>
+        <v>0.36669042044182</v>
       </c>
       <c r="O19" s="16" t="n">
-        <f aca="false">83/$M$3</f>
-        <v>0.00205293099183774</v>
+        <f aca="false">86/$M$3</f>
+        <v>0.00212713331684393</v>
       </c>
       <c r="P19" s="15" t="n">
-        <v>0.357400722021661</v>
+        <v>0.306859205776173</v>
       </c>
       <c r="Q19" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R19" s="15" t="n">
-        <v>0.894374282433984</v>
+        <v>0.855504587155963</v>
       </c>
       <c r="S19" s="16" t="n">
-        <f aca="false">1/$R$3</f>
-        <v>0.00114678899082569</v>
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
       </c>
       <c r="T19" s="15" t="n">
-        <v>0.0103797859681123</v>
+        <v>0.370306926073738</v>
       </c>
       <c r="U19" s="15" t="n">
-        <v>0.119045072158263</v>
+        <v>0.402389871619712</v>
       </c>
       <c r="V19" s="16" t="n">
-        <f aca="false">10/$T$3</f>
-        <v>0.00666666666666667</v>
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
       </c>
       <c r="W19" s="15" t="n">
-        <v>0.450704225352113</v>
+        <v>0.47887323943662</v>
       </c>
       <c r="X19" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3539,7 +3561,7 @@
       <c r="F20" s="15" t="n">
         <v>0.31758314125782</v>
       </c>
-      <c r="G20" s="19" t="n">
+      <c r="G20" s="16" t="n">
         <f aca="false">3741/$F$3</f>
         <v>0.381151299032094</v>
       </c>
@@ -3556,7 +3578,7 @@
       <c r="K20" s="15" t="n">
         <v>0.482825664290343</v>
       </c>
-      <c r="L20" s="19" t="n">
+      <c r="L20" s="16" t="n">
         <f aca="false">3920/$K$3</f>
         <v>0.717554457257917</v>
       </c>
@@ -3603,7 +3625,88 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
+      <c r="A21" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="14" t="n">
+        <f aca="false">AVERAGE(W21,T21:U21,R21,P21,N21,M21,K21,H21,I21,F21,D21)</f>
+        <v>0.338674923063942</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>0.241606739317903</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <f aca="false">7/$D$3</f>
+        <v>0.00671140939597315</v>
+      </c>
+      <c r="F21" s="15" t="n">
+        <v>0.285161027313494</v>
+      </c>
+      <c r="G21" s="16" t="n">
+        <f aca="false">3/$F$3</f>
+        <v>0.000305654610290372</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="I21" s="15" t="n">
+        <v>0.0620689655172414</v>
+      </c>
+      <c r="J21" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="15" t="n">
+        <v>0.32644239804548</v>
+      </c>
+      <c r="L21" s="16" t="n">
+        <f aca="false">142/$K$3</f>
+        <v>0.0259930441149552</v>
+      </c>
+      <c r="M21" s="15" t="n">
+        <v>0.459092373658512</v>
+      </c>
+      <c r="N21" s="15" t="n">
+        <v>0.524490151647202</v>
+      </c>
+      <c r="O21" s="16" t="n">
+        <f aca="false">83/$M$3</f>
+        <v>0.00205293099183774</v>
+      </c>
+      <c r="P21" s="15" t="n">
+        <v>0.357400722021661</v>
+      </c>
+      <c r="Q21" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="15" t="n">
+        <v>0.894374282433984</v>
+      </c>
+      <c r="S21" s="16" t="n">
+        <f aca="false">1/$R$3</f>
+        <v>0.00114678899082569</v>
+      </c>
+      <c r="T21" s="15" t="n">
+        <v>0.0103797859681123</v>
+      </c>
+      <c r="U21" s="15" t="n">
+        <v>0.119045072158263</v>
+      </c>
+      <c r="V21" s="16" t="n">
+        <f aca="false">10/$T$3</f>
+        <v>0.00666666666666667</v>
+      </c>
+      <c r="W21" s="15" t="n">
+        <v>0.450704225352113</v>
+      </c>
+      <c r="X21" s="16" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:X48"/>
@@ -3619,8 +3722,8 @@
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="W2:X2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 V4:V48 X4:X48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+  <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 X4:X48 V4:V48">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3748,20 +3851,21 @@
     <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
     <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
     <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
     <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3770,8 +3874,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <drawing r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -3780,10 +3884,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3805,7 +3909,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="21" width="8.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="19" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="7.69"/>
   </cols>
   <sheetData>
@@ -3817,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3830,12 +3934,12 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -3844,40 +3948,40 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
+      <c r="P2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="n">
+      <c r="A3" s="21" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -3920,10 +4024,10 @@
         <v>2000</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>13</v>
@@ -3982,13 +4086,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="25" t="n">
+      <c r="P4" s="23" t="n">
         <v>0.136446672153424</v>
       </c>
       <c r="Q4" s="15" t="n">
         <v>1.06958782892184</v>
       </c>
-      <c r="R4" s="26" t="n">
+      <c r="R4" s="24" t="n">
         <v>0.033</v>
       </c>
       <c r="S4" s="16" t="n">
@@ -3998,10 +4102,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C5" s="14" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
@@ -4049,13 +4153,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="25" t="n">
+      <c r="P5" s="23" t="n">
         <v>0.130232557010572</v>
       </c>
       <c r="Q5" s="15" t="n">
         <v>1.02813785608942</v>
       </c>
-      <c r="R5" s="26" t="n">
+      <c r="R5" s="24" t="n">
         <v>0.018</v>
       </c>
       <c r="S5" s="16" t="n">
@@ -4065,10 +4169,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" s="14" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
@@ -4116,13 +4220,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="25" t="n">
+      <c r="P6" s="23" t="n">
         <v>0.115675852676348</v>
       </c>
       <c r="Q6" s="15" t="n">
         <v>1.05320394846913</v>
       </c>
-      <c r="R6" s="26" t="n">
+      <c r="R6" s="24" t="n">
         <v>0.029</v>
       </c>
       <c r="S6" s="16" t="n">
@@ -4132,10 +4236,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
@@ -4183,13 +4287,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="25" t="n">
+      <c r="P7" s="23" t="n">
         <v>0.114080663228868</v>
       </c>
       <c r="Q7" s="15" t="n">
         <v>1.03143346379648</v>
       </c>
-      <c r="R7" s="26" t="n">
+      <c r="R7" s="24" t="n">
         <v>0.045</v>
       </c>
       <c r="S7" s="16" t="n">
@@ -4199,10 +4303,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
@@ -4250,13 +4354,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P8" s="25" t="n">
+      <c r="P8" s="23" t="n">
         <v>0.113227204219314</v>
       </c>
       <c r="Q8" s="15" t="n">
         <v>1.02468032181585</v>
       </c>
-      <c r="R8" s="26" t="n">
+      <c r="R8" s="24" t="n">
         <v>0.029</v>
       </c>
       <c r="S8" s="16" t="n">
@@ -4268,43 +4372,43 @@
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
-        <v>0.449693612435578</v>
-      </c>
-      <c r="D9" s="15" t="n">
-        <v>0.204119502057382</v>
+        <v>0.494563798892394</v>
+      </c>
+      <c r="D9" s="18" t="n">
+        <v>0.36951447436442</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F9" s="15" t="n">
-        <v>0.46</v>
+      <c r="F9" s="18" t="n">
+        <v>0.586956521739131</v>
       </c>
       <c r="G9" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="15" t="n">
-        <v>0.368932038834951</v>
+        <f aca="false">54/$F$3</f>
+        <v>0.54</v>
+      </c>
+      <c r="H9" s="18" t="n">
+        <v>0.349514563106796</v>
       </c>
       <c r="I9" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J9" s="15" t="n">
-        <v>0.442148760330579</v>
+      <c r="J9" s="18" t="n">
+        <v>0.444444444444444</v>
       </c>
       <c r="K9" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
-      </c>
-      <c r="L9" s="15" t="n">
-        <v>0.672961373390558</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="18" t="n">
+        <v>0.666952789699571</v>
       </c>
       <c r="M9" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -4318,17 +4422,17 @@
         <v>0</v>
       </c>
       <c r="P9" s="25" t="n">
-        <v>0.0946010077074703</v>
-      </c>
-      <c r="Q9" s="15" t="n">
-        <v>0.950708101886604</v>
-      </c>
-      <c r="R9" s="26" t="n">
-        <v>0.036</v>
+        <v>0.11250845895661</v>
+      </c>
+      <c r="Q9" s="18" t="n">
+        <v>1.029565082082</v>
+      </c>
+      <c r="R9" s="24" t="n">
+        <v>0.032</v>
       </c>
       <c r="S9" s="16" t="n">
-        <f aca="false">506/$P$3</f>
-        <v>0.253</v>
+        <f aca="false">6/$P$3</f>
+        <v>0.003</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4340,38 +4444,38 @@
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
-        <v>0.446939595430147</v>
+        <v>0.449693612435578</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.214844642079834</v>
+        <v>0.204119502057382</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="G10" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.310679611650485</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I10" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J10" s="15" t="n">
-        <v>0.448559670781893</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K10" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L10" s="15" t="n">
-        <v>0.68755364806867</v>
+        <v>0.672961373390558</v>
       </c>
       <c r="M10" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -4384,65 +4488,65 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P10" s="25" t="n">
-        <v>0.0869997613324107</v>
+      <c r="P10" s="23" t="n">
+        <v>0.0946010077074703</v>
       </c>
       <c r="Q10" s="15" t="n">
-        <v>1.1923877607133</v>
-      </c>
-      <c r="R10" s="26" t="n">
-        <v>0.035</v>
+        <v>0.950708101886604</v>
+      </c>
+      <c r="R10" s="24" t="n">
+        <v>0.036</v>
       </c>
       <c r="S10" s="16" t="n">
-        <f aca="false">28/$P$3</f>
-        <v>0.014</v>
+        <f aca="false">506/$P$3</f>
+        <v>0.253</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">AVERAGE(D11,F11,H11,J11,L11,N11)</f>
-        <v>0.456362837616999</v>
+        <v>0.446939595430147</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>0.304699117807113</v>
+        <v>0.214844642079834</v>
       </c>
       <c r="E11" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F11" s="15" t="n">
-        <v>0.466666666666667</v>
+        <v>0.47</v>
       </c>
       <c r="G11" s="16" t="n">
-        <f aca="false">25/$F$3</f>
-        <v>0.25</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H11" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.310679611650485</v>
       </c>
       <c r="I11" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J11" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.448559670781893</v>
       </c>
       <c r="K11" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L11" s="15" t="n">
-        <v>0.622852233676976</v>
+        <v>0.68755364806867</v>
       </c>
       <c r="M11" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N11" s="15" t="n">
         <v>0.55</v>
@@ -4451,118 +4555,118 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P11" s="25" t="n">
-        <v>0.0704660506880692</v>
+      <c r="P11" s="23" t="n">
+        <v>0.0869997613324107</v>
       </c>
       <c r="Q11" s="15" t="n">
-        <v>1.10242179616549</v>
-      </c>
-      <c r="R11" s="26" t="n">
-        <v>0.083</v>
+        <v>1.1923877607133</v>
+      </c>
+      <c r="R11" s="24" t="n">
+        <v>0.035</v>
       </c>
       <c r="S11" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">28/$P$3</f>
+        <v>0.014</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
-        <v>0.478378567077423</v>
-      </c>
-      <c r="D12" s="18" t="n">
-        <v>0.267184035681135</v>
+        <v>0.456362837616999</v>
+      </c>
+      <c r="D12" s="15" t="n">
+        <v>0.304699117807113</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F12" s="18" t="n">
-        <v>0.653846153846154</v>
+      <c r="F12" s="15" t="n">
+        <v>0.466666666666667</v>
       </c>
       <c r="G12" s="16" t="n">
-        <f aca="false">74/$F$3</f>
-        <v>0.74</v>
-      </c>
-      <c r="H12" s="18" t="n">
-        <v>0.343137254901961</v>
+        <f aca="false">25/$F$3</f>
+        <v>0.25</v>
+      </c>
+      <c r="H12" s="15" t="n">
+        <v>0.349514563106796</v>
       </c>
       <c r="I12" s="16" t="n">
-        <f aca="false">1/$H$3</f>
-        <v>0.00970873786407767</v>
-      </c>
-      <c r="J12" s="18" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="15" t="n">
         <v>0.444444444444444</v>
       </c>
       <c r="K12" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L12" s="18" t="n">
-        <v>0.628326180257511</v>
+      <c r="L12" s="15" t="n">
+        <v>0.622852233676976</v>
       </c>
       <c r="M12" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="18" t="n">
-        <v>0.533333333333333</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N12" s="15" t="n">
+        <v>0.55</v>
       </c>
       <c r="O12" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P12" s="27" t="n">
-        <v>0.0672850889690679</v>
-      </c>
-      <c r="Q12" s="18" t="n">
-        <v>1.14115440228223</v>
-      </c>
-      <c r="R12" s="26" t="n">
-        <v>0.08</v>
+      <c r="P12" s="23" t="n">
+        <v>0.0704660506880692</v>
+      </c>
+      <c r="Q12" s="15" t="n">
+        <v>1.10242179616549</v>
+      </c>
+      <c r="R12" s="24" t="n">
+        <v>0.083</v>
       </c>
       <c r="S12" s="16" t="n">
-        <f aca="false">21/$P$3</f>
-        <v>0.0105</v>
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(D13,F13,H13,J13,L13,N13)</f>
-        <v>0.416323225087402</v>
+        <v>0.478378567077423</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.00078604321068414</v>
+        <v>0.267184035681135</v>
       </c>
       <c r="E13" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.49</v>
+        <v>0.653846153846154</v>
       </c>
       <c r="G13" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">74/$F$3</f>
+        <v>0.74</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.343137254901961</v>
       </c>
       <c r="I13" s="16" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
+        <f aca="false">1/$H$3</f>
+        <v>0.00970873786407767</v>
       </c>
       <c r="J13" s="15" t="n">
         <v>0.444444444444444</v>
@@ -4572,74 +4676,74 @@
         <v>0</v>
       </c>
       <c r="L13" s="15" t="n">
-        <v>0.643776824034335</v>
+        <v>0.628326180257511</v>
       </c>
       <c r="M13" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N13" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O13" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P13" s="25" t="n">
-        <v>0.0672142694158681</v>
+      <c r="P13" s="23" t="n">
+        <v>0.0672850889690679</v>
       </c>
       <c r="Q13" s="15" t="n">
-        <v>1.08084074373484</v>
-      </c>
-      <c r="R13" s="26" t="n">
-        <v>0.068</v>
+        <v>1.14115440228223</v>
+      </c>
+      <c r="R13" s="24" t="n">
+        <v>0.08</v>
       </c>
       <c r="S13" s="16" t="n">
-        <f aca="false">1817/$P$3</f>
-        <v>0.9085</v>
+        <f aca="false">21/$P$3</f>
+        <v>0.0105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(D14,F14,H14,J14,L14,N14)</f>
-        <v>0.436042704459863</v>
+        <v>0.416323225087402</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>0.0518271447518188</v>
+        <v>0.00078604321068414</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F14" s="15" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="G14" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.398058252427184</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I14" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J14" s="15" t="n">
-        <v>0.448559670781893</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K14" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L14" s="15" t="n">
-        <v>0.667811158798283</v>
+        <v>0.643776824034335</v>
       </c>
       <c r="M14" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -4652,199 +4756,199 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P14" s="25" t="n">
-        <v>0.0666584744053729</v>
+      <c r="P14" s="23" t="n">
+        <v>0.0672142694158681</v>
       </c>
       <c r="Q14" s="15" t="n">
-        <v>1.05036977813312</v>
-      </c>
-      <c r="R14" s="26" t="n">
-        <v>0.061</v>
+        <v>1.08084074373484</v>
+      </c>
+      <c r="R14" s="24" t="n">
+        <v>0.068</v>
       </c>
       <c r="S14" s="16" t="n">
-        <f aca="false">1206/$P$3</f>
-        <v>0.603</v>
+        <f aca="false">1817/$P$3</f>
+        <v>0.9085</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(D15,F15,H15,J15,L15,N15)</f>
-        <v>0.419278530088385</v>
+        <v>0.436042704459863</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>-0.0155335936055105</v>
+        <v>0.0518271447518188</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="G15" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.398058252427184</v>
       </c>
       <c r="I15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J15" s="15" t="n">
-        <v>0.489711934156379</v>
+        <v>0.448559670781893</v>
       </c>
       <c r="K15" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L15" s="15" t="n">
-        <v>0.659227467811159</v>
+        <v>0.667811158798283</v>
       </c>
       <c r="M15" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N15" s="15" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O15" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P15" s="25" t="n">
-        <v>0.0534217525346316</v>
+      <c r="P15" s="23" t="n">
+        <v>0.0666584744053729</v>
       </c>
       <c r="Q15" s="15" t="n">
-        <v>1.26345272449499</v>
-      </c>
-      <c r="R15" s="26" t="n">
-        <v>0.041</v>
+        <v>1.05036977813312</v>
+      </c>
+      <c r="R15" s="24" t="n">
+        <v>0.061</v>
       </c>
       <c r="S15" s="16" t="n">
-        <f aca="false">213/$P$3</f>
-        <v>0.1065</v>
+        <f aca="false">1206/$P$3</f>
+        <v>0.603</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(D16,F16,H16,J16,L16,N16)</f>
-        <v>0.432443158810545</v>
+        <v>0.419278530088385</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>0.0718486458091463</v>
+        <v>-0.0155335936055105</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J16" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.489711934156379</v>
       </c>
       <c r="K16" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L16" s="15" t="n">
-        <v>0.629725085910653</v>
+        <v>0.659227467811159</v>
       </c>
       <c r="M16" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N16" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O16" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P16" s="25" t="n">
-        <v>0.0497002425066837</v>
+      <c r="P16" s="23" t="n">
+        <v>0.0534217525346316</v>
       </c>
       <c r="Q16" s="15" t="n">
-        <v>1.29332825735224</v>
-      </c>
-      <c r="R16" s="26" t="n">
-        <v>0.079</v>
+        <v>1.26345272449499</v>
+      </c>
+      <c r="R16" s="24" t="n">
+        <v>0.041</v>
       </c>
       <c r="S16" s="16" t="n">
-        <f aca="false">1339/$P$3</f>
-        <v>0.6695</v>
+        <f aca="false">213/$P$3</f>
+        <v>0.1065</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
-        <v>0.439307324929851</v>
+        <v>0.432443158810545</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.127338801833183</v>
+        <v>0.0718486458091463</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F17" s="15" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.388349514563107</v>
+        <v>0.378640776699029</v>
       </c>
       <c r="I17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J17" s="15" t="n">
-        <v>0.442148760330579</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K17" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L17" s="15" t="n">
-        <v>0.628006872852234</v>
+        <v>0.629725085910653</v>
       </c>
       <c r="M17" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N17" s="15" t="n">
         <v>0.55</v>
@@ -4853,33 +4957,33 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P17" s="25" t="n">
-        <v>0.0462020736542011</v>
+      <c r="P17" s="23" t="n">
+        <v>0.0497002425066837</v>
       </c>
       <c r="Q17" s="15" t="n">
-        <v>1.07801109103371</v>
-      </c>
-      <c r="R17" s="26" t="n">
-        <v>0.123</v>
+        <v>1.29332825735224</v>
+      </c>
+      <c r="R17" s="24" t="n">
+        <v>0.079</v>
       </c>
       <c r="S17" s="16" t="n">
-        <f aca="false">776/$P$3</f>
-        <v>0.388</v>
+        <f aca="false">1339/$P$3</f>
+        <v>0.6695</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(D18,F18,H18,J18,L18,N18)</f>
-        <v>0.411633605752468</v>
+        <v>0.439307324929851</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.0289209788221949</v>
+        <v>0.127338801833183</v>
       </c>
       <c r="E18" s="16" t="n">
         <f aca="false">0/$D$3</f>
@@ -4893,25 +4997,25 @@
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.281553398058252</v>
+        <v>0.388349514563107</v>
       </c>
       <c r="I18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J18" s="15" t="n">
-        <v>0.452674897119342</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K18" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L18" s="15" t="n">
-        <v>0.656652360515021</v>
+        <v>0.628006872852234</v>
       </c>
       <c r="M18" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N18" s="15" t="n">
         <v>0.55</v>
@@ -4920,65 +5024,65 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P18" s="25" t="n">
-        <v>0.0450466025027233</v>
+      <c r="P18" s="23" t="n">
+        <v>0.0462020736542011</v>
       </c>
       <c r="Q18" s="15" t="n">
-        <v>1.17910447761194</v>
-      </c>
-      <c r="R18" s="26" t="n">
-        <v>0.135</v>
+        <v>1.07801109103371</v>
+      </c>
+      <c r="R18" s="24" t="n">
+        <v>0.123</v>
       </c>
       <c r="S18" s="16" t="n">
-        <f aca="false">1829/$P$3</f>
-        <v>0.9145</v>
+        <f aca="false">776/$P$3</f>
+        <v>0.388</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>61</v>
+        <v>38</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(D19,F19,H19,J19,L19,N19)</f>
-        <v>0.479783624027799</v>
+        <v>0.411633605752468</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.369274416448439</v>
+        <v>0.0289209788221949</v>
       </c>
       <c r="E19" s="16" t="n">
-        <f aca="false">4/$D$3</f>
-        <v>0.0043956043956044</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F19" s="15" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.281553398058252</v>
       </c>
       <c r="I19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>0.44017094017094</v>
+        <v>0.452674897119342</v>
       </c>
       <c r="K19" s="16" t="n">
-        <f aca="false">9/$J$3</f>
-        <v>0.037037037037037</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L19" s="15" t="n">
-        <v>0.649741824440619</v>
+        <v>0.656652360515021</v>
       </c>
       <c r="M19" s="16" t="n">
-        <f aca="false">3/$L$3</f>
-        <v>0.00257510729613734</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N19" s="15" t="n">
         <v>0.55</v>
@@ -4987,37 +5091,37 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P19" s="25" t="n">
-        <v>0.0263546139456426</v>
+      <c r="P19" s="23" t="n">
+        <v>0.0450466025027233</v>
       </c>
       <c r="Q19" s="15" t="n">
-        <v>0.384891506009518</v>
-      </c>
-      <c r="R19" s="26" t="n">
-        <v>0.08</v>
+        <v>1.17910447761194</v>
+      </c>
+      <c r="R19" s="24" t="n">
+        <v>0.135</v>
       </c>
       <c r="S19" s="16" t="n">
-        <f aca="false">80/$P$3</f>
-        <v>0.04</v>
+        <f aca="false">1829/$P$3</f>
+        <v>0.9145</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>33</v>
+        <v>62</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(D20,F20,H20,J20,L20,N20)</f>
-        <v>0.405257833604129</v>
+        <v>0.479783624027799</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>-0.0714529452409867</v>
+        <v>0.369274416448439</v>
       </c>
       <c r="E20" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">4/$D$3</f>
+        <v>0.0043956043956044</v>
       </c>
       <c r="F20" s="15" t="n">
         <v>0.52</v>
@@ -5027,110 +5131,177 @@
         <v>0</v>
       </c>
       <c r="H20" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I20" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J20" s="15" t="n">
-        <v>0.469135802469136</v>
+        <v>0.44017094017094</v>
       </c>
       <c r="K20" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">9/$J$3</f>
+        <v>0.037037037037037</v>
       </c>
       <c r="L20" s="15" t="n">
-        <v>0.618556701030928</v>
+        <v>0.649741824440619</v>
       </c>
       <c r="M20" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">3/$L$3</f>
+        <v>0.00257510729613734</v>
       </c>
       <c r="N20" s="15" t="n">
-        <v>0.516666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="O20" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P20" s="25" t="n">
-        <v>0.018613476307488</v>
+      <c r="P20" s="23" t="n">
+        <v>0.0263546139456426</v>
       </c>
       <c r="Q20" s="15" t="n">
-        <v>1.12997748971513</v>
-      </c>
-      <c r="R20" s="26" t="n">
-        <v>0.116</v>
+        <v>0.384891506009518</v>
+      </c>
+      <c r="R20" s="24" t="n">
+        <v>0.08</v>
       </c>
       <c r="S20" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">80/$P$3</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(D21,F21,H21,J21,L21,N21)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G21" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I21" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="15" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K21" s="16" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="15" t="n">
+        <v>0.618556701030928</v>
+      </c>
+      <c r="M21" s="16" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N21" s="15" t="n">
+        <v>0.516666666666667</v>
+      </c>
+      <c r="O21" s="16" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="23" t="n">
+        <v>0.018613476307488</v>
+      </c>
+      <c r="Q21" s="15" t="n">
+        <v>1.12997748971513</v>
+      </c>
+      <c r="R21" s="24" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="S21" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="14" t="n">
+        <f aca="false">AVERAGE(D22,F22,H22,J22,L22,N22)</f>
         <v>0.364587789621774</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D22" s="15" t="n">
         <v>0.0266825503923221</v>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">187/$D$3</f>
         <v>0.205494505494505</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F22" s="15" t="n">
         <v>0.461538461538462</v>
       </c>
-      <c r="G21" s="16" t="n">
+      <c r="G22" s="16" t="n">
         <f aca="false">9/$F$3</f>
         <v>0.09</v>
       </c>
-      <c r="H21" s="15" t="n">
+      <c r="H22" s="15" t="n">
         <v>0.237113402061856</v>
       </c>
-      <c r="I21" s="16" t="n">
+      <c r="I22" s="16" t="n">
         <f aca="false">6/$H$3</f>
         <v>0.058252427184466</v>
       </c>
-      <c r="J21" s="15" t="n">
+      <c r="J22" s="15" t="n">
         <v>0.558823529411765</v>
       </c>
-      <c r="K21" s="16" t="n">
+      <c r="K22" s="16" t="n">
         <f aca="false">39/$J$3</f>
         <v>0.160493827160494</v>
       </c>
-      <c r="L21" s="15" t="n">
+      <c r="L22" s="15" t="n">
         <v>0.403368794326241</v>
       </c>
-      <c r="M21" s="16" t="n">
+      <c r="M22" s="16" t="n">
         <f aca="false">37/$L$3</f>
         <v>0.0317596566523605</v>
       </c>
-      <c r="N21" s="15" t="n">
+      <c r="N22" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="O21" s="16" t="n">
+      <c r="O22" s="16" t="n">
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="P21" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="15" t="n">
+      <c r="P22" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="15" t="n">
         <v>1.02530466506249</v>
       </c>
-      <c r="R21" s="26" t="n">
+      <c r="R22" s="24" t="n">
         <v>0.544</v>
       </c>
-      <c r="S21" s="16" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
@@ -5152,8 +5323,8 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="S4:S21 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
+  <conditionalFormatting sqref="S4:S22 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5217,7 +5388,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P21">
+  <conditionalFormatting sqref="P4:P22">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -5243,18 +5414,19 @@
     <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
     <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
     <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B20" r:id="rId17" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B21" r:id="rId18" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B21" r:id="rId18" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B22" r:id="rId19" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5263,7 +5435,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <drawing r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add gemma2 2b eval results
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gemma-2-2b-it-Q6_K_L.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-2b-it-GGUF</t>
   </si>
   <si>
     <t xml:space="preserve">Llama-3.2-3B-Instruct-Q6_K_L.gguf</t>
@@ -446,7 +452,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -493,13 +499,6 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -555,7 +554,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -624,11 +623,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -656,7 +651,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,7 +668,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="145">
+  <dxfs count="147">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -764,6 +759,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF9EA568"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFA2A368"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -948,6 +951,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFF1756D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFF2756D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1012,6 +1023,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF97A967"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF98A967"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1148,6 +1167,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFCF896B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFDD816B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1308,6 +1335,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFED776C"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF79BB66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1324,14 +1359,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF9EA568"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFAB9D69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1429,14 +1456,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFAE9C69"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCF896B"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1505,6 +1524,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC38F6A"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC48F6A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1569,14 +1596,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF1756D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF6726D"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1625,6 +1644,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB99569"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFAF9B69"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1673,14 +1700,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB99569"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFBC936A"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1722,14 +1741,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFE57C6C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED776C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2026,10 +2037,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="9:9 A6"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2135,7 +2146,7 @@
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -2452,14 +2463,14 @@
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
         <v>0.779541622537469</v>
       </c>
-      <c r="D7" s="18" t="n">
+      <c r="D7" s="15" t="n">
         <v>0.592121670308154</v>
       </c>
       <c r="E7" s="16" t="n">
@@ -2490,7 +2501,7 @@
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
-      <c r="M7" s="18" t="n">
+      <c r="M7" s="15" t="n">
         <v>0.814914667326243</v>
       </c>
       <c r="N7" s="15" t="n">
@@ -2507,7 +2518,7 @@
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R7" s="18" t="n">
+      <c r="R7" s="15" t="n">
         <v>0.942660550458716</v>
       </c>
       <c r="S7" s="16" t="n">
@@ -3297,68 +3308,68 @@
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(W17,T17:U17,R17,P17,N17,M17,K17,H17,I17,F17,D17)</f>
-        <v>0.613554278796799</v>
+        <v>0.623563086724128</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.375051720670997</v>
+        <v>0.477381210215107</v>
       </c>
       <c r="E17" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="15" t="n">
-        <v>0.538767193071829</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
+      </c>
+      <c r="F17" s="17" t="n">
+        <v>0.286907794192562</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.730392156862745</v>
+        <v>0.723039215686275</v>
       </c>
       <c r="I17" s="15" t="n">
-        <v>0.827044025157233</v>
+        <v>0.804835924006909</v>
       </c>
       <c r="J17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K17" s="15" t="n">
-        <v>0.557386051619989</v>
+        <v>0.409992652461425</v>
       </c>
       <c r="L17" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">19/$K$3</f>
+        <v>0.00347794252242358</v>
       </c>
       <c r="M17" s="15" t="n">
-        <v>0.608706406134059</v>
+        <v>0.750581251545882</v>
       </c>
       <c r="N17" s="15" t="n">
-        <v>0.625189537528431</v>
+        <v>0.721851381916478</v>
       </c>
       <c r="O17" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P17" s="15" t="n">
-        <v>0.425992779783394</v>
+        <v>0.245487364620939</v>
       </c>
       <c r="Q17" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R17" s="15" t="n">
-        <v>0.932339449541284</v>
+        <v>0.870412844036697</v>
       </c>
       <c r="S17" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T17" s="15" t="n">
-        <v>0.573663619974553</v>
+        <v>0.810628242029225</v>
       </c>
       <c r="U17" s="15" t="n">
-        <v>0.590653616484677</v>
+        <v>0.80417437124564</v>
       </c>
       <c r="V17" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3381,75 +3392,75 @@
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(W18,T18:U18,R18,P18,N18,M18,K18,H18,I18,F18,D18)</f>
-        <v>0.588337454921144</v>
+        <v>0.613554278796799</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.275218494690191</v>
+        <v>0.375051720670997</v>
       </c>
       <c r="E18" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F18" s="15" t="n">
-        <v>0.256342333163525</v>
+        <v>0.538767193071829</v>
       </c>
       <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.718137254901961</v>
+        <v>0.730392156862745</v>
       </c>
       <c r="I18" s="15" t="n">
-        <v>0.822804314329738</v>
+        <v>0.827044025157233</v>
       </c>
       <c r="J18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K18" s="15" t="n">
-        <v>0.33260113490756</v>
+        <v>0.557386051619989</v>
       </c>
       <c r="L18" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M18" s="15" t="n">
-        <v>0.730112793113684</v>
+        <v>0.608706406134059</v>
       </c>
       <c r="N18" s="15" t="n">
-        <v>0.707110836711137</v>
+        <v>0.625189537528431</v>
       </c>
       <c r="O18" s="16" t="n">
-        <f aca="false">2/$M$3</f>
-        <v>4.9468216670789E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P18" s="15" t="n">
-        <v>0.339350180505415</v>
+        <v>0.425992779783394</v>
       </c>
       <c r="Q18" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R18" s="15" t="n">
-        <v>0.918577981651376</v>
+        <v>0.932339449541284</v>
       </c>
       <c r="S18" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T18" s="15" t="n">
-        <v>0.730177716008711</v>
+        <v>0.573663619974553</v>
       </c>
       <c r="U18" s="15" t="n">
-        <v>0.750743179633811</v>
+        <v>0.590653616484677</v>
       </c>
       <c r="V18" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W18" s="15" t="n">
-        <v>0.47887323943662</v>
+        <v>0.577464788732394</v>
       </c>
       <c r="X18" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3465,68 +3476,68 @@
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(W19,T19:U19,R19,P19,N19,M19,K19,H19,I19,F19,D19)</f>
-        <v>0.499454443668613</v>
+        <v>0.588337454921144</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.333471865271531</v>
+        <v>0.275218494690191</v>
       </c>
       <c r="E19" s="16" t="n">
-        <f aca="false">6/$D$3</f>
-        <v>0.00575263662511985</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F19" s="15" t="n">
-        <v>0.292103922567499</v>
+        <v>0.256342333163525</v>
       </c>
       <c r="G19" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.698529411764706</v>
+        <v>0.718137254901961</v>
       </c>
       <c r="I19" s="15" t="n">
-        <v>0.805687203791469</v>
+        <v>0.822804314329738</v>
       </c>
       <c r="J19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K19" s="15" t="n">
-        <v>0.391434449223864</v>
+        <v>0.33260113490756</v>
       </c>
       <c r="L19" s="16" t="n">
-        <f aca="false">116/$K$3</f>
-        <v>0.0212337543474282</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M19" s="15" t="n">
-        <v>0.691602220900258</v>
+        <v>0.730112793113684</v>
       </c>
       <c r="N19" s="15" t="n">
-        <v>0.36669042044182</v>
+        <v>0.707110836711137</v>
       </c>
       <c r="O19" s="16" t="n">
-        <f aca="false">86/$M$3</f>
-        <v>0.00212713331684393</v>
+        <f aca="false">2/$M$3</f>
+        <v>4.9468216670789E-005</v>
       </c>
       <c r="P19" s="15" t="n">
-        <v>0.306859205776173</v>
+        <v>0.339350180505415</v>
       </c>
       <c r="Q19" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R19" s="15" t="n">
-        <v>0.855504587155963</v>
+        <v>0.918577981651376</v>
       </c>
       <c r="S19" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T19" s="15" t="n">
-        <v>0.370306926073738</v>
+        <v>0.730177716008711</v>
       </c>
       <c r="U19" s="15" t="n">
-        <v>0.402389871619712</v>
+        <v>0.750743179633811</v>
       </c>
       <c r="V19" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3549,75 +3560,75 @@
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(W20,T20:U20,R20,P20,N20,M20,K20,H20,I20,F20,D20)</f>
-        <v>0.457777805523234</v>
+        <v>0.499454443668613</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>0</v>
+        <v>0.333471865271531</v>
       </c>
       <c r="E20" s="16" t="n">
-        <f aca="false">12/$D$3</f>
-        <v>0.0115052732502397</v>
+        <f aca="false">6/$D$3</f>
+        <v>0.00575263662511985</v>
       </c>
       <c r="F20" s="15" t="n">
-        <v>0.31758314125782</v>
+        <v>0.292103922567499</v>
       </c>
       <c r="G20" s="16" t="n">
-        <f aca="false">3741/$F$3</f>
-        <v>0.381151299032094</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H20" s="15" t="n">
-        <v>0.679389312977099</v>
+        <v>0.698529411764706</v>
       </c>
       <c r="I20" s="15" t="n">
-        <v>0.809090909090909</v>
+        <v>0.805687203791469</v>
       </c>
       <c r="J20" s="16" t="n">
-        <f aca="false">15/$H$3</f>
-        <v>0.0367647058823529</v>
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
       </c>
       <c r="K20" s="15" t="n">
-        <v>0.482825664290343</v>
+        <v>0.391434449223864</v>
       </c>
       <c r="L20" s="16" t="n">
-        <f aca="false">3920/$K$3</f>
-        <v>0.717554457257917</v>
-      </c>
-      <c r="M20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="N20" s="15" t="s">
-        <v>48</v>
+        <f aca="false">116/$K$3</f>
+        <v>0.0212337543474282</v>
+      </c>
+      <c r="M20" s="15" t="n">
+        <v>0.691602220900258</v>
+      </c>
+      <c r="N20" s="15" t="n">
+        <v>0.36669042044182</v>
       </c>
       <c r="O20" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>48</v>
+        <f aca="false">86/$M$3</f>
+        <v>0.00212713331684393</v>
+      </c>
+      <c r="P20" s="15" t="n">
+        <v>0.306859205776173</v>
       </c>
       <c r="Q20" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R20" s="15" t="s">
-        <v>48</v>
+      <c r="R20" s="15" t="n">
+        <v>0.855504587155963</v>
       </c>
       <c r="S20" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="U20" s="15" t="s">
-        <v>48</v>
+      <c r="T20" s="15" t="n">
+        <v>0.370306926073738</v>
+      </c>
+      <c r="U20" s="15" t="n">
+        <v>0.402389871619712</v>
       </c>
       <c r="V20" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W20" s="15" t="s">
-        <v>48</v>
+      <c r="W20" s="15" t="n">
+        <v>0.47887323943662</v>
       </c>
       <c r="X20" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3626,84 +3637,168 @@
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(W21,T21:U21,R21,P21,N21,M21,K21,H21,I21,F21,D21)</f>
+        <v>0.457777805523234</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <f aca="false">12/$D$3</f>
+        <v>0.0115052732502397</v>
+      </c>
+      <c r="F21" s="15" t="n">
+        <v>0.31758314125782</v>
+      </c>
+      <c r="G21" s="16" t="n">
+        <f aca="false">3741/$F$3</f>
+        <v>0.381151299032094</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <v>0.679389312977099</v>
+      </c>
+      <c r="I21" s="15" t="n">
+        <v>0.809090909090909</v>
+      </c>
+      <c r="J21" s="16" t="n">
+        <f aca="false">15/$H$3</f>
+        <v>0.0367647058823529</v>
+      </c>
+      <c r="K21" s="15" t="n">
+        <v>0.482825664290343</v>
+      </c>
+      <c r="L21" s="16" t="n">
+        <f aca="false">3920/$K$3</f>
+        <v>0.717554457257917</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O21" s="16" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q21" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="16" t="n">
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="U21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" s="16" t="n">
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="X21" s="16" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="14" t="n">
+        <f aca="false">AVERAGE(W22,T22:U22,R22,P22,N22,M22,K22,H22,I22,F22,D22)</f>
         <v>0.338674923063942</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D22" s="15" t="n">
         <v>0.241606739317903</v>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">7/$D$3</f>
         <v>0.00671140939597315</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F22" s="15" t="n">
         <v>0.285161027313494</v>
       </c>
-      <c r="G21" s="16" t="n">
+      <c r="G22" s="16" t="n">
         <f aca="false">3/$F$3</f>
         <v>0.000305654610290372</v>
       </c>
-      <c r="H21" s="15" t="n">
+      <c r="H22" s="15" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="I21" s="15" t="n">
+      <c r="I22" s="15" t="n">
         <v>0.0620689655172414</v>
       </c>
-      <c r="J21" s="16" t="n">
+      <c r="J22" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="K21" s="15" t="n">
+      <c r="K22" s="15" t="n">
         <v>0.32644239804548</v>
       </c>
-      <c r="L21" s="16" t="n">
+      <c r="L22" s="16" t="n">
         <f aca="false">142/$K$3</f>
         <v>0.0259930441149552</v>
       </c>
-      <c r="M21" s="15" t="n">
+      <c r="M22" s="15" t="n">
         <v>0.459092373658512</v>
       </c>
-      <c r="N21" s="15" t="n">
+      <c r="N22" s="15" t="n">
         <v>0.524490151647202</v>
       </c>
-      <c r="O21" s="16" t="n">
+      <c r="O22" s="16" t="n">
         <f aca="false">83/$M$3</f>
         <v>0.00205293099183774</v>
       </c>
-      <c r="P21" s="15" t="n">
+      <c r="P22" s="15" t="n">
         <v>0.357400722021661</v>
       </c>
-      <c r="Q21" s="16" t="n">
+      <c r="Q22" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R21" s="15" t="n">
+      <c r="R22" s="15" t="n">
         <v>0.894374282433984</v>
       </c>
-      <c r="S21" s="16" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">1/$R$3</f>
         <v>0.00114678899082569</v>
       </c>
-      <c r="T21" s="15" t="n">
+      <c r="T22" s="15" t="n">
         <v>0.0103797859681123</v>
       </c>
-      <c r="U21" s="15" t="n">
+      <c r="U22" s="15" t="n">
         <v>0.119045072158263</v>
       </c>
-      <c r="V21" s="16" t="n">
+      <c r="V22" s="16" t="n">
         <f aca="false">10/$T$3</f>
         <v>0.00666666666666667</v>
       </c>
-      <c r="W21" s="15" t="n">
+      <c r="W22" s="15" t="n">
         <v>0.450704225352113</v>
       </c>
-      <c r="X21" s="16" t="n">
+      <c r="X22" s="16" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
@@ -3723,7 +3818,7 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 X4:X48 V4:V48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3861,11 +3956,12 @@
     <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
     <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
     <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3874,8 +3970,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <drawing r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -3884,10 +3980,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3909,7 +4005,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="19" width="8.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="7.69"/>
   </cols>
   <sheetData>
@@ -3921,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3934,12 +4030,12 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="P1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -3948,40 +4044,40 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="P2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
+      <c r="A3" s="20" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -4024,10 +4120,10 @@
         <v>2000</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="R3" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>13</v>
@@ -4086,13 +4182,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="22" t="n">
         <v>0.136446672153424</v>
       </c>
       <c r="Q4" s="15" t="n">
         <v>1.06958782892184</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="23" t="n">
         <v>0.033</v>
       </c>
       <c r="S4" s="16" t="n">
@@ -4102,10 +4198,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="14" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
@@ -4153,13 +4249,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P5" s="23" t="n">
+      <c r="P5" s="22" t="n">
         <v>0.130232557010572</v>
       </c>
       <c r="Q5" s="15" t="n">
         <v>1.02813785608942</v>
       </c>
-      <c r="R5" s="24" t="n">
+      <c r="R5" s="23" t="n">
         <v>0.018</v>
       </c>
       <c r="S5" s="16" t="n">
@@ -4169,10 +4265,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6" s="14" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
@@ -4220,13 +4316,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P6" s="23" t="n">
+      <c r="P6" s="22" t="n">
         <v>0.115675852676348</v>
       </c>
       <c r="Q6" s="15" t="n">
         <v>1.05320394846913</v>
       </c>
-      <c r="R6" s="24" t="n">
+      <c r="R6" s="23" t="n">
         <v>0.029</v>
       </c>
       <c r="S6" s="16" t="n">
@@ -4287,13 +4383,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P7" s="23" t="n">
+      <c r="P7" s="22" t="n">
         <v>0.114080663228868</v>
       </c>
       <c r="Q7" s="15" t="n">
         <v>1.03143346379648</v>
       </c>
-      <c r="R7" s="24" t="n">
+      <c r="R7" s="23" t="n">
         <v>0.045</v>
       </c>
       <c r="S7" s="16" t="n">
@@ -4303,10 +4399,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
@@ -4354,13 +4450,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P8" s="23" t="n">
+      <c r="P8" s="22" t="n">
         <v>0.113227204219314</v>
       </c>
       <c r="Q8" s="15" t="n">
         <v>1.02468032181585</v>
       </c>
-      <c r="R8" s="24" t="n">
+      <c r="R8" s="23" t="n">
         <v>0.029</v>
       </c>
       <c r="S8" s="16" t="n">
@@ -4372,42 +4468,42 @@
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
         <v>0.494563798892394</v>
       </c>
-      <c r="D9" s="18" t="n">
+      <c r="D9" s="15" t="n">
         <v>0.36951447436442</v>
       </c>
       <c r="E9" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F9" s="18" t="n">
+      <c r="F9" s="15" t="n">
         <v>0.586956521739131</v>
       </c>
       <c r="G9" s="16" t="n">
         <f aca="false">54/$F$3</f>
         <v>0.54</v>
       </c>
-      <c r="H9" s="18" t="n">
+      <c r="H9" s="15" t="n">
         <v>0.349514563106796</v>
       </c>
       <c r="I9" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
-      <c r="J9" s="18" t="n">
+      <c r="J9" s="15" t="n">
         <v>0.444444444444444</v>
       </c>
       <c r="K9" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L9" s="18" t="n">
+      <c r="L9" s="15" t="n">
         <v>0.666952789699571</v>
       </c>
       <c r="M9" s="16" t="n">
@@ -4421,13 +4517,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P9" s="25" t="n">
+      <c r="P9" s="22" t="n">
         <v>0.11250845895661</v>
       </c>
-      <c r="Q9" s="18" t="n">
+      <c r="Q9" s="15" t="n">
         <v>1.029565082082</v>
       </c>
-      <c r="R9" s="24" t="n">
+      <c r="R9" s="23" t="n">
         <v>0.032</v>
       </c>
       <c r="S9" s="16" t="n">
@@ -4488,13 +4584,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P10" s="23" t="n">
+      <c r="P10" s="22" t="n">
         <v>0.0946010077074703</v>
       </c>
       <c r="Q10" s="15" t="n">
         <v>0.950708101886604</v>
       </c>
-      <c r="R10" s="24" t="n">
+      <c r="R10" s="23" t="n">
         <v>0.036</v>
       </c>
       <c r="S10" s="16" t="n">
@@ -4555,13 +4651,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P11" s="23" t="n">
+      <c r="P11" s="22" t="n">
         <v>0.0869997613324107</v>
       </c>
       <c r="Q11" s="15" t="n">
         <v>1.1923877607133</v>
       </c>
-      <c r="R11" s="24" t="n">
+      <c r="R11" s="23" t="n">
         <v>0.035</v>
       </c>
       <c r="S11" s="16" t="n">
@@ -4622,13 +4718,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P12" s="23" t="n">
+      <c r="P12" s="22" t="n">
         <v>0.0704660506880692</v>
       </c>
       <c r="Q12" s="15" t="n">
         <v>1.10242179616549</v>
       </c>
-      <c r="R12" s="24" t="n">
+      <c r="R12" s="23" t="n">
         <v>0.083</v>
       </c>
       <c r="S12" s="16" t="n">
@@ -4689,13 +4785,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P13" s="23" t="n">
+      <c r="P13" s="22" t="n">
         <v>0.0672850889690679</v>
       </c>
       <c r="Q13" s="15" t="n">
         <v>1.14115440228223</v>
       </c>
-      <c r="R13" s="24" t="n">
+      <c r="R13" s="23" t="n">
         <v>0.08</v>
       </c>
       <c r="S13" s="16" t="n">
@@ -4756,13 +4852,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P14" s="23" t="n">
+      <c r="P14" s="22" t="n">
         <v>0.0672142694158681</v>
       </c>
       <c r="Q14" s="15" t="n">
         <v>1.08084074373484</v>
       </c>
-      <c r="R14" s="24" t="n">
+      <c r="R14" s="23" t="n">
         <v>0.068</v>
       </c>
       <c r="S14" s="16" t="n">
@@ -4823,13 +4919,13 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P15" s="23" t="n">
+      <c r="P15" s="22" t="n">
         <v>0.0666584744053729</v>
       </c>
       <c r="Q15" s="15" t="n">
         <v>1.05036977813312</v>
       </c>
-      <c r="R15" s="24" t="n">
+      <c r="R15" s="23" t="n">
         <v>0.061</v>
       </c>
       <c r="S15" s="16" t="n">
@@ -4846,176 +4942,176 @@
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(D16,F16,H16,J16,L16,N16)</f>
-        <v>0.419278530088385</v>
+        <v>0.425537790635605</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>-0.0155335936055105</v>
+        <v>0.128651460584234</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.320388349514563</v>
       </c>
       <c r="I16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J16" s="15" t="n">
-        <v>0.489711934156379</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K16" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L16" s="15" t="n">
-        <v>0.659227467811159</v>
+        <v>0.619742489270386</v>
       </c>
       <c r="M16" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N16" s="15" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O16" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P16" s="23" t="n">
-        <v>0.0534217525346316</v>
-      </c>
-      <c r="Q16" s="15" t="n">
-        <v>1.26345272449499</v>
-      </c>
-      <c r="R16" s="24" t="n">
-        <v>0.041</v>
+      <c r="P16" s="24" t="n">
+        <v>0.0618591437609282</v>
+      </c>
+      <c r="Q16" s="17" t="n">
+        <v>1.07679555721331</v>
+      </c>
+      <c r="R16" s="23" t="n">
+        <v>0.045</v>
       </c>
       <c r="S16" s="16" t="n">
-        <f aca="false">213/$P$3</f>
-        <v>0.1065</v>
+        <f aca="false">175/$P$3</f>
+        <v>0.0875</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
-        <v>0.432443158810545</v>
+        <v>0.419278530088385</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.0718486458091463</v>
+        <v>-0.0155335936055105</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F17" s="15" t="n">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J17" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.489711934156379</v>
       </c>
       <c r="K17" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L17" s="15" t="n">
-        <v>0.629725085910653</v>
+        <v>0.659227467811159</v>
       </c>
       <c r="M17" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N17" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O17" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P17" s="23" t="n">
-        <v>0.0497002425066837</v>
+      <c r="P17" s="22" t="n">
+        <v>0.0534217525346316</v>
       </c>
       <c r="Q17" s="15" t="n">
-        <v>1.29332825735224</v>
-      </c>
-      <c r="R17" s="24" t="n">
-        <v>0.079</v>
+        <v>1.26345272449499</v>
+      </c>
+      <c r="R17" s="23" t="n">
+        <v>0.041</v>
       </c>
       <c r="S17" s="16" t="n">
-        <f aca="false">1339/$P$3</f>
-        <v>0.6695</v>
+        <f aca="false">213/$P$3</f>
+        <v>0.1065</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(D18,F18,H18,J18,L18,N18)</f>
-        <v>0.439307324929851</v>
+        <v>0.432443158810545</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.127338801833183</v>
+        <v>0.0718486458091463</v>
       </c>
       <c r="E18" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F18" s="15" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.388349514563107</v>
+        <v>0.378640776699029</v>
       </c>
       <c r="I18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J18" s="15" t="n">
-        <v>0.442148760330579</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K18" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L18" s="15" t="n">
-        <v>0.628006872852234</v>
+        <v>0.629725085910653</v>
       </c>
       <c r="M18" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N18" s="15" t="n">
         <v>0.55</v>
@@ -5024,33 +5120,33 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P18" s="23" t="n">
-        <v>0.0462020736542011</v>
+      <c r="P18" s="22" t="n">
+        <v>0.0497002425066837</v>
       </c>
       <c r="Q18" s="15" t="n">
-        <v>1.07801109103371</v>
-      </c>
-      <c r="R18" s="24" t="n">
-        <v>0.123</v>
+        <v>1.29332825735224</v>
+      </c>
+      <c r="R18" s="23" t="n">
+        <v>0.079</v>
       </c>
       <c r="S18" s="16" t="n">
-        <f aca="false">776/$P$3</f>
-        <v>0.388</v>
+        <f aca="false">1339/$P$3</f>
+        <v>0.6695</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(D19,F19,H19,J19,L19,N19)</f>
-        <v>0.411633605752468</v>
+        <v>0.439307324929851</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.0289209788221949</v>
+        <v>0.127338801833183</v>
       </c>
       <c r="E19" s="16" t="n">
         <f aca="false">0/$D$3</f>
@@ -5064,25 +5160,25 @@
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.281553398058252</v>
+        <v>0.388349514563107</v>
       </c>
       <c r="I19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>0.452674897119342</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K19" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L19" s="15" t="n">
-        <v>0.656652360515021</v>
+        <v>0.628006872852234</v>
       </c>
       <c r="M19" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N19" s="15" t="n">
         <v>0.55</v>
@@ -5091,65 +5187,65 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P19" s="23" t="n">
-        <v>0.0450466025027233</v>
+      <c r="P19" s="22" t="n">
+        <v>0.0462020736542011</v>
       </c>
       <c r="Q19" s="15" t="n">
-        <v>1.17910447761194</v>
-      </c>
-      <c r="R19" s="24" t="n">
-        <v>0.135</v>
+        <v>1.07801109103371</v>
+      </c>
+      <c r="R19" s="23" t="n">
+        <v>0.123</v>
       </c>
       <c r="S19" s="16" t="n">
-        <f aca="false">1829/$P$3</f>
-        <v>0.9145</v>
+        <f aca="false">776/$P$3</f>
+        <v>0.388</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(D20,F20,H20,J20,L20,N20)</f>
-        <v>0.479783624027799</v>
+        <v>0.411633605752468</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>0.369274416448439</v>
+        <v>0.0289209788221949</v>
       </c>
       <c r="E20" s="16" t="n">
-        <f aca="false">4/$D$3</f>
-        <v>0.0043956043956044</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F20" s="15" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="G20" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H20" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.281553398058252</v>
       </c>
       <c r="I20" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J20" s="15" t="n">
-        <v>0.44017094017094</v>
+        <v>0.452674897119342</v>
       </c>
       <c r="K20" s="16" t="n">
-        <f aca="false">9/$J$3</f>
-        <v>0.037037037037037</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L20" s="15" t="n">
-        <v>0.649741824440619</v>
+        <v>0.656652360515021</v>
       </c>
       <c r="M20" s="16" t="n">
-        <f aca="false">3/$L$3</f>
-        <v>0.00257510729613734</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N20" s="15" t="n">
         <v>0.55</v>
@@ -5158,37 +5254,37 @@
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P20" s="23" t="n">
-        <v>0.0263546139456426</v>
+      <c r="P20" s="22" t="n">
+        <v>0.0450466025027233</v>
       </c>
       <c r="Q20" s="15" t="n">
-        <v>0.384891506009518</v>
-      </c>
-      <c r="R20" s="24" t="n">
-        <v>0.08</v>
+        <v>1.17910447761194</v>
+      </c>
+      <c r="R20" s="23" t="n">
+        <v>0.135</v>
       </c>
       <c r="S20" s="16" t="n">
-        <f aca="false">80/$P$3</f>
-        <v>0.04</v>
+        <f aca="false">1829/$P$3</f>
+        <v>0.9145</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>35</v>
+        <v>64</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(D21,F21,H21,J21,L21,N21)</f>
-        <v>0.405257833604129</v>
+        <v>0.479783624027799</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>-0.0714529452409867</v>
+        <v>0.369274416448439</v>
       </c>
       <c r="E21" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">4/$D$3</f>
+        <v>0.0043956043956044</v>
       </c>
       <c r="F21" s="15" t="n">
         <v>0.52</v>
@@ -5198,110 +5294,177 @@
         <v>0</v>
       </c>
       <c r="H21" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I21" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J21" s="15" t="n">
-        <v>0.469135802469136</v>
+        <v>0.44017094017094</v>
       </c>
       <c r="K21" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">9/$J$3</f>
+        <v>0.037037037037037</v>
       </c>
       <c r="L21" s="15" t="n">
-        <v>0.618556701030928</v>
+        <v>0.649741824440619</v>
       </c>
       <c r="M21" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">3/$L$3</f>
+        <v>0.00257510729613734</v>
       </c>
       <c r="N21" s="15" t="n">
-        <v>0.516666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="O21" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P21" s="23" t="n">
-        <v>0.018613476307488</v>
+      <c r="P21" s="22" t="n">
+        <v>0.0263546139456426</v>
       </c>
       <c r="Q21" s="15" t="n">
-        <v>1.12997748971513</v>
-      </c>
-      <c r="R21" s="24" t="n">
-        <v>0.116</v>
+        <v>0.384891506009518</v>
+      </c>
+      <c r="R21" s="23" t="n">
+        <v>0.08</v>
       </c>
       <c r="S21" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">80/$P$3</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C22" s="14" t="n">
         <f aca="false">AVERAGE(D22,F22,H22,J22,L22,N22)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G22" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="15" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I22" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="15" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K22" s="16" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="15" t="n">
+        <v>0.618556701030928</v>
+      </c>
+      <c r="M22" s="16" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N22" s="15" t="n">
+        <v>0.516666666666667</v>
+      </c>
+      <c r="O22" s="16" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="22" t="n">
+        <v>0.018613476307488</v>
+      </c>
+      <c r="Q22" s="15" t="n">
+        <v>1.12997748971513</v>
+      </c>
+      <c r="R22" s="23" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="S22" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="n">
+        <f aca="false">AVERAGE(D23,F23,H23,J23,L23,N23)</f>
         <v>0.364587789621774</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D23" s="15" t="n">
         <v>0.0266825503923221</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E23" s="16" t="n">
         <f aca="false">187/$D$3</f>
         <v>0.205494505494505</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F23" s="15" t="n">
         <v>0.461538461538462</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G23" s="16" t="n">
         <f aca="false">9/$F$3</f>
         <v>0.09</v>
       </c>
-      <c r="H22" s="15" t="n">
+      <c r="H23" s="15" t="n">
         <v>0.237113402061856</v>
       </c>
-      <c r="I22" s="16" t="n">
+      <c r="I23" s="16" t="n">
         <f aca="false">6/$H$3</f>
         <v>0.058252427184466</v>
       </c>
-      <c r="J22" s="15" t="n">
+      <c r="J23" s="15" t="n">
         <v>0.558823529411765</v>
       </c>
-      <c r="K22" s="16" t="n">
+      <c r="K23" s="16" t="n">
         <f aca="false">39/$J$3</f>
         <v>0.160493827160494</v>
       </c>
-      <c r="L22" s="15" t="n">
+      <c r="L23" s="15" t="n">
         <v>0.403368794326241</v>
       </c>
-      <c r="M22" s="16" t="n">
+      <c r="M23" s="16" t="n">
         <f aca="false">37/$L$3</f>
         <v>0.0317596566523605</v>
       </c>
-      <c r="N22" s="15" t="n">
+      <c r="N23" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="O22" s="16" t="n">
+      <c r="O23" s="16" t="n">
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="P22" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="15" t="n">
+      <c r="P23" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="15" t="n">
         <v>1.02530466506249</v>
       </c>
-      <c r="R22" s="24" t="n">
+      <c r="R23" s="23" t="n">
         <v>0.544</v>
       </c>
-      <c r="S22" s="16" t="n">
+      <c r="S23" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
@@ -5323,8 +5486,8 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="S4:S22 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
+  <conditionalFormatting sqref="S4:S23 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5388,7 +5551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P22">
+  <conditionalFormatting sqref="P4:P23">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -5421,12 +5584,13 @@
     <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
     <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
     <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B21" r:id="rId18" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B22" r:id="rId19" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B22" r:id="rId19" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B23" r:id="rId20" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5435,7 +5599,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <drawing r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eval llama 3.3 70b results
</commit_message>
<xml_diff>
--- a/LLM_Eval.xlsx
+++ b/LLM_Eval.xlsx
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'GLUE Results'!$A$3:$X$48</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'HuLU Results'!$A$3:$S$47</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'VerbGrammar Results'!$A$3:$F$10</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'VerbGrammar Results'!$A$3:$F$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="75">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://huggingface.co/bartowski/gemma-2-27b-it-GGUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llama-3.3-70B-Instruct-Q2_K.gguf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://huggingface.co/unsloth/Llama-3.3-70B-Instruct-GGUF</t>
   </si>
   <si>
     <t xml:space="preserve">gemma-2-9b-it-Q6_K_L.gguf</t>
@@ -702,7 +708,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="167">
+  <dxfs count="171">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -913,6 +919,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFA4A168"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFA7A068"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1041,6 +1055,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF7BBA66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF83B566"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1129,6 +1151,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF79BB66"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF7ABA66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1505,7 +1535,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF79BB66"/>
+          <fgColor rgb="FF79BA66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1546,14 +1576,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFC58E6A"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7BBA66"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1813,14 +1835,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF93AB67"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF8EAE67"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1829,6 +1843,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFA0A468"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFA99F68"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -1958,6 +1980,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF88B366"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8AB166"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2042,6 +2072,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFEA796B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3746C"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2236,7 +2274,7 @@
   <dimension ref="A1:X48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2342,7 +2380,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -2659,80 +2697,80 @@
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">AVERAGE(W7,T7:U7,R7,P7,N7,M7,K7,H7,I7,F7,D7)</f>
-        <v>0.779541622537469</v>
+        <v>0.788062668883991</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0.592121670308154</v>
+        <v>0.487457290708985</v>
       </c>
       <c r="E7" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.351299032093734</v>
+        <v>0.438920020376974</v>
       </c>
       <c r="G7" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>0.767156862745098</v>
+        <v>0.825980392156863</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.816955684007707</v>
+        <v>0.874336283185841</v>
       </c>
       <c r="J7" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>0.894197327475746</v>
+        <v>0.891268533772652</v>
       </c>
       <c r="L7" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.814914667326243</v>
+        <v>0.829581993569132</v>
       </c>
       <c r="N7" s="15" t="n">
-        <v>0.772172324554727</v>
+        <v>0.786488999070344</v>
       </c>
       <c r="O7" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P7" s="15" t="n">
-        <v>0.88086642599278</v>
+        <v>0.819494584837545</v>
       </c>
       <c r="Q7" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R7" s="15" t="n">
-        <v>0.942660550458716</v>
+        <v>0.950688073394496</v>
       </c>
       <c r="S7" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T7" s="15" t="n">
-        <v>0.85733495291754</v>
+        <v>0.863680137923041</v>
       </c>
       <c r="U7" s="15" t="n">
-        <v>0.876087578202987</v>
+        <v>0.871954309161318</v>
       </c>
       <c r="V7" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W7" s="15" t="n">
-        <v>0.788732394366197</v>
+        <v>0.816901408450704</v>
       </c>
       <c r="X7" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2748,75 +2786,75 @@
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(W8,T8:U8,R8,P8,N8,M8,K8,H8,I8,F8,D8)</f>
-        <v>0.761759832782204</v>
+        <v>0.779541622537469</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.597514874790058</v>
+        <v>0.592121670308154</v>
       </c>
       <c r="E8" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.478247580234335</v>
+        <v>0.351299032093734</v>
       </c>
       <c r="G8" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.757352941176471</v>
+        <v>0.767156862745098</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>0.834170854271357</v>
+        <v>0.816955684007707</v>
       </c>
       <c r="J8" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>0.767975055025679</v>
+        <v>0.894197327475746</v>
       </c>
       <c r="L8" s="16" t="n">
-        <f aca="false">11/$K$3</f>
-        <v>0.00201354567087681</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.824560969577047</v>
+        <v>0.814914667326243</v>
       </c>
       <c r="N8" s="15" t="n">
-        <v>0.785041064339182</v>
+        <v>0.772172324554727</v>
       </c>
       <c r="O8" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P8" s="15" t="n">
-        <v>0.746376811594203</v>
+        <v>0.88086642599278</v>
       </c>
       <c r="Q8" s="16" t="n">
-        <f aca="false">1/$P$3</f>
-        <v>0.0036101083032491</v>
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
       </c>
       <c r="R8" s="15" t="n">
-        <v>0.95752009184845</v>
+        <v>0.942660550458716</v>
       </c>
       <c r="S8" s="16" t="n">
-        <f aca="false">1/$R$3</f>
-        <v>0.00114678899082569</v>
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
       </c>
       <c r="T8" s="15" t="n">
-        <v>0.87058607341487</v>
+        <v>0.85733495291754</v>
       </c>
       <c r="U8" s="15" t="n">
-        <v>0.873884353171137</v>
+        <v>0.876087578202987</v>
       </c>
       <c r="V8" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W8" s="15" t="n">
-        <v>0.647887323943662</v>
+        <v>0.788732394366197</v>
       </c>
       <c r="X8" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2832,75 +2870,75 @@
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">AVERAGE(W9,T9:U9,R9,P9,N9,M9,K9,H9,I9,F9,D9)</f>
-        <v>0.740393758714782</v>
+        <v>0.761759832782204</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.526754313381707</v>
+        <v>0.597514874790058</v>
       </c>
       <c r="E9" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>0.418644931227713</v>
+        <v>0.478247580234335</v>
       </c>
       <c r="G9" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.737745098039216</v>
+        <v>0.757352941176471</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.820770519262982</v>
+        <v>0.834170854271357</v>
       </c>
       <c r="J9" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>0.833424858136555</v>
+        <v>0.767975055025679</v>
       </c>
       <c r="L9" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">11/$K$3</f>
+        <v>0.00201354567087681</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.765767994063814</v>
+        <v>0.824560969577047</v>
       </c>
       <c r="N9" s="15" t="n">
-        <v>0.742172610944732</v>
+        <v>0.785041064339182</v>
       </c>
       <c r="O9" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P9" s="15" t="n">
-        <v>0.84115523465704</v>
+        <v>0.746376811594203</v>
       </c>
       <c r="Q9" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">1/$P$3</f>
+        <v>0.0036101083032491</v>
       </c>
       <c r="R9" s="15" t="n">
-        <v>0.940366972477064</v>
+        <v>0.95752009184845</v>
       </c>
       <c r="S9" s="16" t="n">
-        <f aca="false">0/$R$3</f>
-        <v>0</v>
+        <f aca="false">1/$R$3</f>
+        <v>0.00114678899082569</v>
       </c>
       <c r="T9" s="15" t="n">
-        <v>0.767106912789686</v>
+        <v>0.87058607341487</v>
       </c>
       <c r="U9" s="15" t="n">
-        <v>0.772505800441942</v>
+        <v>0.873884353171137</v>
       </c>
       <c r="V9" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W9" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.647887323943662</v>
       </c>
       <c r="X9" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -2916,75 +2954,75 @@
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">AVERAGE(W10,T10:U10,R10,P10,N10,M10,K10,H10,I10,F10,D10)</f>
-        <v>0.728207755738953</v>
+        <v>0.740393758714782</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.417240141074992</v>
+        <v>0.526754313381707</v>
       </c>
       <c r="E10" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.315944982170148</v>
+        <v>0.418644931227713</v>
       </c>
       <c r="G10" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.779411764705882</v>
+        <v>0.737745098039216</v>
       </c>
       <c r="I10" s="15" t="n">
-        <v>0.84375</v>
+        <v>0.820770519262982</v>
       </c>
       <c r="J10" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K10" s="15" t="n">
-        <v>0.733088909257562</v>
+        <v>0.833424858136555</v>
       </c>
       <c r="L10" s="16" t="n">
-        <f aca="false">8/$K$3</f>
-        <v>0.00146439685154677</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M10" s="15" t="n">
-        <v>0.814964135542914</v>
+        <v>0.765767994063814</v>
       </c>
       <c r="N10" s="15" t="n">
-        <v>0.753954941621444</v>
+        <v>0.742172610944732</v>
       </c>
       <c r="O10" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P10" s="15" t="n">
-        <v>0.707581227436823</v>
+        <v>0.84115523465704</v>
       </c>
       <c r="Q10" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R10" s="15" t="n">
-        <v>0.907110091743119</v>
+        <v>0.940366972477064</v>
       </c>
       <c r="S10" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T10" s="15" t="n">
-        <v>0.817610857364514</v>
+        <v>0.767106912789686</v>
       </c>
       <c r="U10" s="15" t="n">
-        <v>0.830934609499328</v>
+        <v>0.772505800441942</v>
       </c>
       <c r="V10" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W10" s="15" t="n">
-        <v>0.816901408450704</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X10" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3000,75 +3038,75 @@
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">AVERAGE(W11,T11:U11,R11,P11,N11,M11,K11,H11,I11,F11,D11)</f>
-        <v>0.723374373278101</v>
+        <v>0.728207755738953</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>0.451542212782268</v>
+        <v>0.417240141074992</v>
       </c>
       <c r="E11" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F11" s="15" t="n">
-        <v>0.462964849719817</v>
+        <v>0.315944982170148</v>
       </c>
       <c r="G11" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H11" s="15" t="n">
-        <v>0.801470588235294</v>
+        <v>0.779411764705882</v>
       </c>
       <c r="I11" s="15" t="n">
-        <v>0.850828729281768</v>
+        <v>0.84375</v>
       </c>
       <c r="J11" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K11" s="15" t="n">
-        <v>0.8555738605162</v>
+        <v>0.733088909257562</v>
       </c>
       <c r="L11" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
       </c>
       <c r="M11" s="15" t="n">
-        <v>0.822681177343557</v>
+        <v>0.814964135542914</v>
       </c>
       <c r="N11" s="15" t="n">
-        <v>0.777062536928196</v>
+        <v>0.753954941621444</v>
       </c>
       <c r="O11" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P11" s="15" t="n">
-        <v>0.317689530685921</v>
+        <v>0.707581227436823</v>
       </c>
       <c r="Q11" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R11" s="15" t="n">
-        <v>0.951834862385321</v>
+        <v>0.907110091743119</v>
       </c>
       <c r="S11" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T11" s="15" t="n">
-        <v>0.831672916702132</v>
+        <v>0.817610857364514</v>
       </c>
       <c r="U11" s="15" t="n">
-        <v>0.838861355601802</v>
+        <v>0.830934609499328</v>
       </c>
       <c r="V11" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W11" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.816901408450704</v>
       </c>
       <c r="X11" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3084,75 +3122,75 @@
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(W12,T12:U12,R12,P12,N12,M12,K12,H12,I12,F12,D12)</f>
-        <v>0.71588881644893</v>
+        <v>0.723374373278101</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>0.618527281006798</v>
+        <v>0.451542212782268</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F12" s="15" t="n">
-        <v>0.388588894549159</v>
+        <v>0.462964849719817</v>
       </c>
       <c r="G12" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H12" s="15" t="n">
-        <v>0.754901960784314</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I12" s="15" t="n">
-        <v>0.841269841269841</v>
+        <v>0.850828729281768</v>
       </c>
       <c r="J12" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K12" s="15" t="n">
-        <v>0.468423942888523</v>
+        <v>0.8555738605162</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M12" s="15" t="n">
-        <v>0.804551075933713</v>
+        <v>0.822681177343557</v>
       </c>
       <c r="N12" s="15" t="n">
-        <v>0.772224143894846</v>
+        <v>0.777062536928196</v>
       </c>
       <c r="O12" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P12" s="15" t="n">
-        <v>0.407942238267148</v>
+        <v>0.317689530685921</v>
       </c>
       <c r="Q12" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R12" s="15" t="n">
-        <v>0.939220183486239</v>
+        <v>0.951834862385321</v>
       </c>
       <c r="S12" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T12" s="15" t="n">
-        <v>0.878811589487953</v>
+        <v>0.831672916702132</v>
       </c>
       <c r="U12" s="15" t="n">
-        <v>0.885218730325664</v>
+        <v>0.838861355601802</v>
       </c>
       <c r="V12" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W12" s="15" t="n">
-        <v>0.830985915492958</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X12" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3168,75 +3206,75 @@
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(W13,T13:U13,R13,P13,N13,M13,K13,H13,I13,F13,D13)</f>
-        <v>0.704245669484917</v>
+        <v>0.71588881644893</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.61400038680535</v>
+        <v>0.618527281006798</v>
       </c>
       <c r="E13" s="16" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.417524197656648</v>
+        <v>0.388588894549159</v>
       </c>
       <c r="G13" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.742647058823529</v>
+        <v>0.754901960784314</v>
       </c>
       <c r="I13" s="15" t="n">
-        <v>0.837209302325581</v>
+        <v>0.841269841269841</v>
       </c>
       <c r="J13" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K13" s="15" t="n">
-        <v>0.317480719794344</v>
+        <v>0.468423942888523</v>
       </c>
       <c r="L13" s="16" t="n">
-        <f aca="false">17/$K$3</f>
-        <v>0.00311184330953688</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M13" s="15" t="n">
-        <v>0.720652980460054</v>
+        <v>0.804551075933713</v>
       </c>
       <c r="N13" s="15" t="n">
-        <v>0.719543084181773</v>
+        <v>0.772224143894846</v>
       </c>
       <c r="O13" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P13" s="15" t="n">
-        <v>0.68231046931408</v>
+        <v>0.407942238267148</v>
       </c>
       <c r="Q13" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R13" s="15" t="n">
-        <v>0.935779816513762</v>
+        <v>0.939220183486239</v>
       </c>
       <c r="S13" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T13" s="15" t="n">
-        <v>0.860305870097761</v>
+        <v>0.878811589487953</v>
       </c>
       <c r="U13" s="15" t="n">
-        <v>0.871099781648942</v>
+        <v>0.885218730325664</v>
       </c>
       <c r="V13" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W13" s="15" t="n">
-        <v>0.732394366197183</v>
+        <v>0.830985915492958</v>
       </c>
       <c r="X13" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3252,75 +3290,75 @@
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(W14,T14:U14,R14,P14,N14,M14,K14,H14,I14,F14,D14)</f>
-        <v>0.699391112337297</v>
+        <v>0.704245669484917</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>0.625980868840778</v>
+        <v>0.61400038680535</v>
       </c>
       <c r="E14" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F14" s="15" t="n">
-        <v>0.37493632195619</v>
+        <v>0.417524197656648</v>
       </c>
       <c r="G14" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.801470588235294</v>
+        <v>0.742647058823529</v>
       </c>
       <c r="I14" s="15" t="n">
-        <v>0.86522462562396</v>
+        <v>0.837209302325581</v>
       </c>
       <c r="J14" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K14" s="15" t="n">
-        <v>0.438496791934006</v>
+        <v>0.317480719794344</v>
       </c>
       <c r="L14" s="16" t="n">
-        <f aca="false">8/$K$3</f>
-        <v>0.00146439685154677</v>
+        <f aca="false">17/$K$3</f>
+        <v>0.00311184330953688</v>
       </c>
       <c r="M14" s="15" t="n">
-        <v>0.852128527963984</v>
+        <v>0.720652980460054</v>
       </c>
       <c r="N14" s="15" t="n">
-        <v>0.805846053913608</v>
+        <v>0.719543084181773</v>
       </c>
       <c r="O14" s="16" t="n">
-        <f aca="false">3/$M$3</f>
-        <v>7.42023250061835E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P14" s="15" t="n">
-        <v>0.133574007220217</v>
+        <v>0.68231046931408</v>
       </c>
       <c r="Q14" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R14" s="15" t="n">
-        <v>0.930045871559633</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S14" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T14" s="15" t="n">
-        <v>0.886137481283129</v>
+        <v>0.860305870097761</v>
       </c>
       <c r="U14" s="15" t="n">
-        <v>0.890119815150565</v>
+        <v>0.871099781648942</v>
       </c>
       <c r="V14" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W14" s="15" t="n">
-        <v>0.788732394366197</v>
+        <v>0.732394366197183</v>
       </c>
       <c r="X14" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3336,75 +3374,75 @@
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(W15,T15:U15,R15,P15,N15,M15,K15,H15,I15,F15,D15)</f>
-        <v>0.658513623474907</v>
+        <v>0.699391112337297</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>0.523854029130735</v>
+        <v>0.625980868840778</v>
       </c>
       <c r="E15" s="16" t="n">
-        <f aca="false">3/$D$3</f>
-        <v>0.00287631831255992</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.480334216425515</v>
+        <v>0.37493632195619</v>
       </c>
       <c r="G15" s="16" t="n">
-        <f aca="false">1/$F$3</f>
-        <v>0.000101884870096791</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.727941176470588</v>
+        <v>0.801470588235294</v>
       </c>
       <c r="I15" s="15" t="n">
-        <v>0.821829855537721</v>
+        <v>0.86522462562396</v>
       </c>
       <c r="J15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K15" s="15" t="n">
-        <v>0.696448187477115</v>
+        <v>0.438496791934006</v>
       </c>
       <c r="L15" s="16" t="n">
-        <f aca="false">1/$K$3</f>
-        <v>0.000183049606443346</v>
+        <f aca="false">8/$K$3</f>
+        <v>0.00146439685154677</v>
       </c>
       <c r="M15" s="15" t="n">
-        <v>0.509271935283136</v>
+        <v>0.852128527963984</v>
       </c>
       <c r="N15" s="15" t="n">
-        <v>0.593278732490252</v>
+        <v>0.805846053913608</v>
       </c>
       <c r="O15" s="16" t="n">
-        <f aca="false">255/$M$3</f>
-        <v>0.0063071976255256</v>
+        <f aca="false">3/$M$3</f>
+        <v>7.42023250061835E-005</v>
       </c>
       <c r="P15" s="15" t="n">
-        <v>0.249097472924188</v>
+        <v>0.133574007220217</v>
       </c>
       <c r="Q15" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R15" s="15" t="n">
-        <v>0.934633027522936</v>
+        <v>0.930045871559633</v>
       </c>
       <c r="S15" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T15" s="15" t="n">
-        <v>0.821663265900952</v>
+        <v>0.886137481283129</v>
       </c>
       <c r="U15" s="15" t="n">
-        <v>0.825501723380821</v>
+        <v>0.890119815150565</v>
       </c>
       <c r="V15" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W15" s="15" t="n">
-        <v>0.71830985915493</v>
+        <v>0.788732394366197</v>
       </c>
       <c r="X15" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3420,68 +3458,68 @@
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(W16,T16:U16,R16,P16,N16,M16,K16,H16,I16,F16,D16)</f>
-        <v>0.653779197430066</v>
+        <v>0.658513623474907</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>0.455627237079107</v>
+        <v>0.523854029130735</v>
       </c>
       <c r="E16" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">3/$D$3</f>
+        <v>0.00287631831255992</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.386958736627611</v>
+        <v>0.480334216425515</v>
       </c>
       <c r="G16" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">1/$F$3</f>
+        <v>0.000101884870096791</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.754901960784314</v>
+        <v>0.727941176470588</v>
       </c>
       <c r="I16" s="15" t="n">
-        <v>0.835526315789474</v>
+        <v>0.821829855537721</v>
       </c>
       <c r="J16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K16" s="15" t="n">
-        <v>0.136371956800293</v>
+        <v>0.696448187477115</v>
       </c>
       <c r="L16" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">1/$K$3</f>
+        <v>0.000183049606443346</v>
       </c>
       <c r="M16" s="15" t="n">
-        <v>0.82352213702696</v>
+        <v>0.509271935283136</v>
       </c>
       <c r="N16" s="15" t="n">
-        <v>0.77733046219143</v>
+        <v>0.593278732490252</v>
       </c>
       <c r="O16" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
+        <f aca="false">255/$M$3</f>
+        <v>0.0063071976255256</v>
       </c>
       <c r="P16" s="15" t="n">
-        <v>0.353790613718412</v>
+        <v>0.249097472924188</v>
       </c>
       <c r="Q16" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R16" s="15" t="n">
-        <v>0.935779816513762</v>
+        <v>0.934633027522936</v>
       </c>
       <c r="S16" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T16" s="15" t="n">
-        <v>0.826388381403035</v>
+        <v>0.821663265900952</v>
       </c>
       <c r="U16" s="15" t="n">
-        <v>0.840842892071465</v>
+        <v>0.825501723380821</v>
       </c>
       <c r="V16" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3504,75 +3542,75 @@
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">AVERAGE(W17,T17:U17,R17,P17,N17,M17,K17,H17,I17,F17,D17)</f>
-        <v>0.64108637065082</v>
+        <v>0.653779197430066</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>0.531920773750409</v>
+        <v>0.455627237079107</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F17" s="15" t="n">
-        <v>0.42985226693836</v>
+        <v>0.386958736627611</v>
       </c>
       <c r="G17" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H17" s="15" t="n">
-        <v>0.705882352941177</v>
+        <v>0.754901960784314</v>
       </c>
       <c r="I17" s="15" t="n">
-        <v>0.82089552238806</v>
+        <v>0.835526315789474</v>
       </c>
       <c r="J17" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K17" s="15" t="n">
-        <v>0.540377220289324</v>
+        <v>0.136371956800293</v>
       </c>
       <c r="L17" s="16" t="n">
-        <f aca="false">2/$K$3</f>
-        <v>0.000366099212886692</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M17" s="15" t="n">
-        <v>0.80123670541677</v>
+        <v>0.82352213702696</v>
       </c>
       <c r="N17" s="15" t="n">
-        <v>0.772955868226253</v>
+        <v>0.77733046219143</v>
       </c>
       <c r="O17" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P17" s="15" t="n">
-        <v>0.296028880866426</v>
+        <v>0.353790613718412</v>
       </c>
       <c r="Q17" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R17" s="15" t="n">
-        <v>0.928899082568807</v>
+        <v>0.935779816513762</v>
       </c>
       <c r="S17" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T17" s="15" t="n">
-        <v>0.621129369842947</v>
+        <v>0.826388381403035</v>
       </c>
       <c r="U17" s="15" t="n">
-        <v>0.666393615848911</v>
+        <v>0.840842892071465</v>
       </c>
       <c r="V17" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W17" s="15" t="n">
-        <v>0.577464788732394</v>
+        <v>0.71830985915493</v>
       </c>
       <c r="X17" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3588,68 +3626,68 @@
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">AVERAGE(W18,T18:U18,R18,P18,N18,M18,K18,H18,I18,F18,D18)</f>
-        <v>0.623563086724128</v>
+        <v>0.64108637065082</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>0.477381210215107</v>
+        <v>0.531920773750409</v>
       </c>
       <c r="E18" s="16" t="n">
         <f aca="false">1/$D$3</f>
         <v>0.000958772770853308</v>
       </c>
       <c r="F18" s="15" t="n">
-        <v>0.286907794192562</v>
+        <v>0.42985226693836</v>
       </c>
       <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H18" s="15" t="n">
-        <v>0.723039215686275</v>
+        <v>0.705882352941177</v>
       </c>
       <c r="I18" s="15" t="n">
-        <v>0.804835924006909</v>
+        <v>0.82089552238806</v>
       </c>
       <c r="J18" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K18" s="15" t="n">
-        <v>0.409992652461425</v>
+        <v>0.540377220289324</v>
       </c>
       <c r="L18" s="16" t="n">
-        <f aca="false">19/$K$3</f>
-        <v>0.00347794252242358</v>
+        <f aca="false">2/$K$3</f>
+        <v>0.000366099212886692</v>
       </c>
       <c r="M18" s="15" t="n">
-        <v>0.750581251545882</v>
+        <v>0.80123670541677</v>
       </c>
       <c r="N18" s="15" t="n">
-        <v>0.721851381916478</v>
+        <v>0.772955868226253</v>
       </c>
       <c r="O18" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P18" s="15" t="n">
-        <v>0.245487364620939</v>
+        <v>0.296028880866426</v>
       </c>
       <c r="Q18" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R18" s="15" t="n">
-        <v>0.870412844036697</v>
+        <v>0.928899082568807</v>
       </c>
       <c r="S18" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T18" s="15" t="n">
-        <v>0.810628242029225</v>
+        <v>0.621129369842947</v>
       </c>
       <c r="U18" s="15" t="n">
-        <v>0.80417437124564</v>
+        <v>0.666393615848911</v>
       </c>
       <c r="V18" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3672,68 +3710,68 @@
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(W19,T19:U19,R19,P19,N19,M19,K19,H19,I19,F19,D19)</f>
-        <v>0.613554278796799</v>
+        <v>0.623563086724128</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.375051720670997</v>
+        <v>0.477381210215107</v>
       </c>
       <c r="E19" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F19" s="15" t="n">
-        <v>0.538767193071829</v>
+        <v>0.286907794192562</v>
       </c>
       <c r="G19" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.730392156862745</v>
+        <v>0.723039215686275</v>
       </c>
       <c r="I19" s="15" t="n">
-        <v>0.827044025157233</v>
+        <v>0.804835924006909</v>
       </c>
       <c r="J19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K19" s="15" t="n">
-        <v>0.557386051619989</v>
+        <v>0.409992652461425</v>
       </c>
       <c r="L19" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">19/$K$3</f>
+        <v>0.00347794252242358</v>
       </c>
       <c r="M19" s="15" t="n">
-        <v>0.608706406134059</v>
+        <v>0.750581251545882</v>
       </c>
       <c r="N19" s="15" t="n">
-        <v>0.625189537528431</v>
+        <v>0.721851381916478</v>
       </c>
       <c r="O19" s="16" t="n">
         <f aca="false">0/$M$3</f>
         <v>0</v>
       </c>
       <c r="P19" s="15" t="n">
-        <v>0.425992779783394</v>
+        <v>0.245487364620939</v>
       </c>
       <c r="Q19" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R19" s="15" t="n">
-        <v>0.932339449541284</v>
+        <v>0.870412844036697</v>
       </c>
       <c r="S19" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T19" s="15" t="n">
-        <v>0.573663619974553</v>
+        <v>0.810628242029225</v>
       </c>
       <c r="U19" s="15" t="n">
-        <v>0.590653616484677</v>
+        <v>0.80417437124564</v>
       </c>
       <c r="V19" s="16" t="n">
         <f aca="false">0/$T$3</f>
@@ -3756,75 +3794,75 @@
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(W20,T20:U20,R20,P20,N20,M20,K20,H20,I20,F20,D20)</f>
-        <v>0.588337454921144</v>
+        <v>0.613554278796799</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>0.275218494690191</v>
+        <v>0.375051720670997</v>
       </c>
       <c r="E20" s="16" t="n">
-        <f aca="false">1/$D$3</f>
-        <v>0.000958772770853308</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F20" s="15" t="n">
-        <v>0.256342333163525</v>
+        <v>0.538767193071829</v>
       </c>
       <c r="G20" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H20" s="15" t="n">
-        <v>0.718137254901961</v>
+        <v>0.730392156862745</v>
       </c>
       <c r="I20" s="15" t="n">
-        <v>0.822804314329738</v>
+        <v>0.827044025157233</v>
       </c>
       <c r="J20" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K20" s="15" t="n">
-        <v>0.33260113490756</v>
+        <v>0.557386051619989</v>
       </c>
       <c r="L20" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M20" s="15" t="n">
-        <v>0.730112793113684</v>
+        <v>0.608706406134059</v>
       </c>
       <c r="N20" s="15" t="n">
-        <v>0.707110836711137</v>
+        <v>0.625189537528431</v>
       </c>
       <c r="O20" s="16" t="n">
-        <f aca="false">2/$M$3</f>
-        <v>4.9468216670789E-005</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
       </c>
       <c r="P20" s="15" t="n">
-        <v>0.339350180505415</v>
+        <v>0.425992779783394</v>
       </c>
       <c r="Q20" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R20" s="15" t="n">
-        <v>0.918577981651376</v>
+        <v>0.932339449541284</v>
       </c>
       <c r="S20" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T20" s="15" t="n">
-        <v>0.730177716008711</v>
+        <v>0.573663619974553</v>
       </c>
       <c r="U20" s="15" t="n">
-        <v>0.750743179633811</v>
+        <v>0.590653616484677</v>
       </c>
       <c r="V20" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W20" s="15" t="n">
-        <v>0.47887323943662</v>
+        <v>0.577464788732394</v>
       </c>
       <c r="X20" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3835,80 +3873,80 @@
       <c r="A21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(W21,T21:U21,R21,P21,N21,M21,K21,H21,I21,F21,D21)</f>
-        <v>0.573931674979746</v>
+        <v>0.588337454921144</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>0.486972221108263</v>
+        <v>0.275218494690191</v>
       </c>
       <c r="E21" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">1/$D$3</f>
+        <v>0.000958772770853308</v>
       </c>
       <c r="F21" s="15" t="n">
-        <v>0.23555781966378</v>
+        <v>0.256342333163525</v>
       </c>
       <c r="G21" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H21" s="15" t="n">
-        <v>0.723039215686275</v>
+        <v>0.718137254901961</v>
       </c>
       <c r="I21" s="15" t="n">
-        <v>0.81505728314239</v>
+        <v>0.822804314329738</v>
       </c>
       <c r="J21" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K21" s="15" t="n">
-        <v>0.357678930990298</v>
+        <v>0.33260113490756</v>
       </c>
       <c r="L21" s="16" t="n">
         <f aca="false">0/$K$3</f>
         <v>0</v>
       </c>
       <c r="M21" s="15" t="n">
-        <v>0.671671696432989</v>
+        <v>0.730112793113684</v>
       </c>
       <c r="N21" s="15" t="n">
-        <v>0.656291270683896</v>
+        <v>0.707110836711137</v>
       </c>
       <c r="O21" s="16" t="n">
-        <f aca="false">4/$M$3</f>
-        <v>9.8936433341578E-005</v>
+        <f aca="false">2/$M$3</f>
+        <v>4.9468216670789E-005</v>
       </c>
       <c r="P21" s="15" t="n">
-        <v>0.306859205776173</v>
+        <v>0.339350180505415</v>
       </c>
       <c r="Q21" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R21" s="15" t="n">
-        <v>0.815366972477064</v>
+        <v>0.918577981651376</v>
       </c>
       <c r="S21" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T21" s="15" t="n">
-        <v>0.662651642860851</v>
+        <v>0.730177716008711</v>
       </c>
       <c r="U21" s="15" t="n">
-        <v>0.64899158741385</v>
+        <v>0.750743179633811</v>
       </c>
       <c r="V21" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W21" s="15" t="n">
-        <v>0.507042253521127</v>
+        <v>0.47887323943662</v>
       </c>
       <c r="X21" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -3924,48 +3962,48 @@
       </c>
       <c r="C22" s="14" t="n">
         <f aca="false">AVERAGE(W22,T22:U22,R22,P22,N22,M22,K22,H22,I22,F22,D22)</f>
-        <v>0.499454443668613</v>
+        <v>0.573931674979746</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>0.333471865271531</v>
+        <v>0.486972221108263</v>
       </c>
       <c r="E22" s="16" t="n">
-        <f aca="false">6/$D$3</f>
-        <v>0.00575263662511985</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F22" s="15" t="n">
-        <v>0.292103922567499</v>
+        <v>0.23555781966378</v>
       </c>
       <c r="G22" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H22" s="15" t="n">
-        <v>0.698529411764706</v>
+        <v>0.723039215686275</v>
       </c>
       <c r="I22" s="15" t="n">
-        <v>0.805687203791469</v>
+        <v>0.81505728314239</v>
       </c>
       <c r="J22" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K22" s="15" t="n">
-        <v>0.391434449223864</v>
+        <v>0.357678930990298</v>
       </c>
       <c r="L22" s="16" t="n">
-        <f aca="false">116/$K$3</f>
-        <v>0.0212337543474282</v>
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
       </c>
       <c r="M22" s="15" t="n">
-        <v>0.691602220900258</v>
+        <v>0.671671696432989</v>
       </c>
       <c r="N22" s="15" t="n">
-        <v>0.36669042044182</v>
+        <v>0.656291270683896</v>
       </c>
       <c r="O22" s="16" t="n">
-        <f aca="false">86/$M$3</f>
-        <v>0.00212713331684393</v>
+        <f aca="false">4/$M$3</f>
+        <v>9.8936433341578E-005</v>
       </c>
       <c r="P22" s="15" t="n">
         <v>0.306859205776173</v>
@@ -3975,24 +4013,24 @@
         <v>0</v>
       </c>
       <c r="R22" s="15" t="n">
-        <v>0.855504587155963</v>
+        <v>0.815366972477064</v>
       </c>
       <c r="S22" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
       <c r="T22" s="15" t="n">
-        <v>0.370306926073738</v>
+        <v>0.662651642860851</v>
       </c>
       <c r="U22" s="15" t="n">
-        <v>0.402389871619712</v>
+        <v>0.64899158741385</v>
       </c>
       <c r="V22" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
       <c r="W22" s="15" t="n">
-        <v>0.47887323943662</v>
+        <v>0.507042253521127</v>
       </c>
       <c r="X22" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -4008,75 +4046,75 @@
       </c>
       <c r="C23" s="14" t="n">
         <f aca="false">AVERAGE(W23,T23:U23,R23,P23,N23,M23,K23,H23,I23,F23,D23)</f>
-        <v>0.457777805523234</v>
+        <v>0.499454443668613</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>0</v>
+        <v>0.333471865271531</v>
       </c>
       <c r="E23" s="16" t="n">
-        <f aca="false">12/$D$3</f>
-        <v>0.0115052732502397</v>
+        <f aca="false">6/$D$3</f>
+        <v>0.00575263662511985</v>
       </c>
       <c r="F23" s="15" t="n">
-        <v>0.31758314125782</v>
+        <v>0.292103922567499</v>
       </c>
       <c r="G23" s="16" t="n">
-        <f aca="false">3741/$F$3</f>
-        <v>0.381151299032094</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H23" s="15" t="n">
-        <v>0.679389312977099</v>
+        <v>0.698529411764706</v>
       </c>
       <c r="I23" s="15" t="n">
-        <v>0.809090909090909</v>
+        <v>0.805687203791469</v>
       </c>
       <c r="J23" s="16" t="n">
-        <f aca="false">15/$H$3</f>
-        <v>0.0367647058823529</v>
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
       </c>
       <c r="K23" s="15" t="n">
-        <v>0.482825664290343</v>
+        <v>0.391434449223864</v>
       </c>
       <c r="L23" s="16" t="n">
-        <f aca="false">3920/$K$3</f>
-        <v>0.717554457257917</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N23" s="15" t="s">
-        <v>54</v>
+        <f aca="false">116/$K$3</f>
+        <v>0.0212337543474282</v>
+      </c>
+      <c r="M23" s="15" t="n">
+        <v>0.691602220900258</v>
+      </c>
+      <c r="N23" s="15" t="n">
+        <v>0.36669042044182</v>
       </c>
       <c r="O23" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
-      </c>
-      <c r="P23" s="15" t="s">
-        <v>54</v>
+        <f aca="false">86/$M$3</f>
+        <v>0.00212713331684393</v>
+      </c>
+      <c r="P23" s="15" t="n">
+        <v>0.306859205776173</v>
       </c>
       <c r="Q23" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R23" s="15" t="s">
-        <v>54</v>
+      <c r="R23" s="15" t="n">
+        <v>0.855504587155963</v>
       </c>
       <c r="S23" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="U23" s="15" t="s">
-        <v>54</v>
+      <c r="T23" s="15" t="n">
+        <v>0.370306926073738</v>
+      </c>
+      <c r="U23" s="15" t="n">
+        <v>0.402389871619712</v>
       </c>
       <c r="V23" s="16" t="n">
         <f aca="false">0/$T$3</f>
         <v>0</v>
       </c>
-      <c r="W23" s="15" t="s">
-        <v>54</v>
+      <c r="W23" s="15" t="n">
+        <v>0.47887323943662</v>
       </c>
       <c r="X23" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -4085,82 +4123,82 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="C24" s="14" t="n">
         <f aca="false">AVERAGE(W24,T24:U24,R24,P24,N24,M24,K24,H24,I24,F24,D24)</f>
-        <v>0.338674923063942</v>
+        <v>0.457777805523234</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>0.241606739317903</v>
+        <v>0</v>
       </c>
       <c r="E24" s="16" t="n">
-        <f aca="false">7/$D$3</f>
-        <v>0.00671140939597315</v>
+        <f aca="false">12/$D$3</f>
+        <v>0.0115052732502397</v>
       </c>
       <c r="F24" s="15" t="n">
-        <v>0.285161027313494</v>
+        <v>0.31758314125782</v>
       </c>
       <c r="G24" s="16" t="n">
-        <f aca="false">3/$F$3</f>
-        <v>0.000305654610290372</v>
+        <f aca="false">3741/$F$3</f>
+        <v>0.381151299032094</v>
       </c>
       <c r="H24" s="15" t="n">
-        <v>0.333333333333333</v>
+        <v>0.679389312977099</v>
       </c>
       <c r="I24" s="15" t="n">
-        <v>0.0620689655172414</v>
+        <v>0.809090909090909</v>
       </c>
       <c r="J24" s="16" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
+        <f aca="false">15/$H$3</f>
+        <v>0.0367647058823529</v>
       </c>
       <c r="K24" s="15" t="n">
-        <v>0.32644239804548</v>
+        <v>0.482825664290343</v>
       </c>
       <c r="L24" s="16" t="n">
-        <f aca="false">142/$K$3</f>
-        <v>0.0259930441149552</v>
-      </c>
-      <c r="M24" s="15" t="n">
-        <v>0.459092373658512</v>
-      </c>
-      <c r="N24" s="15" t="n">
-        <v>0.524490151647202</v>
+        <f aca="false">3920/$K$3</f>
+        <v>0.717554457257917</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="O24" s="16" t="n">
-        <f aca="false">83/$M$3</f>
-        <v>0.00205293099183774</v>
-      </c>
-      <c r="P24" s="15" t="n">
-        <v>0.357400722021661</v>
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="Q24" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
-      <c r="R24" s="15" t="n">
-        <v>0.894374282433984</v>
+      <c r="R24" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="S24" s="16" t="n">
-        <f aca="false">1/$R$3</f>
-        <v>0.00114678899082569</v>
-      </c>
-      <c r="T24" s="15" t="n">
-        <v>0.0103797859681123</v>
-      </c>
-      <c r="U24" s="15" t="n">
-        <v>0.119045072158263</v>
+        <f aca="false">0/$R$3</f>
+        <v>0</v>
+      </c>
+      <c r="T24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="U24" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="V24" s="16" t="n">
-        <f aca="false">10/$T$3</f>
-        <v>0.00666666666666667</v>
-      </c>
-      <c r="W24" s="15" t="n">
-        <v>0.450704225352113</v>
+        <f aca="false">0/$T$3</f>
+        <v>0</v>
+      </c>
+      <c r="W24" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="X24" s="16" t="n">
         <f aca="false">0/$W$3</f>
@@ -4172,86 +4210,169 @@
         <v>57</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C25" s="14" t="n">
         <f aca="false">AVERAGE(W25,T25:U25,R25,P25,N25,M25,K25,H25,I25,F25,D25)</f>
-        <v>0.315867617188256</v>
+        <v>0.338674923063942</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>0.0292920614513275</v>
+        <v>0.241606739317903</v>
       </c>
       <c r="E25" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">7/$D$3</f>
+        <v>0.00671140939597315</v>
       </c>
       <c r="F25" s="15" t="n">
-        <v>0.35588385124809</v>
+        <v>0.285161027313494</v>
       </c>
       <c r="G25" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">3/$F$3</f>
+        <v>0.000305654610290372</v>
       </c>
       <c r="H25" s="15" t="n">
-        <v>0.321078431372549</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="I25" s="15" t="n">
-        <v>0.0142348754448399</v>
+        <v>0.0620689655172414</v>
       </c>
       <c r="J25" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="K25" s="15" t="n">
-        <v>0.494783086216365</v>
+        <v>0.32644239804548</v>
       </c>
       <c r="L25" s="16" t="n">
-        <f aca="false">0/$K$3</f>
-        <v>0</v>
+        <f aca="false">142/$K$3</f>
+        <v>0.0259930441149552</v>
       </c>
       <c r="M25" s="15" t="n">
-        <v>0.664506554538709</v>
+        <v>0.459092373658512</v>
       </c>
       <c r="N25" s="15" t="n">
-        <v>0.366819157875082</v>
+        <v>0.524490151647202</v>
       </c>
       <c r="O25" s="16" t="n">
-        <f aca="false">0/$M$3</f>
-        <v>0</v>
+        <f aca="false">83/$M$3</f>
+        <v>0.00205293099183774</v>
       </c>
       <c r="P25" s="15" t="n">
-        <v>0.509025270758123</v>
+        <v>0.357400722021661</v>
       </c>
       <c r="Q25" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
       <c r="R25" s="15" t="n">
+        <v>0.894374282433984</v>
+      </c>
+      <c r="S25" s="16" t="n">
+        <f aca="false">1/$R$3</f>
+        <v>0.00114678899082569</v>
+      </c>
+      <c r="T25" s="15" t="n">
+        <v>0.0103797859681123</v>
+      </c>
+      <c r="U25" s="15" t="n">
+        <v>0.119045072158263</v>
+      </c>
+      <c r="V25" s="16" t="n">
+        <f aca="false">10/$T$3</f>
+        <v>0.00666666666666667</v>
+      </c>
+      <c r="W25" s="15" t="n">
+        <v>0.450704225352113</v>
+      </c>
+      <c r="X25" s="16" t="n">
+        <f aca="false">0/$W$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="14" t="n">
+        <f aca="false">AVERAGE(W26,T26:U26,R26,P26,N26,M26,K26,H26,I26,F26,D26)</f>
+        <v>0.315867617188256</v>
+      </c>
+      <c r="D26" s="15" t="n">
+        <v>0.0292920614513275</v>
+      </c>
+      <c r="E26" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="15" t="n">
+        <v>0.35588385124809</v>
+      </c>
+      <c r="G26" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="15" t="n">
+        <v>0.321078431372549</v>
+      </c>
+      <c r="I26" s="15" t="n">
+        <v>0.0142348754448399</v>
+      </c>
+      <c r="J26" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="15" t="n">
+        <v>0.494783086216365</v>
+      </c>
+      <c r="L26" s="16" t="n">
+        <f aca="false">0/$K$3</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="15" t="n">
+        <v>0.664506554538709</v>
+      </c>
+      <c r="N26" s="15" t="n">
+        <v>0.366819157875082</v>
+      </c>
+      <c r="O26" s="16" t="n">
+        <f aca="false">0/$M$3</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="15" t="n">
+        <v>0.509025270758123</v>
+      </c>
+      <c r="Q26" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="15" t="n">
         <v>0.49197247706422</v>
       </c>
-      <c r="S25" s="16" t="n">
+      <c r="S26" s="16" t="n">
         <f aca="false">0/$R$3</f>
         <v>0</v>
       </c>
-      <c r="T25" s="15" t="n">
+      <c r="T26" s="15" t="n">
         <v>-0.0284464151760631</v>
       </c>
-      <c r="U25" s="15" t="n">
+      <c r="U26" s="15" t="n">
         <v>0.0219662808179385</v>
       </c>
-      <c r="V25" s="16" t="n">
+      <c r="V26" s="16" t="n">
         <f aca="false">2/$T$3</f>
         <v>0.00133333333333333</v>
       </c>
-      <c r="W25" s="15" t="n">
+      <c r="W26" s="15" t="n">
         <v>0.549295774647887</v>
       </c>
-      <c r="X25" s="16" t="n">
+      <c r="X26" s="16" t="n">
         <f aca="false">0/$W$3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4289,7 +4410,7 @@
     <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E48 G4:G48 J4:J48 L4:L48 O4:O48 Q4:Q48 S4:S48 X4:X48 V4:V48">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4417,25 +4538,26 @@
     <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
     <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
     <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Phi-3-medium-4k-instruct-GGUF"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/bartowski/OLMoE-1B-7B-0924-Instruct-GGUF"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/unsloth/Llama-3.3-70B-Instruct-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Phi-3-medium-4k-instruct-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://huggingface.co/bartowski/OLMoE-1B-7B-0924-Instruct-GGUF"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4444,8 +4566,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId24"/>
-  <legacyDrawing r:id="rId25"/>
+  <drawing r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -4457,7 +4579,7 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4491,7 +4613,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -4505,7 +4627,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
@@ -4518,31 +4640,31 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
@@ -4551,7 +4673,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="8"/>
       <c r="D3" s="9" t="n">
@@ -4594,10 +4716,10 @@
         <v>2000</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S3" s="10" t="s">
         <v>13</v>
@@ -4672,10 +4794,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="14" t="n">
         <f aca="false">AVERAGE(D5,F5,H5,J5,L5,N5)</f>
@@ -4739,10 +4861,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C6" s="14" t="n">
         <f aca="false">AVERAGE(D6,F6,H6,J6,L6,N6)</f>
@@ -4806,10 +4928,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="14" t="n">
         <f aca="false">AVERAGE(D7,F7,H7,J7,L7,N7)</f>
@@ -4873,10 +4995,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="14" t="n">
         <f aca="false">AVERAGE(D8,F8,H8,J8,L8,N8)</f>
@@ -4940,10 +5062,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">AVERAGE(D9,F9,H9,J9,L9,N9)</f>
@@ -5007,45 +5129,45 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">AVERAGE(D10,F10,H10,J10,L10,N10)</f>
-        <v>0.449693612435578</v>
+        <v>0.46200321745164</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.204119502057382</v>
+        <v>0.234498065398941</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I10" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J10" s="15" t="n">
-        <v>0.442148760330579</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K10" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L10" s="15" t="n">
-        <v>0.672961373390558</v>
+        <v>0.693562231759657</v>
       </c>
       <c r="M10" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -5059,17 +5181,17 @@
         <v>0</v>
       </c>
       <c r="P10" s="22" t="n">
-        <v>0.0946010077074703</v>
+        <v>0.0954311625486168</v>
       </c>
       <c r="Q10" s="15" t="n">
-        <v>0.950708101886604</v>
+        <v>1.07805990095118</v>
       </c>
       <c r="R10" s="23" t="n">
-        <v>0.036</v>
+        <v>0.093</v>
       </c>
       <c r="S10" s="16" t="n">
-        <f aca="false">506/$P$3</f>
-        <v>0.253</v>
+        <f aca="false">39/$P$3</f>
+        <v>0.0195</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5081,38 +5203,38 @@
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">AVERAGE(D11,F11,H11,J11,L11,N11)</f>
-        <v>0.446939595430147</v>
+        <v>0.449693612435578</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>0.214844642079834</v>
+        <v>0.204119502057382</v>
       </c>
       <c r="E11" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F11" s="15" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="G11" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H11" s="15" t="n">
-        <v>0.310679611650485</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I11" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J11" s="15" t="n">
-        <v>0.448559670781893</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K11" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L11" s="15" t="n">
-        <v>0.68755364806867</v>
+        <v>0.672961373390558</v>
       </c>
       <c r="M11" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -5126,64 +5248,64 @@
         <v>0</v>
       </c>
       <c r="P11" s="22" t="n">
-        <v>0.0869997613324107</v>
+        <v>0.0946010077074703</v>
       </c>
       <c r="Q11" s="15" t="n">
-        <v>1.1923877607133</v>
+        <v>0.950708101886604</v>
       </c>
       <c r="R11" s="23" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="S11" s="16" t="n">
-        <f aca="false">28/$P$3</f>
-        <v>0.014</v>
+        <f aca="false">506/$P$3</f>
+        <v>0.253</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">AVERAGE(D12,F12,H12,J12,L12,N12)</f>
-        <v>0.456362837616999</v>
+        <v>0.446939595430147</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>0.304699117807113</v>
+        <v>0.214844642079834</v>
       </c>
       <c r="E12" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F12" s="15" t="n">
-        <v>0.466666666666667</v>
+        <v>0.47</v>
       </c>
       <c r="G12" s="16" t="n">
-        <f aca="false">25/$F$3</f>
-        <v>0.25</v>
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
       </c>
       <c r="H12" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.310679611650485</v>
       </c>
       <c r="I12" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J12" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.448559670781893</v>
       </c>
       <c r="K12" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L12" s="15" t="n">
-        <v>0.622852233676976</v>
+        <v>0.68755364806867</v>
       </c>
       <c r="M12" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N12" s="15" t="n">
         <v>0.55</v>
@@ -5193,50 +5315,50 @@
         <v>0</v>
       </c>
       <c r="P12" s="22" t="n">
-        <v>0.0704660506880692</v>
+        <v>0.0869997613324107</v>
       </c>
       <c r="Q12" s="15" t="n">
-        <v>1.10242179616549</v>
+        <v>1.1923877607133</v>
       </c>
       <c r="R12" s="23" t="n">
-        <v>0.083</v>
+        <v>0.035</v>
       </c>
       <c r="S12" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">28/$P$3</f>
+        <v>0.014</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">AVERAGE(D13,F13,H13,J13,L13,N13)</f>
-        <v>0.478378567077423</v>
+        <v>0.456362837616999</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>0.267184035681135</v>
+        <v>0.304699117807113</v>
       </c>
       <c r="E13" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F13" s="15" t="n">
-        <v>0.653846153846154</v>
+        <v>0.466666666666667</v>
       </c>
       <c r="G13" s="16" t="n">
-        <f aca="false">74/$F$3</f>
-        <v>0.74</v>
+        <f aca="false">25/$F$3</f>
+        <v>0.25</v>
       </c>
       <c r="H13" s="15" t="n">
-        <v>0.343137254901961</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I13" s="16" t="n">
-        <f aca="false">1/$H$3</f>
-        <v>0.00970873786407767</v>
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
       </c>
       <c r="J13" s="15" t="n">
         <v>0.444444444444444</v>
@@ -5246,64 +5368,64 @@
         <v>0</v>
       </c>
       <c r="L13" s="15" t="n">
-        <v>0.628326180257511</v>
+        <v>0.622852233676976</v>
       </c>
       <c r="M13" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N13" s="15" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O13" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P13" s="22" t="n">
-        <v>0.0672850889690679</v>
+        <v>0.0704660506880692</v>
       </c>
       <c r="Q13" s="15" t="n">
-        <v>1.14115440228223</v>
+        <v>1.10242179616549</v>
       </c>
       <c r="R13" s="23" t="n">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="S13" s="16" t="n">
-        <f aca="false">21/$P$3</f>
-        <v>0.0105</v>
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">AVERAGE(D14,F14,H14,J14,L14,N14)</f>
-        <v>0.416323225087402</v>
+        <v>0.478378567077423</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>0.00078604321068414</v>
+        <v>0.267184035681135</v>
       </c>
       <c r="E14" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F14" s="15" t="n">
-        <v>0.49</v>
+        <v>0.653846153846154</v>
       </c>
       <c r="G14" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
+        <f aca="false">74/$F$3</f>
+        <v>0.74</v>
       </c>
       <c r="H14" s="15" t="n">
-        <v>0.368932038834951</v>
+        <v>0.343137254901961</v>
       </c>
       <c r="I14" s="16" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
+        <f aca="false">1/$H$3</f>
+        <v>0.00970873786407767</v>
       </c>
       <c r="J14" s="15" t="n">
         <v>0.444444444444444</v>
@@ -5313,74 +5435,74 @@
         <v>0</v>
       </c>
       <c r="L14" s="15" t="n">
-        <v>0.643776824034335</v>
+        <v>0.628326180257511</v>
       </c>
       <c r="M14" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N14" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O14" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P14" s="22" t="n">
-        <v>0.0672142694158681</v>
+        <v>0.0672850889690679</v>
       </c>
       <c r="Q14" s="15" t="n">
-        <v>1.08084074373484</v>
+        <v>1.14115440228223</v>
       </c>
       <c r="R14" s="23" t="n">
-        <v>0.068</v>
+        <v>0.08</v>
       </c>
       <c r="S14" s="16" t="n">
-        <f aca="false">1817/$P$3</f>
-        <v>0.9085</v>
+        <f aca="false">21/$P$3</f>
+        <v>0.0105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">AVERAGE(D15,F15,H15,J15,L15,N15)</f>
-        <v>0.436042704459863</v>
+        <v>0.416323225087402</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>0.0518271447518188</v>
+        <v>0.00078604321068414</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F15" s="15" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="G15" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H15" s="15" t="n">
-        <v>0.398058252427184</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I15" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J15" s="15" t="n">
-        <v>0.448559670781893</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K15" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L15" s="15" t="n">
-        <v>0.667811158798283</v>
+        <v>0.643776824034335</v>
       </c>
       <c r="M15" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -5394,60 +5516,60 @@
         <v>0</v>
       </c>
       <c r="P15" s="22" t="n">
-        <v>0.0666584744053729</v>
+        <v>0.0672142694158681</v>
       </c>
       <c r="Q15" s="15" t="n">
-        <v>1.05036977813312</v>
+        <v>1.08084074373484</v>
       </c>
       <c r="R15" s="23" t="n">
-        <v>0.061</v>
+        <v>0.068</v>
       </c>
       <c r="S15" s="16" t="n">
-        <f aca="false">1206/$P$3</f>
-        <v>0.603</v>
+        <f aca="false">1817/$P$3</f>
+        <v>0.9085</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">AVERAGE(D16,F16,H16,J16,L16,N16)</f>
-        <v>0.425537790635605</v>
+        <v>0.436042704459863</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>0.128651460584234</v>
+        <v>0.0518271447518188</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F16" s="15" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="15" t="n">
-        <v>0.320388349514563</v>
+        <v>0.398058252427184</v>
       </c>
       <c r="I16" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J16" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.448559670781893</v>
       </c>
       <c r="K16" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L16" s="15" t="n">
-        <v>0.619742489270386</v>
+        <v>0.667811158798283</v>
       </c>
       <c r="M16" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -5461,265 +5583,265 @@
         <v>0</v>
       </c>
       <c r="P16" s="22" t="n">
+        <v>0.0666584744053729</v>
+      </c>
+      <c r="Q16" s="15" t="n">
+        <v>1.05036977813312</v>
+      </c>
+      <c r="R16" s="23" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="S16" s="16" t="n">
+        <f aca="false">1206/$P$3</f>
+        <v>0.603</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="14" t="n">
+        <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
+        <v>0.425537790635605</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.128651460584234</v>
+      </c>
+      <c r="E17" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="15" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="G17" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="15" t="n">
+        <v>0.320388349514563</v>
+      </c>
+      <c r="I17" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="15" t="n">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K17" s="16" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="15" t="n">
+        <v>0.619742489270386</v>
+      </c>
+      <c r="M17" s="16" t="n">
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="15" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O17" s="16" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="22" t="n">
         <v>0.0618591437609282</v>
       </c>
-      <c r="Q16" s="15" t="n">
+      <c r="Q17" s="15" t="n">
         <v>1.07679555721331</v>
       </c>
-      <c r="R16" s="23" t="n">
+      <c r="R17" s="23" t="n">
         <v>0.045</v>
       </c>
-      <c r="S16" s="16" t="n">
+      <c r="S17" s="16" t="n">
         <f aca="false">175/$P$3</f>
         <v>0.0875</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="14" t="n">
-        <f aca="false">AVERAGE(D17,F17,H17,J17,L17,N17)</f>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="14" t="n">
+        <f aca="false">AVERAGE(D18,F18,H18,J18,L18,N18)</f>
         <v>0.424592652235</v>
       </c>
-      <c r="D17" s="15" t="n">
+      <c r="D18" s="15" t="n">
         <v>-0.0425570189562919</v>
       </c>
-      <c r="E17" s="16" t="n">
+      <c r="E18" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
-      <c r="F17" s="15" t="n">
+      <c r="F18" s="15" t="n">
         <v>0.49</v>
       </c>
-      <c r="G17" s="16" t="n">
+      <c r="G18" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
-      <c r="H17" s="15" t="n">
+      <c r="H18" s="15" t="n">
         <v>0.42156862745098</v>
       </c>
-      <c r="I17" s="16" t="n">
+      <c r="I18" s="16" t="n">
         <f aca="false">1/$H$3</f>
         <v>0.00970873786407767</v>
       </c>
-      <c r="J17" s="15" t="n">
+      <c r="J18" s="15" t="n">
         <v>0.473251028806584</v>
       </c>
-      <c r="K17" s="16" t="n">
+      <c r="K18" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
-      <c r="L17" s="15" t="n">
+      <c r="L18" s="15" t="n">
         <v>0.63862660944206</v>
       </c>
-      <c r="M17" s="16" t="n">
+      <c r="M18" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
-      <c r="N17" s="15" t="n">
+      <c r="N18" s="15" t="n">
         <v>0.566666666666667</v>
       </c>
-      <c r="O17" s="16" t="n">
+      <c r="O18" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
-      <c r="P17" s="22" t="n">
+      <c r="P18" s="22" t="n">
         <v>0.0599833472677267</v>
       </c>
-      <c r="Q17" s="15" t="n">
+      <c r="Q18" s="15" t="n">
         <v>1.22623545413329</v>
       </c>
-      <c r="R17" s="23" t="n">
+      <c r="R18" s="23" t="n">
         <v>0.086</v>
       </c>
-      <c r="S17" s="16" t="n">
+      <c r="S18" s="16" t="n">
         <f aca="false">611/$P$3</f>
         <v>0.3055</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="14" t="n">
-        <f aca="false">AVERAGE(D18,F18,H18,J18,L18,N18)</f>
-        <v>0.419278530088385</v>
-      </c>
-      <c r="D18" s="15" t="n">
-        <v>-0.0155335936055105</v>
-      </c>
-      <c r="E18" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="15" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="G18" s="16" t="n">
-        <f aca="false">0/$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="n">
-        <v>0.368932038834951</v>
-      </c>
-      <c r="I18" s="16" t="n">
-        <f aca="false">0/$H$3</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="15" t="n">
-        <v>0.489711934156379</v>
-      </c>
-      <c r="K18" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="15" t="n">
-        <v>0.659227467811159</v>
-      </c>
-      <c r="M18" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="15" t="n">
-        <v>0.533333333333333</v>
-      </c>
-      <c r="O18" s="16" t="n">
-        <f aca="false">0/$N$3</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="22" t="n">
-        <v>0.0534217525346316</v>
-      </c>
-      <c r="Q18" s="15" t="n">
-        <v>1.26345272449499</v>
-      </c>
-      <c r="R18" s="23" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="S18" s="16" t="n">
-        <f aca="false">213/$P$3</f>
-        <v>0.1065</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">AVERAGE(D19,F19,H19,J19,L19,N19)</f>
-        <v>0.432443158810545</v>
+        <v>0.419278530088385</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>0.0718486458091463</v>
+        <v>-0.0155335936055105</v>
       </c>
       <c r="E19" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F19" s="15" t="n">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G19" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H19" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.368932038834951</v>
       </c>
       <c r="I19" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>0.444444444444444</v>
+        <v>0.489711934156379</v>
       </c>
       <c r="K19" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L19" s="15" t="n">
-        <v>0.629725085910653</v>
+        <v>0.659227467811159</v>
       </c>
       <c r="M19" s="16" t="n">
         <f aca="false">0/$L$3</f>
         <v>0</v>
       </c>
       <c r="N19" s="15" t="n">
-        <v>0.55</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O19" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P19" s="22" t="n">
-        <v>0.0497002425066837</v>
+        <v>0.0534217525346316</v>
       </c>
       <c r="Q19" s="15" t="n">
-        <v>1.29332825735224</v>
+        <v>1.26345272449499</v>
       </c>
       <c r="R19" s="23" t="n">
-        <v>0.079</v>
+        <v>0.041</v>
       </c>
       <c r="S19" s="16" t="n">
-        <f aca="false">1339/$P$3</f>
-        <v>0.6695</v>
+        <f aca="false">213/$P$3</f>
+        <v>0.1065</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">AVERAGE(D20,F20,H20,J20,L20,N20)</f>
-        <v>0.439307324929851</v>
+        <v>0.432443158810545</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>0.127338801833183</v>
+        <v>0.0718486458091463</v>
       </c>
       <c r="E20" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F20" s="15" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G20" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H20" s="15" t="n">
-        <v>0.388349514563107</v>
+        <v>0.378640776699029</v>
       </c>
       <c r="I20" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J20" s="15" t="n">
-        <v>0.442148760330579</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="K20" s="16" t="n">
-        <f aca="false">1/$J$3</f>
-        <v>0.00411522633744856</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L20" s="15" t="n">
-        <v>0.628006872852234</v>
+        <v>0.629725085910653</v>
       </c>
       <c r="M20" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N20" s="15" t="n">
         <v>0.55</v>
@@ -5729,32 +5851,32 @@
         <v>0</v>
       </c>
       <c r="P20" s="22" t="n">
-        <v>0.0462020736542011</v>
+        <v>0.0497002425066837</v>
       </c>
       <c r="Q20" s="15" t="n">
-        <v>1.07801109103371</v>
+        <v>1.29332825735224</v>
       </c>
       <c r="R20" s="23" t="n">
-        <v>0.123</v>
+        <v>0.079</v>
       </c>
       <c r="S20" s="16" t="n">
-        <f aca="false">776/$P$3</f>
-        <v>0.388</v>
+        <f aca="false">1339/$P$3</f>
+        <v>0.6695</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">AVERAGE(D21,F21,H21,J21,L21,N21)</f>
-        <v>0.411633605752468</v>
+        <v>0.439307324929851</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>0.0289209788221949</v>
+        <v>0.127338801833183</v>
       </c>
       <c r="E21" s="16" t="n">
         <f aca="false">0/$D$3</f>
@@ -5768,25 +5890,25 @@
         <v>0</v>
       </c>
       <c r="H21" s="15" t="n">
-        <v>0.281553398058252</v>
+        <v>0.388349514563107</v>
       </c>
       <c r="I21" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J21" s="15" t="n">
-        <v>0.452674897119342</v>
+        <v>0.442148760330579</v>
       </c>
       <c r="K21" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">1/$J$3</f>
+        <v>0.00411522633744856</v>
       </c>
       <c r="L21" s="15" t="n">
-        <v>0.656652360515021</v>
+        <v>0.628006872852234</v>
       </c>
       <c r="M21" s="16" t="n">
-        <f aca="false">0/$L$3</f>
-        <v>0</v>
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
       </c>
       <c r="N21" s="15" t="n">
         <v>0.55</v>
@@ -5796,46 +5918,46 @@
         <v>0</v>
       </c>
       <c r="P21" s="22" t="n">
-        <v>0.0450466025027233</v>
+        <v>0.0462020736542011</v>
       </c>
       <c r="Q21" s="15" t="n">
-        <v>1.17910447761194</v>
+        <v>1.07801109103371</v>
       </c>
       <c r="R21" s="23" t="n">
-        <v>0.135</v>
+        <v>0.123</v>
       </c>
       <c r="S21" s="16" t="n">
-        <f aca="false">1829/$P$3</f>
-        <v>0.9145</v>
+        <f aca="false">776/$P$3</f>
+        <v>0.388</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C22" s="14" t="n">
         <f aca="false">AVERAGE(D22,F22,H22,J22,L22,N22)</f>
-        <v>0.41273629360193</v>
+        <v>0.411633605752468</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>0.0238941207945824</v>
+        <v>0.0289209788221949</v>
       </c>
       <c r="E22" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F22" s="15" t="n">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="G22" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H22" s="15" t="n">
-        <v>0.339805825242718</v>
+        <v>0.281553398058252</v>
       </c>
       <c r="I22" s="16" t="n">
         <f aca="false">0/$H$3</f>
@@ -5849,7 +5971,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="15" t="n">
-        <v>0.630042918454936</v>
+        <v>0.656652360515021</v>
       </c>
       <c r="M22" s="16" t="n">
         <f aca="false">0/$L$3</f>
@@ -5863,64 +5985,64 @@
         <v>0</v>
       </c>
       <c r="P22" s="22" t="n">
-        <v>0.0372835531044292</v>
+        <v>0.0450466025027233</v>
       </c>
       <c r="Q22" s="15" t="n">
-        <v>1.20252219690422</v>
+        <v>1.17910447761194</v>
       </c>
       <c r="R22" s="23" t="n">
-        <v>0.084</v>
+        <v>0.135</v>
       </c>
       <c r="S22" s="16" t="n">
-        <f aca="false">31/$P$3</f>
-        <v>0.0155</v>
+        <f aca="false">1829/$P$3</f>
+        <v>0.9145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>71</v>
+        <v>32</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C23" s="14" t="n">
         <f aca="false">AVERAGE(D23,F23,H23,J23,L23,N23)</f>
-        <v>0.479783624027799</v>
+        <v>0.41273629360193</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>0.369274416448439</v>
+        <v>0.0238941207945824</v>
       </c>
       <c r="E23" s="16" t="n">
-        <f aca="false">4/$D$3</f>
-        <v>0.0043956043956044</v>
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
       </c>
       <c r="F23" s="15" t="n">
-        <v>0.52</v>
+        <v>0.48</v>
       </c>
       <c r="G23" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H23" s="15" t="n">
-        <v>0.349514563106796</v>
+        <v>0.339805825242718</v>
       </c>
       <c r="I23" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J23" s="15" t="n">
-        <v>0.44017094017094</v>
+        <v>0.452674897119342</v>
       </c>
       <c r="K23" s="16" t="n">
-        <f aca="false">9/$J$3</f>
-        <v>0.037037037037037</v>
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
       </c>
       <c r="L23" s="15" t="n">
-        <v>0.649741824440619</v>
+        <v>0.630042918454936</v>
       </c>
       <c r="M23" s="16" t="n">
-        <f aca="false">3/$L$3</f>
-        <v>0.00257510729613734</v>
+        <f aca="false">0/$L$3</f>
+        <v>0</v>
       </c>
       <c r="N23" s="15" t="n">
         <v>0.55</v>
@@ -5930,147 +6052,147 @@
         <v>0</v>
       </c>
       <c r="P23" s="22" t="n">
-        <v>0.0263546139456426</v>
+        <v>0.0372835531044292</v>
       </c>
       <c r="Q23" s="15" t="n">
-        <v>0.384891506009518</v>
+        <v>1.20252219690422</v>
       </c>
       <c r="R23" s="23" t="n">
-        <v>0.08</v>
+        <v>0.084</v>
       </c>
       <c r="S23" s="16" t="n">
-        <f aca="false">80/$P$3</f>
-        <v>0.04</v>
+        <f aca="false">31/$P$3</f>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>49</v>
+        <v>72</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="C24" s="14" t="n">
         <f aca="false">AVERAGE(D24,F24,H24,J24,L24,N24)</f>
-        <v>0.373693198829491</v>
+        <v>0.479783624027799</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>-0.0220534635916509</v>
+        <v>0.369274416448439</v>
       </c>
       <c r="E24" s="16" t="n">
-        <f aca="false">0/$D$3</f>
-        <v>0</v>
+        <f aca="false">4/$D$3</f>
+        <v>0.0043956043956044</v>
       </c>
       <c r="F24" s="15" t="n">
-        <v>0.47</v>
+        <v>0.52</v>
       </c>
       <c r="G24" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H24" s="15" t="n">
-        <v>0.398058252427184</v>
+        <v>0.349514563106796</v>
       </c>
       <c r="I24" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J24" s="15" t="n">
-        <v>0.452674897119342</v>
+        <v>0.44017094017094</v>
       </c>
       <c r="K24" s="16" t="n">
-        <f aca="false">0/$J$3</f>
-        <v>0</v>
+        <f aca="false">9/$J$3</f>
+        <v>0.037037037037037</v>
       </c>
       <c r="L24" s="15" t="n">
-        <v>0.410146173688736</v>
+        <v>0.649741824440619</v>
       </c>
       <c r="M24" s="16" t="n">
-        <f aca="false">2/$L$3</f>
-        <v>0.00171673819742489</v>
+        <f aca="false">3/$L$3</f>
+        <v>0.00257510729613734</v>
       </c>
       <c r="N24" s="15" t="n">
-        <v>0.533333333333333</v>
+        <v>0.55</v>
       </c>
       <c r="O24" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P24" s="22" t="n">
-        <v>0.0200592465655649</v>
+        <v>0.0263546139456426</v>
       </c>
       <c r="Q24" s="15" t="n">
-        <v>1.33598540712567</v>
+        <v>0.384891506009518</v>
       </c>
       <c r="R24" s="23" t="n">
-        <v>0.106</v>
+        <v>0.08</v>
       </c>
       <c r="S24" s="16" t="n">
-        <f aca="false">0/$P$3</f>
-        <v>0</v>
+        <f aca="false">80/$P$3</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C25" s="14" t="n">
         <f aca="false">AVERAGE(D25,F25,H25,J25,L25,N25)</f>
-        <v>0.405257833604129</v>
+        <v>0.373693198829491</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>-0.0714529452409867</v>
+        <v>-0.0220534635916509</v>
       </c>
       <c r="E25" s="16" t="n">
         <f aca="false">0/$D$3</f>
         <v>0</v>
       </c>
       <c r="F25" s="15" t="n">
-        <v>0.52</v>
+        <v>0.47</v>
       </c>
       <c r="G25" s="16" t="n">
         <f aca="false">0/$F$3</f>
         <v>0</v>
       </c>
       <c r="H25" s="15" t="n">
-        <v>0.378640776699029</v>
+        <v>0.398058252427184</v>
       </c>
       <c r="I25" s="16" t="n">
         <f aca="false">0/$H$3</f>
         <v>0</v>
       </c>
       <c r="J25" s="15" t="n">
-        <v>0.469135802469136</v>
+        <v>0.452674897119342</v>
       </c>
       <c r="K25" s="16" t="n">
         <f aca="false">0/$J$3</f>
         <v>0</v>
       </c>
       <c r="L25" s="15" t="n">
-        <v>0.618556701030928</v>
+        <v>0.410146173688736</v>
       </c>
       <c r="M25" s="16" t="n">
-        <f aca="false">1/$L$3</f>
-        <v>0.000858369098712446</v>
+        <f aca="false">2/$L$3</f>
+        <v>0.00171673819742489</v>
       </c>
       <c r="N25" s="15" t="n">
-        <v>0.516666666666667</v>
+        <v>0.533333333333333</v>
       </c>
       <c r="O25" s="16" t="n">
         <f aca="false">0/$N$3</f>
         <v>0</v>
       </c>
       <c r="P25" s="22" t="n">
-        <v>0.018613476307488</v>
+        <v>0.0200592465655649</v>
       </c>
       <c r="Q25" s="15" t="n">
-        <v>1.12997748971513</v>
+        <v>1.33598540712567</v>
       </c>
       <c r="R25" s="23" t="n">
-        <v>0.116</v>
+        <v>0.106</v>
       </c>
       <c r="S25" s="16" t="n">
         <f aca="false">0/$P$3</f>
@@ -6079,72 +6201,138 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C26" s="14" t="n">
         <f aca="false">AVERAGE(D26,F26,H26,J26,L26,N26)</f>
+        <v>0.405257833604129</v>
+      </c>
+      <c r="D26" s="15" t="n">
+        <v>-0.0714529452409867</v>
+      </c>
+      <c r="E26" s="16" t="n">
+        <f aca="false">0/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G26" s="16" t="n">
+        <f aca="false">0/$F$3</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="15" t="n">
+        <v>0.378640776699029</v>
+      </c>
+      <c r="I26" s="16" t="n">
+        <f aca="false">0/$H$3</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="15" t="n">
+        <v>0.469135802469136</v>
+      </c>
+      <c r="K26" s="16" t="n">
+        <f aca="false">0/$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="15" t="n">
+        <v>0.618556701030928</v>
+      </c>
+      <c r="M26" s="16" t="n">
+        <f aca="false">1/$L$3</f>
+        <v>0.000858369098712446</v>
+      </c>
+      <c r="N26" s="15" t="n">
+        <v>0.516666666666667</v>
+      </c>
+      <c r="O26" s="16" t="n">
+        <f aca="false">0/$N$3</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="22" t="n">
+        <v>0.018613476307488</v>
+      </c>
+      <c r="Q26" s="15" t="n">
+        <v>1.12997748971513</v>
+      </c>
+      <c r="R26" s="23" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="S26" s="16" t="n">
+        <f aca="false">0/$P$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="14" t="n">
+        <f aca="false">AVERAGE(D27,F27,H27,J27,L27,N27)</f>
         <v>0.364587789621774</v>
       </c>
-      <c r="D26" s="15" t="n">
+      <c r="D27" s="15" t="n">
         <v>0.0266825503923221</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E27" s="16" t="n">
         <f aca="false">187/$D$3</f>
         <v>0.205494505494505</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F27" s="15" t="n">
         <v>0.461538461538462</v>
       </c>
-      <c r="G26" s="16" t="n">
+      <c r="G27" s="16" t="n">
         <f aca="false">9/$F$3</f>
         <v>0.09</v>
       </c>
-      <c r="H26" s="15" t="n">
+      <c r="H27" s="15" t="n">
         <v>0.237113402061856</v>
       </c>
-      <c r="I26" s="16" t="n">
+      <c r="I27" s="16" t="n">
         <f aca="false">6/$H$3</f>
         <v>0.058252427184466</v>
       </c>
-      <c r="J26" s="15" t="n">
+      <c r="J27" s="15" t="n">
         <v>0.558823529411765</v>
       </c>
-      <c r="K26" s="16" t="n">
+      <c r="K27" s="16" t="n">
         <f aca="false">39/$J$3</f>
         <v>0.160493827160494</v>
       </c>
-      <c r="L26" s="15" t="n">
+      <c r="L27" s="15" t="n">
         <v>0.403368794326241</v>
       </c>
-      <c r="M26" s="16" t="n">
+      <c r="M27" s="16" t="n">
         <f aca="false">37/$L$3</f>
         <v>0.0317596566523605</v>
       </c>
-      <c r="N26" s="15" t="n">
+      <c r="N27" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="O26" s="16" t="n">
+      <c r="O27" s="16" t="n">
         <f aca="false">2/$N$3</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="P26" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="15" t="n">
+      <c r="P27" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="15" t="n">
         <v>1.02530466506249</v>
       </c>
-      <c r="R26" s="23" t="n">
+      <c r="R27" s="23" t="n">
         <v>0.544</v>
       </c>
-      <c r="S26" s="16" t="n">
+      <c r="S27" s="16" t="n">
         <f aca="false">0/$P$3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6178,8 +6366,8 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:S2"/>
   </mergeCells>
-  <conditionalFormatting sqref="S4:S26 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+  <conditionalFormatting sqref="S4:S27 E4:E28 G4:G28 I4:I28 K4:K28 M4:M28 O4:O28">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6243,7 +6431,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P26">
+  <conditionalFormatting sqref="P4:P27">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6270,22 +6458,23 @@
     <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
     <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
     <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/robbiemu/salamandra-2b-instruct"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://huggingface.co/bartowski/Phi-3-medium-4k-instruct-GGUF"/>
-    <hyperlink ref="B24" r:id="rId21" display="https://huggingface.co/bartowski/OLMoE-1B-7B-0924-Instruct-GGUF"/>
-    <hyperlink ref="B25" r:id="rId22" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
-    <hyperlink ref="B26" r:id="rId23" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/unsloth/Llama-3.3-70B-Instruct-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://huggingface.co/bartowski/Meta-Llama-3.1-8B-Instruct-GGUF"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://huggingface.co/bartowski/Qwen2.5-32B-Instruct-GGUF"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://huggingface.co/TheBloke/SOLAR-10.7B-Instruct-v1.0-GGUF"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://huggingface.co/bartowski/Ministral-8B-Instruct-2410-GGUF"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://huggingface.co/mradermacher/c4ai-command-r-v01-i1-GGUF"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://huggingface.co/bartowski/gemma-2-2b-it-GGUF"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://huggingface.co/robbiemu/salamandra-2b-instruct"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://huggingface.co/bartowski/Llama-3.2-3B-Instruct-GGUF"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://huggingface.co/bartowski/Mistral-NeMo-Minitron-8B-Instruct-GGUF"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://huggingface.co/bartowski/Yi-1.5-34B-Chat-GGUF"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://huggingface.co/TheBloke/Llama-2-7B-32K-Instruct-GGUF"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://huggingface.co/bartowski/Phi-3-medium-4k-instruct-GGUF"/>
+    <hyperlink ref="B25" r:id="rId22" display="https://huggingface.co/bartowski/OLMoE-1B-7B-0924-Instruct-GGUF"/>
+    <hyperlink ref="B26" r:id="rId23" display="https://huggingface.co/microsoft/Phi-3-mini-4k-instruct-gguf"/>
+    <hyperlink ref="B27" r:id="rId24" display="https://huggingface.co/mradermacher/falcon-mamba-7b-instruct-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6294,8 +6483,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId24"/>
-  <legacyDrawing r:id="rId25"/>
+  <drawing r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -6304,10 +6493,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6323,7 +6512,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -6333,7 +6522,7 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -6342,17 +6531,17 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="n">
         <f aca="false" t="array" ref="A3:A3">SUM(IF(A4:A50&lt;&gt;"",1,0))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="n">
         <v>88</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -6360,10 +6549,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="22" t="n">
         <v>0.468944019791467</v>
@@ -6404,17 +6593,17 @@
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="22" t="n">
-        <v>0.420595627761371</v>
+        <v>0.451205869803034</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>1</v>
+        <v>1.02059659090909</v>
       </c>
       <c r="E6" s="23" t="n">
-        <v>0.227</v>
+        <v>0.237</v>
       </c>
       <c r="F6" s="16" t="n">
         <f aca="false">0/$C$3</f>
@@ -6423,100 +6612,121 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C7" s="22" t="n">
-        <v>0.407822035664075</v>
+        <v>0.420595627761371</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>1.01204819277108</v>
+        <v>1</v>
       </c>
       <c r="E7" s="23" t="n">
-        <v>0.192</v>
+        <v>0.227</v>
       </c>
       <c r="F7" s="16" t="n">
-        <f aca="false">5/$C$3</f>
-        <v>0.0568181818181818</v>
+        <f aca="false">0/$C$3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C8" s="22" t="n">
-        <v>0.326448804334111</v>
+        <v>0.407822035664075</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>1.01491477272727</v>
+        <v>1.01204819277108</v>
       </c>
       <c r="E8" s="23" t="n">
-        <v>0.158</v>
+        <v>0.192</v>
       </c>
       <c r="F8" s="16" t="n">
-        <f aca="false">0/$C$3</f>
-        <v>0</v>
+        <f aca="false">5/$C$3</f>
+        <v>0.0568181818181818</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C9" s="22" t="n">
-        <v>0.151003586436886</v>
+        <v>0.326448804334111</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>1.84195402298851</v>
+        <v>1.01491477272727</v>
       </c>
       <c r="E9" s="23" t="n">
-        <v>0.166</v>
+        <v>0.158</v>
       </c>
       <c r="F9" s="16" t="n">
-        <f aca="false">1/$C$3</f>
-        <v>0.0113636363636364</v>
+        <f aca="false">0/$C$3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C10" s="22" t="n">
+        <v>0.151003586436886</v>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>1.84195402298851</v>
+      </c>
+      <c r="E10" s="23" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="F10" s="16" t="n">
+        <f aca="false">1/$C$3</f>
+        <v>0.0113636363636364</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="22" t="n">
         <v>0.12890377983389</v>
       </c>
-      <c r="D10" s="15" t="n">
+      <c r="D11" s="15" t="n">
         <v>2.10511363636364</v>
       </c>
-      <c r="E10" s="23" t="n">
+      <c r="E11" s="23" t="n">
         <v>0.103</v>
       </c>
-      <c r="F10" s="16" t="n">
+      <c r="F11" s="16" t="n">
         <f aca="false">66/$C$3</f>
         <v>0.75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F10"/>
+  <autoFilter ref="A3:F11"/>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F4:F10">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+  <conditionalFormatting sqref="F4:F11">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C10">
+  <conditionalFormatting sqref="C4:C11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6526,7 +6736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E10">
+  <conditionalFormatting sqref="E4:E11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6539,11 +6749,12 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId2" display="https://huggingface.co/bartowski/Meta-Llama-3.1-70B-Instruct-GGUF"/>
     <hyperlink ref="B5" r:id="rId3" display="https://huggingface.co/bartowski/gemma-2-27b-it-GGUF"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://huggingface.co/unsloth/Llama-3.3-70B-Instruct-GGUF"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://huggingface.co/bartowski/gemma-2-9b-it-GGUF"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://huggingface.co/RichardErkhov/BSC-LT_-_salamandra-7b-instruct-gguf"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://huggingface.co/ariel-ml/SambaLingo-Hungarian-Chat-GGUF"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://huggingface.co/fragata/PULI-LlumiX-32K-Instruct-Q4_K_M-GGUF"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://huggingface.co/TheBloke/Mixtral-8x7B-Instruct-v0.1-GGUF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -6552,7 +6763,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <drawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>